<commit_message>
:adhesive_bandage: CORRIGINDO ARQUIVO CORROMPIDO
Arquivo havia se corrompido (ModeloCarteirinha) então estou upando uma cópia utlizável do arquivo novamente
</commit_message>
<xml_diff>
--- a/ModeloCarteirinha.xlsx
+++ b/ModeloCarteirinha.xlsx
@@ -213,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -234,24 +234,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2448,21 +2449,21 @@
   <dimension ref="A5:O284"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="5.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="3" style="2" customWidth="1"/>
     <col min="9" max="9" width="10.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" customWidth="1"/>
     <col min="13" max="13" width="12.42578125" style="2" customWidth="1"/>
     <col min="14" max="14" width="8" style="2" customWidth="1"/>
@@ -2472,98 +2473,98 @@
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="25"/>
-      <c r="C6" s="21" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="22"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="22"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="19"/>
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="18"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="22"/>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
-      <c r="C8" s="23" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="22"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="18"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="22"/>
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="26"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
       <c r="I9" s="7"/>
       <c r="J9" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="18"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="22"/>
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-      <c r="C10" s="16" t="s">
+      <c r="B10" s="27"/>
+      <c r="C10" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="18"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="22"/>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2605,12 +2606,14 @@
       <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="C14" s="16"/>
       <c r="D14"/>
       <c r="F14" s="3"/>
       <c r="G14" s="8"/>
       <c r="I14" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="J14" s="16"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="3"/>
@@ -2629,18 +2632,18 @@
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
       <c r="F16" s="4"/>
       <c r="G16" s="8"/>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
       <c r="L16" s="2"/>
       <c r="M16" s="4"/>
       <c r="N16" s="8"/>
@@ -2677,59 +2680,59 @@
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="22"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="19"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="21" t="s">
+      <c r="J20" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="22"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="19"/>
       <c r="O20" s="2"/>
     </row>
     <row r="21" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="22"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="23" t="s">
+      <c r="J21" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="18"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="22"/>
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="22"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="23" t="s">
+      <c r="J22" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="18"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="22"/>
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
@@ -2737,37 +2740,37 @@
       <c r="C23" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="22"/>
       <c r="I23" s="7"/>
       <c r="J23" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="18"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="22"/>
       <c r="O23" s="2"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="18"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="22"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="16" t="s">
+      <c r="J24" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="18"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="22"/>
       <c r="O24" s="2"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -2837,18 +2840,18 @@
       <c r="O29" s="2"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
       <c r="F30" s="4"/>
       <c r="G30" s="8"/>
-      <c r="I30" s="19" t="s">
+      <c r="I30" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
       <c r="L30" s="2"/>
       <c r="M30" s="4"/>
       <c r="N30" s="8"/>
@@ -2884,103 +2887,103 @@
       <c r="O33" s="2"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="25"/>
-      <c r="C34" s="21" t="s">
+      <c r="B34" s="26"/>
+      <c r="C34" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="22"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="19"/>
       <c r="H34" s="14"/>
       <c r="I34" s="6"/>
-      <c r="J34" s="21" t="s">
+      <c r="J34" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="22"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="19"/>
       <c r="O34" s="2"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="26"/>
-      <c r="C35" s="23" t="s">
+      <c r="B35" s="27"/>
+      <c r="C35" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="22"/>
       <c r="H35" s="14"/>
       <c r="I35" s="7"/>
-      <c r="J35" s="23" t="s">
+      <c r="J35" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="18"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="22"/>
       <c r="O35" s="2"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="26"/>
-      <c r="C36" s="23" t="s">
+      <c r="B36" s="27"/>
+      <c r="C36" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="18"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="22"/>
       <c r="H36" s="14"/>
       <c r="I36" s="7"/>
-      <c r="J36" s="23" t="s">
+      <c r="J36" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="18"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="22"/>
       <c r="O36" s="2"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="26"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="18"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="22"/>
       <c r="H37" s="14"/>
       <c r="I37" s="7"/>
       <c r="J37" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="18"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="22"/>
       <c r="O37" s="2"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="26"/>
-      <c r="C38" s="16" t="s">
+      <c r="B38" s="27"/>
+      <c r="C38" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="18"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="22"/>
       <c r="H38" s="14"/>
       <c r="I38" s="7"/>
-      <c r="J38" s="16" t="s">
+      <c r="J38" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
-      <c r="M38" s="17"/>
-      <c r="N38" s="18"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="22"/>
       <c r="O38" s="2"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
@@ -3080,20 +3083,20 @@
       <c r="O43" s="2"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
       <c r="E44" s="14"/>
       <c r="F44" s="4"/>
       <c r="G44" s="15"/>
       <c r="H44" s="14"/>
-      <c r="I44" s="19" t="s">
+      <c r="I44" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
       <c r="L44" s="14"/>
       <c r="M44" s="4"/>
       <c r="N44" s="15"/>
@@ -3149,62 +3152,62 @@
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
-      <c r="C48" s="21" t="s">
+      <c r="C48" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="22"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="19"/>
       <c r="H48" s="14"/>
       <c r="I48" s="6"/>
-      <c r="J48" s="21" t="s">
+      <c r="J48" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K48" s="20"/>
-      <c r="L48" s="20"/>
-      <c r="M48" s="20"/>
-      <c r="N48" s="22"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="19"/>
       <c r="O48" s="2"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="23" t="s">
+      <c r="C49" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="18"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="22"/>
       <c r="H49" s="14"/>
       <c r="I49" s="7"/>
-      <c r="J49" s="23" t="s">
+      <c r="J49" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K49" s="17"/>
-      <c r="L49" s="17"/>
-      <c r="M49" s="17"/>
-      <c r="N49" s="18"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="22"/>
       <c r="O49" s="2"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="23" t="s">
+      <c r="C50" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="18"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="22"/>
       <c r="H50" s="14"/>
       <c r="I50" s="7"/>
-      <c r="J50" s="23" t="s">
+      <c r="J50" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K50" s="17"/>
-      <c r="L50" s="17"/>
-      <c r="M50" s="17"/>
-      <c r="N50" s="18"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="22"/>
       <c r="O50" s="2"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
@@ -3212,39 +3215,39 @@
       <c r="C51" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="18"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="22"/>
       <c r="H51" s="14"/>
       <c r="I51" s="7"/>
       <c r="J51" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K51" s="17"/>
-      <c r="L51" s="17"/>
-      <c r="M51" s="17"/>
-      <c r="N51" s="18"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="22"/>
       <c r="O51" s="2"/>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
-      <c r="C52" s="16" t="s">
+      <c r="C52" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="18"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="22"/>
       <c r="H52" s="14"/>
       <c r="I52" s="7"/>
-      <c r="J52" s="16" t="s">
+      <c r="J52" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K52" s="17"/>
-      <c r="L52" s="17"/>
-      <c r="M52" s="17"/>
-      <c r="N52" s="18"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="21"/>
+      <c r="M52" s="21"/>
+      <c r="N52" s="22"/>
       <c r="O52" s="2"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
@@ -3344,20 +3347,20 @@
       <c r="O57" s="2"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="19" t="s">
+      <c r="B58" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
       <c r="E58" s="14"/>
       <c r="F58" s="4"/>
       <c r="G58" s="15"/>
       <c r="H58" s="14"/>
-      <c r="I58" s="19" t="s">
+      <c r="I58" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J58" s="20"/>
-      <c r="K58" s="20"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
       <c r="L58" s="14"/>
       <c r="M58" s="4"/>
       <c r="N58" s="15"/>
@@ -3399,103 +3402,103 @@
       <c r="O61" s="2"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="25"/>
-      <c r="C62" s="21" t="s">
+      <c r="B62" s="26"/>
+      <c r="C62" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="22"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="19"/>
       <c r="H62" s="14"/>
       <c r="I62" s="6"/>
-      <c r="J62" s="21" t="s">
+      <c r="J62" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K62" s="20"/>
-      <c r="L62" s="20"/>
-      <c r="M62" s="20"/>
-      <c r="N62" s="22"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="18"/>
+      <c r="M62" s="18"/>
+      <c r="N62" s="19"/>
       <c r="O62" s="2"/>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="26"/>
-      <c r="C63" s="23" t="s">
+      <c r="B63" s="27"/>
+      <c r="C63" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="18"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="22"/>
       <c r="H63" s="14"/>
       <c r="I63" s="7"/>
-      <c r="J63" s="23" t="s">
+      <c r="J63" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K63" s="17"/>
-      <c r="L63" s="17"/>
-      <c r="M63" s="17"/>
-      <c r="N63" s="18"/>
+      <c r="K63" s="21"/>
+      <c r="L63" s="21"/>
+      <c r="M63" s="21"/>
+      <c r="N63" s="22"/>
       <c r="O63" s="2"/>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="26"/>
-      <c r="C64" s="23" t="s">
+      <c r="B64" s="27"/>
+      <c r="C64" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="18"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="22"/>
       <c r="H64" s="14"/>
       <c r="I64" s="7"/>
-      <c r="J64" s="23" t="s">
+      <c r="J64" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K64" s="17"/>
-      <c r="L64" s="17"/>
-      <c r="M64" s="17"/>
-      <c r="N64" s="18"/>
+      <c r="K64" s="21"/>
+      <c r="L64" s="21"/>
+      <c r="M64" s="21"/>
+      <c r="N64" s="22"/>
       <c r="O64" s="2"/>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="26"/>
+      <c r="B65" s="27"/>
       <c r="C65" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="18"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="22"/>
       <c r="H65" s="14"/>
       <c r="I65" s="7"/>
       <c r="J65" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K65" s="17"/>
-      <c r="L65" s="17"/>
-      <c r="M65" s="17"/>
-      <c r="N65" s="18"/>
+      <c r="K65" s="21"/>
+      <c r="L65" s="21"/>
+      <c r="M65" s="21"/>
+      <c r="N65" s="22"/>
       <c r="O65" s="2"/>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="26"/>
-      <c r="C66" s="16" t="s">
+      <c r="B66" s="27"/>
+      <c r="C66" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="18"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="22"/>
       <c r="H66" s="14"/>
       <c r="I66" s="7"/>
-      <c r="J66" s="16" t="s">
+      <c r="J66" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K66" s="17"/>
-      <c r="L66" s="17"/>
-      <c r="M66" s="17"/>
-      <c r="N66" s="18"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="21"/>
+      <c r="M66" s="21"/>
+      <c r="N66" s="22"/>
       <c r="O66" s="2"/>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
@@ -3595,20 +3598,20 @@
       <c r="O71" s="2"/>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="19" t="s">
+      <c r="B72" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C72" s="20"/>
-      <c r="D72" s="20"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
       <c r="E72" s="14"/>
       <c r="F72" s="4"/>
       <c r="G72" s="15"/>
       <c r="H72" s="14"/>
-      <c r="I72" s="19" t="s">
+      <c r="I72" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J72" s="20"/>
-      <c r="K72" s="20"/>
+      <c r="J72" s="18"/>
+      <c r="K72" s="18"/>
       <c r="L72" s="14"/>
       <c r="M72" s="4"/>
       <c r="N72" s="15"/>
@@ -3664,62 +3667,62 @@
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
-      <c r="C76" s="21" t="s">
+      <c r="C76" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D76" s="20"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="20"/>
-      <c r="G76" s="22"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="19"/>
       <c r="H76" s="14"/>
       <c r="I76" s="6"/>
-      <c r="J76" s="21" t="s">
+      <c r="J76" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K76" s="20"/>
-      <c r="L76" s="20"/>
-      <c r="M76" s="20"/>
-      <c r="N76" s="22"/>
+      <c r="K76" s="18"/>
+      <c r="L76" s="18"/>
+      <c r="M76" s="18"/>
+      <c r="N76" s="19"/>
       <c r="O76" s="2"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B77" s="7"/>
-      <c r="C77" s="23" t="s">
+      <c r="C77" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="17"/>
-      <c r="G77" s="18"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="22"/>
       <c r="H77" s="14"/>
       <c r="I77" s="7"/>
-      <c r="J77" s="23" t="s">
+      <c r="J77" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K77" s="17"/>
-      <c r="L77" s="17"/>
-      <c r="M77" s="17"/>
-      <c r="N77" s="18"/>
+      <c r="K77" s="21"/>
+      <c r="L77" s="21"/>
+      <c r="M77" s="21"/>
+      <c r="N77" s="22"/>
       <c r="O77" s="2"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B78" s="7"/>
-      <c r="C78" s="23" t="s">
+      <c r="C78" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D78" s="17"/>
-      <c r="E78" s="17"/>
-      <c r="F78" s="17"/>
-      <c r="G78" s="18"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="22"/>
       <c r="H78" s="14"/>
       <c r="I78" s="7"/>
-      <c r="J78" s="23" t="s">
+      <c r="J78" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K78" s="17"/>
-      <c r="L78" s="17"/>
-      <c r="M78" s="17"/>
-      <c r="N78" s="18"/>
+      <c r="K78" s="21"/>
+      <c r="L78" s="21"/>
+      <c r="M78" s="21"/>
+      <c r="N78" s="22"/>
       <c r="O78" s="2"/>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
@@ -3727,39 +3730,39 @@
       <c r="C79" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D79" s="17"/>
-      <c r="E79" s="17"/>
-      <c r="F79" s="17"/>
-      <c r="G79" s="18"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="22"/>
       <c r="H79" s="14"/>
       <c r="I79" s="7"/>
       <c r="J79" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K79" s="17"/>
-      <c r="L79" s="17"/>
-      <c r="M79" s="17"/>
-      <c r="N79" s="18"/>
+      <c r="K79" s="21"/>
+      <c r="L79" s="21"/>
+      <c r="M79" s="21"/>
+      <c r="N79" s="22"/>
       <c r="O79" s="2"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B80" s="7"/>
-      <c r="C80" s="16" t="s">
+      <c r="C80" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="G80" s="18"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="22"/>
       <c r="H80" s="14"/>
       <c r="I80" s="7"/>
-      <c r="J80" s="16" t="s">
+      <c r="J80" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K80" s="17"/>
-      <c r="L80" s="17"/>
-      <c r="M80" s="17"/>
-      <c r="N80" s="18"/>
+      <c r="K80" s="21"/>
+      <c r="L80" s="21"/>
+      <c r="M80" s="21"/>
+      <c r="N80" s="22"/>
       <c r="O80" s="2"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
@@ -3859,20 +3862,20 @@
       <c r="O85" s="2"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B86" s="19" t="s">
+      <c r="B86" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C86" s="20"/>
-      <c r="D86" s="20"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="18"/>
       <c r="E86" s="14"/>
       <c r="F86" s="4"/>
       <c r="G86" s="15"/>
       <c r="H86" s="14"/>
-      <c r="I86" s="19" t="s">
+      <c r="I86" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J86" s="20"/>
-      <c r="K86" s="20"/>
+      <c r="J86" s="18"/>
+      <c r="K86" s="18"/>
       <c r="L86" s="14"/>
       <c r="M86" s="4"/>
       <c r="N86" s="15"/>
@@ -3914,103 +3917,103 @@
       <c r="O89" s="2"/>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B90" s="25"/>
-      <c r="C90" s="21" t="s">
+      <c r="B90" s="26"/>
+      <c r="C90" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D90" s="20"/>
-      <c r="E90" s="20"/>
-      <c r="F90" s="20"/>
-      <c r="G90" s="22"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="19"/>
       <c r="H90" s="14"/>
       <c r="I90" s="6"/>
-      <c r="J90" s="21" t="s">
+      <c r="J90" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K90" s="20"/>
-      <c r="L90" s="20"/>
-      <c r="M90" s="20"/>
-      <c r="N90" s="22"/>
+      <c r="K90" s="18"/>
+      <c r="L90" s="18"/>
+      <c r="M90" s="18"/>
+      <c r="N90" s="19"/>
       <c r="O90" s="2"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B91" s="26"/>
-      <c r="C91" s="23" t="s">
+      <c r="B91" s="27"/>
+      <c r="C91" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D91" s="17"/>
-      <c r="E91" s="17"/>
-      <c r="F91" s="17"/>
-      <c r="G91" s="18"/>
+      <c r="D91" s="21"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="21"/>
+      <c r="G91" s="22"/>
       <c r="H91" s="14"/>
       <c r="I91" s="7"/>
-      <c r="J91" s="23" t="s">
+      <c r="J91" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K91" s="17"/>
-      <c r="L91" s="17"/>
-      <c r="M91" s="17"/>
-      <c r="N91" s="18"/>
+      <c r="K91" s="21"/>
+      <c r="L91" s="21"/>
+      <c r="M91" s="21"/>
+      <c r="N91" s="22"/>
       <c r="O91" s="2"/>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B92" s="26"/>
-      <c r="C92" s="23" t="s">
+      <c r="B92" s="27"/>
+      <c r="C92" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D92" s="17"/>
-      <c r="E92" s="17"/>
-      <c r="F92" s="17"/>
-      <c r="G92" s="18"/>
+      <c r="D92" s="21"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="21"/>
+      <c r="G92" s="22"/>
       <c r="H92" s="14"/>
       <c r="I92" s="7"/>
-      <c r="J92" s="23" t="s">
+      <c r="J92" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K92" s="17"/>
-      <c r="L92" s="17"/>
-      <c r="M92" s="17"/>
-      <c r="N92" s="18"/>
+      <c r="K92" s="21"/>
+      <c r="L92" s="21"/>
+      <c r="M92" s="21"/>
+      <c r="N92" s="22"/>
       <c r="O92" s="2"/>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B93" s="26"/>
+      <c r="B93" s="27"/>
       <c r="C93" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D93" s="17"/>
-      <c r="E93" s="17"/>
-      <c r="F93" s="17"/>
-      <c r="G93" s="18"/>
+      <c r="D93" s="21"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="22"/>
       <c r="H93" s="14"/>
       <c r="I93" s="7"/>
       <c r="J93" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K93" s="17"/>
-      <c r="L93" s="17"/>
-      <c r="M93" s="17"/>
-      <c r="N93" s="18"/>
+      <c r="K93" s="21"/>
+      <c r="L93" s="21"/>
+      <c r="M93" s="21"/>
+      <c r="N93" s="22"/>
       <c r="O93" s="2"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B94" s="26"/>
-      <c r="C94" s="16" t="s">
+      <c r="B94" s="27"/>
+      <c r="C94" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D94" s="17"/>
-      <c r="E94" s="17"/>
-      <c r="F94" s="17"/>
-      <c r="G94" s="18"/>
+      <c r="D94" s="21"/>
+      <c r="E94" s="21"/>
+      <c r="F94" s="21"/>
+      <c r="G94" s="22"/>
       <c r="H94" s="14"/>
       <c r="I94" s="7"/>
-      <c r="J94" s="16" t="s">
+      <c r="J94" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K94" s="17"/>
-      <c r="L94" s="17"/>
-      <c r="M94" s="17"/>
-      <c r="N94" s="18"/>
+      <c r="K94" s="21"/>
+      <c r="L94" s="21"/>
+      <c r="M94" s="21"/>
+      <c r="N94" s="22"/>
       <c r="O94" s="2"/>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
@@ -4110,20 +4113,20 @@
       <c r="O99" s="2"/>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B100" s="19" t="s">
+      <c r="B100" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C100" s="20"/>
-      <c r="D100" s="20"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="18"/>
       <c r="E100" s="14"/>
       <c r="F100" s="4"/>
       <c r="G100" s="15"/>
       <c r="H100" s="14"/>
-      <c r="I100" s="19" t="s">
+      <c r="I100" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J100" s="20"/>
-      <c r="K100" s="20"/>
+      <c r="J100" s="18"/>
+      <c r="K100" s="18"/>
       <c r="L100" s="14"/>
       <c r="M100" s="4"/>
       <c r="N100" s="15"/>
@@ -4179,62 +4182,62 @@
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104" s="6"/>
-      <c r="C104" s="21" t="s">
+      <c r="C104" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D104" s="20"/>
-      <c r="E104" s="20"/>
-      <c r="F104" s="20"/>
-      <c r="G104" s="22"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="18"/>
+      <c r="G104" s="19"/>
       <c r="H104" s="14"/>
       <c r="I104" s="6"/>
-      <c r="J104" s="21" t="s">
+      <c r="J104" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K104" s="20"/>
-      <c r="L104" s="20"/>
-      <c r="M104" s="20"/>
-      <c r="N104" s="22"/>
+      <c r="K104" s="18"/>
+      <c r="L104" s="18"/>
+      <c r="M104" s="18"/>
+      <c r="N104" s="19"/>
       <c r="O104" s="2"/>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B105" s="7"/>
-      <c r="C105" s="23" t="s">
+      <c r="C105" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D105" s="17"/>
-      <c r="E105" s="17"/>
-      <c r="F105" s="17"/>
-      <c r="G105" s="18"/>
+      <c r="D105" s="21"/>
+      <c r="E105" s="21"/>
+      <c r="F105" s="21"/>
+      <c r="G105" s="22"/>
       <c r="H105" s="14"/>
       <c r="I105" s="7"/>
-      <c r="J105" s="23" t="s">
+      <c r="J105" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K105" s="17"/>
-      <c r="L105" s="17"/>
-      <c r="M105" s="17"/>
-      <c r="N105" s="18"/>
+      <c r="K105" s="21"/>
+      <c r="L105" s="21"/>
+      <c r="M105" s="21"/>
+      <c r="N105" s="22"/>
       <c r="O105" s="2"/>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106" s="7"/>
-      <c r="C106" s="23" t="s">
+      <c r="C106" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D106" s="17"/>
-      <c r="E106" s="17"/>
-      <c r="F106" s="17"/>
-      <c r="G106" s="18"/>
+      <c r="D106" s="21"/>
+      <c r="E106" s="21"/>
+      <c r="F106" s="21"/>
+      <c r="G106" s="22"/>
       <c r="H106" s="14"/>
       <c r="I106" s="7"/>
-      <c r="J106" s="23" t="s">
+      <c r="J106" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K106" s="17"/>
-      <c r="L106" s="17"/>
-      <c r="M106" s="17"/>
-      <c r="N106" s="18"/>
+      <c r="K106" s="21"/>
+      <c r="L106" s="21"/>
+      <c r="M106" s="21"/>
+      <c r="N106" s="22"/>
       <c r="O106" s="2"/>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
@@ -4242,39 +4245,39 @@
       <c r="C107" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D107" s="17"/>
-      <c r="E107" s="17"/>
-      <c r="F107" s="17"/>
-      <c r="G107" s="18"/>
+      <c r="D107" s="21"/>
+      <c r="E107" s="21"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="22"/>
       <c r="H107" s="14"/>
       <c r="I107" s="7"/>
       <c r="J107" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K107" s="17"/>
-      <c r="L107" s="17"/>
-      <c r="M107" s="17"/>
-      <c r="N107" s="18"/>
+      <c r="K107" s="21"/>
+      <c r="L107" s="21"/>
+      <c r="M107" s="21"/>
+      <c r="N107" s="22"/>
       <c r="O107" s="2"/>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B108" s="7"/>
-      <c r="C108" s="16" t="s">
+      <c r="C108" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D108" s="17"/>
-      <c r="E108" s="17"/>
-      <c r="F108" s="17"/>
-      <c r="G108" s="18"/>
+      <c r="D108" s="21"/>
+      <c r="E108" s="21"/>
+      <c r="F108" s="21"/>
+      <c r="G108" s="22"/>
       <c r="H108" s="14"/>
       <c r="I108" s="7"/>
-      <c r="J108" s="16" t="s">
+      <c r="J108" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K108" s="17"/>
-      <c r="L108" s="17"/>
-      <c r="M108" s="17"/>
-      <c r="N108" s="18"/>
+      <c r="K108" s="21"/>
+      <c r="L108" s="21"/>
+      <c r="M108" s="21"/>
+      <c r="N108" s="22"/>
       <c r="O108" s="2"/>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.25">
@@ -4374,20 +4377,20 @@
       <c r="O113" s="2"/>
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B114" s="19" t="s">
+      <c r="B114" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C114" s="20"/>
-      <c r="D114" s="20"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="18"/>
       <c r="E114" s="14"/>
       <c r="F114" s="4"/>
       <c r="G114" s="15"/>
       <c r="H114" s="14"/>
-      <c r="I114" s="19" t="s">
+      <c r="I114" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J114" s="20"/>
-      <c r="K114" s="20"/>
+      <c r="J114" s="18"/>
+      <c r="K114" s="18"/>
       <c r="L114" s="14"/>
       <c r="M114" s="4"/>
       <c r="N114" s="15"/>
@@ -4429,103 +4432,103 @@
       <c r="O117" s="2"/>
     </row>
     <row r="118" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B118" s="25"/>
-      <c r="C118" s="21" t="s">
+      <c r="B118" s="26"/>
+      <c r="C118" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D118" s="20"/>
-      <c r="E118" s="20"/>
-      <c r="F118" s="20"/>
-      <c r="G118" s="22"/>
+      <c r="D118" s="18"/>
+      <c r="E118" s="18"/>
+      <c r="F118" s="18"/>
+      <c r="G118" s="19"/>
       <c r="H118" s="14"/>
       <c r="I118" s="6"/>
-      <c r="J118" s="21" t="s">
+      <c r="J118" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K118" s="20"/>
-      <c r="L118" s="20"/>
-      <c r="M118" s="20"/>
-      <c r="N118" s="22"/>
+      <c r="K118" s="18"/>
+      <c r="L118" s="18"/>
+      <c r="M118" s="18"/>
+      <c r="N118" s="19"/>
       <c r="O118" s="2"/>
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B119" s="26"/>
-      <c r="C119" s="23" t="s">
+      <c r="B119" s="27"/>
+      <c r="C119" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D119" s="17"/>
-      <c r="E119" s="17"/>
-      <c r="F119" s="17"/>
-      <c r="G119" s="18"/>
+      <c r="D119" s="21"/>
+      <c r="E119" s="21"/>
+      <c r="F119" s="21"/>
+      <c r="G119" s="22"/>
       <c r="H119" s="14"/>
       <c r="I119" s="7"/>
-      <c r="J119" s="23" t="s">
+      <c r="J119" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K119" s="17"/>
-      <c r="L119" s="17"/>
-      <c r="M119" s="17"/>
-      <c r="N119" s="18"/>
+      <c r="K119" s="21"/>
+      <c r="L119" s="21"/>
+      <c r="M119" s="21"/>
+      <c r="N119" s="22"/>
       <c r="O119" s="2"/>
     </row>
     <row r="120" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B120" s="26"/>
-      <c r="C120" s="23" t="s">
+      <c r="B120" s="27"/>
+      <c r="C120" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D120" s="17"/>
-      <c r="E120" s="17"/>
-      <c r="F120" s="17"/>
-      <c r="G120" s="18"/>
+      <c r="D120" s="21"/>
+      <c r="E120" s="21"/>
+      <c r="F120" s="21"/>
+      <c r="G120" s="22"/>
       <c r="H120" s="14"/>
       <c r="I120" s="7"/>
-      <c r="J120" s="23" t="s">
+      <c r="J120" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K120" s="17"/>
-      <c r="L120" s="17"/>
-      <c r="M120" s="17"/>
-      <c r="N120" s="18"/>
+      <c r="K120" s="21"/>
+      <c r="L120" s="21"/>
+      <c r="M120" s="21"/>
+      <c r="N120" s="22"/>
       <c r="O120" s="2"/>
     </row>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B121" s="26"/>
+      <c r="B121" s="27"/>
       <c r="C121" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D121" s="17"/>
-      <c r="E121" s="17"/>
-      <c r="F121" s="17"/>
-      <c r="G121" s="18"/>
+      <c r="D121" s="21"/>
+      <c r="E121" s="21"/>
+      <c r="F121" s="21"/>
+      <c r="G121" s="22"/>
       <c r="H121" s="14"/>
       <c r="I121" s="7"/>
       <c r="J121" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K121" s="17"/>
-      <c r="L121" s="17"/>
-      <c r="M121" s="17"/>
-      <c r="N121" s="18"/>
+      <c r="K121" s="21"/>
+      <c r="L121" s="21"/>
+      <c r="M121" s="21"/>
+      <c r="N121" s="22"/>
       <c r="O121" s="2"/>
     </row>
     <row r="122" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B122" s="26"/>
-      <c r="C122" s="16" t="s">
+      <c r="B122" s="27"/>
+      <c r="C122" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D122" s="17"/>
-      <c r="E122" s="17"/>
-      <c r="F122" s="17"/>
-      <c r="G122" s="18"/>
+      <c r="D122" s="21"/>
+      <c r="E122" s="21"/>
+      <c r="F122" s="21"/>
+      <c r="G122" s="22"/>
       <c r="H122" s="14"/>
       <c r="I122" s="7"/>
-      <c r="J122" s="16" t="s">
+      <c r="J122" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K122" s="17"/>
-      <c r="L122" s="17"/>
-      <c r="M122" s="17"/>
-      <c r="N122" s="18"/>
+      <c r="K122" s="21"/>
+      <c r="L122" s="21"/>
+      <c r="M122" s="21"/>
+      <c r="N122" s="22"/>
       <c r="O122" s="2"/>
     </row>
     <row r="123" spans="2:15" x14ac:dyDescent="0.25">
@@ -4625,20 +4628,20 @@
       <c r="O127" s="2"/>
     </row>
     <row r="128" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B128" s="19" t="s">
+      <c r="B128" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C128" s="20"/>
-      <c r="D128" s="20"/>
+      <c r="C128" s="18"/>
+      <c r="D128" s="18"/>
       <c r="E128" s="14"/>
       <c r="F128" s="4"/>
       <c r="G128" s="15"/>
       <c r="H128" s="14"/>
-      <c r="I128" s="19" t="s">
+      <c r="I128" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J128" s="20"/>
-      <c r="K128" s="20"/>
+      <c r="J128" s="18"/>
+      <c r="K128" s="18"/>
       <c r="L128" s="14"/>
       <c r="M128" s="4"/>
       <c r="N128" s="15"/>
@@ -4694,62 +4697,62 @@
     </row>
     <row r="132" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
-      <c r="C132" s="21" t="s">
+      <c r="C132" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D132" s="20"/>
-      <c r="E132" s="20"/>
-      <c r="F132" s="20"/>
-      <c r="G132" s="22"/>
+      <c r="D132" s="18"/>
+      <c r="E132" s="18"/>
+      <c r="F132" s="18"/>
+      <c r="G132" s="19"/>
       <c r="H132" s="14"/>
       <c r="I132" s="6"/>
-      <c r="J132" s="21" t="s">
+      <c r="J132" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K132" s="20"/>
-      <c r="L132" s="20"/>
-      <c r="M132" s="20"/>
-      <c r="N132" s="22"/>
+      <c r="K132" s="18"/>
+      <c r="L132" s="18"/>
+      <c r="M132" s="18"/>
+      <c r="N132" s="19"/>
       <c r="O132" s="2"/>
     </row>
     <row r="133" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B133" s="7"/>
-      <c r="C133" s="23" t="s">
+      <c r="C133" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D133" s="17"/>
-      <c r="E133" s="17"/>
-      <c r="F133" s="17"/>
-      <c r="G133" s="18"/>
+      <c r="D133" s="21"/>
+      <c r="E133" s="21"/>
+      <c r="F133" s="21"/>
+      <c r="G133" s="22"/>
       <c r="H133" s="14"/>
       <c r="I133" s="7"/>
-      <c r="J133" s="23" t="s">
+      <c r="J133" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K133" s="17"/>
-      <c r="L133" s="17"/>
-      <c r="M133" s="17"/>
-      <c r="N133" s="18"/>
+      <c r="K133" s="21"/>
+      <c r="L133" s="21"/>
+      <c r="M133" s="21"/>
+      <c r="N133" s="22"/>
       <c r="O133" s="2"/>
     </row>
     <row r="134" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B134" s="7"/>
-      <c r="C134" s="23" t="s">
+      <c r="C134" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D134" s="17"/>
-      <c r="E134" s="17"/>
-      <c r="F134" s="17"/>
-      <c r="G134" s="18"/>
+      <c r="D134" s="21"/>
+      <c r="E134" s="21"/>
+      <c r="F134" s="21"/>
+      <c r="G134" s="22"/>
       <c r="H134" s="14"/>
       <c r="I134" s="7"/>
-      <c r="J134" s="23" t="s">
+      <c r="J134" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K134" s="17"/>
-      <c r="L134" s="17"/>
-      <c r="M134" s="17"/>
-      <c r="N134" s="18"/>
+      <c r="K134" s="21"/>
+      <c r="L134" s="21"/>
+      <c r="M134" s="21"/>
+      <c r="N134" s="22"/>
       <c r="O134" s="2"/>
     </row>
     <row r="135" spans="2:15" x14ac:dyDescent="0.25">
@@ -4757,39 +4760,39 @@
       <c r="C135" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D135" s="17"/>
-      <c r="E135" s="17"/>
-      <c r="F135" s="17"/>
-      <c r="G135" s="18"/>
+      <c r="D135" s="21"/>
+      <c r="E135" s="21"/>
+      <c r="F135" s="21"/>
+      <c r="G135" s="22"/>
       <c r="H135" s="14"/>
       <c r="I135" s="7"/>
       <c r="J135" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K135" s="17"/>
-      <c r="L135" s="17"/>
-      <c r="M135" s="17"/>
-      <c r="N135" s="18"/>
+      <c r="K135" s="21"/>
+      <c r="L135" s="21"/>
+      <c r="M135" s="21"/>
+      <c r="N135" s="22"/>
       <c r="O135" s="2"/>
     </row>
     <row r="136" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B136" s="7"/>
-      <c r="C136" s="16" t="s">
+      <c r="C136" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D136" s="17"/>
-      <c r="E136" s="17"/>
-      <c r="F136" s="17"/>
-      <c r="G136" s="18"/>
+      <c r="D136" s="21"/>
+      <c r="E136" s="21"/>
+      <c r="F136" s="21"/>
+      <c r="G136" s="22"/>
       <c r="H136" s="14"/>
       <c r="I136" s="7"/>
-      <c r="J136" s="16" t="s">
+      <c r="J136" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K136" s="17"/>
-      <c r="L136" s="17"/>
-      <c r="M136" s="17"/>
-      <c r="N136" s="18"/>
+      <c r="K136" s="21"/>
+      <c r="L136" s="21"/>
+      <c r="M136" s="21"/>
+      <c r="N136" s="22"/>
       <c r="O136" s="2"/>
     </row>
     <row r="137" spans="2:15" x14ac:dyDescent="0.25">
@@ -4889,20 +4892,20 @@
       <c r="O141" s="2"/>
     </row>
     <row r="142" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B142" s="19" t="s">
+      <c r="B142" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C142" s="20"/>
-      <c r="D142" s="20"/>
+      <c r="C142" s="18"/>
+      <c r="D142" s="18"/>
       <c r="E142" s="14"/>
       <c r="F142" s="4"/>
       <c r="G142" s="15"/>
       <c r="H142" s="14"/>
-      <c r="I142" s="19" t="s">
+      <c r="I142" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J142" s="20"/>
-      <c r="K142" s="20"/>
+      <c r="J142" s="18"/>
+      <c r="K142" s="18"/>
       <c r="L142" s="14"/>
       <c r="M142" s="4"/>
       <c r="N142" s="15"/>
@@ -4944,103 +4947,103 @@
       <c r="O145" s="2"/>
     </row>
     <row r="146" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B146" s="25"/>
-      <c r="C146" s="21" t="s">
+      <c r="B146" s="26"/>
+      <c r="C146" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D146" s="20"/>
-      <c r="E146" s="20"/>
-      <c r="F146" s="20"/>
-      <c r="G146" s="22"/>
+      <c r="D146" s="18"/>
+      <c r="E146" s="18"/>
+      <c r="F146" s="18"/>
+      <c r="G146" s="19"/>
       <c r="H146" s="14"/>
       <c r="I146" s="6"/>
-      <c r="J146" s="21" t="s">
+      <c r="J146" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K146" s="20"/>
-      <c r="L146" s="20"/>
-      <c r="M146" s="20"/>
-      <c r="N146" s="22"/>
+      <c r="K146" s="18"/>
+      <c r="L146" s="18"/>
+      <c r="M146" s="18"/>
+      <c r="N146" s="19"/>
       <c r="O146" s="2"/>
     </row>
     <row r="147" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B147" s="26"/>
-      <c r="C147" s="23" t="s">
+      <c r="B147" s="27"/>
+      <c r="C147" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D147" s="17"/>
-      <c r="E147" s="17"/>
-      <c r="F147" s="17"/>
-      <c r="G147" s="18"/>
+      <c r="D147" s="21"/>
+      <c r="E147" s="21"/>
+      <c r="F147" s="21"/>
+      <c r="G147" s="22"/>
       <c r="H147" s="14"/>
       <c r="I147" s="7"/>
-      <c r="J147" s="23" t="s">
+      <c r="J147" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K147" s="17"/>
-      <c r="L147" s="17"/>
-      <c r="M147" s="17"/>
-      <c r="N147" s="18"/>
+      <c r="K147" s="21"/>
+      <c r="L147" s="21"/>
+      <c r="M147" s="21"/>
+      <c r="N147" s="22"/>
       <c r="O147" s="2"/>
     </row>
     <row r="148" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B148" s="26"/>
-      <c r="C148" s="23" t="s">
+      <c r="B148" s="27"/>
+      <c r="C148" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D148" s="17"/>
-      <c r="E148" s="17"/>
-      <c r="F148" s="17"/>
-      <c r="G148" s="18"/>
+      <c r="D148" s="21"/>
+      <c r="E148" s="21"/>
+      <c r="F148" s="21"/>
+      <c r="G148" s="22"/>
       <c r="H148" s="14"/>
       <c r="I148" s="7"/>
-      <c r="J148" s="23" t="s">
+      <c r="J148" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K148" s="17"/>
-      <c r="L148" s="17"/>
-      <c r="M148" s="17"/>
-      <c r="N148" s="18"/>
+      <c r="K148" s="21"/>
+      <c r="L148" s="21"/>
+      <c r="M148" s="21"/>
+      <c r="N148" s="22"/>
       <c r="O148" s="2"/>
     </row>
     <row r="149" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B149" s="26"/>
+      <c r="B149" s="27"/>
       <c r="C149" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D149" s="17"/>
-      <c r="E149" s="17"/>
-      <c r="F149" s="17"/>
-      <c r="G149" s="18"/>
+      <c r="D149" s="21"/>
+      <c r="E149" s="21"/>
+      <c r="F149" s="21"/>
+      <c r="G149" s="22"/>
       <c r="H149" s="14"/>
       <c r="I149" s="7"/>
       <c r="J149" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K149" s="17"/>
-      <c r="L149" s="17"/>
-      <c r="M149" s="17"/>
-      <c r="N149" s="18"/>
+      <c r="K149" s="21"/>
+      <c r="L149" s="21"/>
+      <c r="M149" s="21"/>
+      <c r="N149" s="22"/>
       <c r="O149" s="2"/>
     </row>
     <row r="150" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B150" s="26"/>
-      <c r="C150" s="16" t="s">
+      <c r="B150" s="27"/>
+      <c r="C150" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D150" s="17"/>
-      <c r="E150" s="17"/>
-      <c r="F150" s="17"/>
-      <c r="G150" s="18"/>
+      <c r="D150" s="21"/>
+      <c r="E150" s="21"/>
+      <c r="F150" s="21"/>
+      <c r="G150" s="22"/>
       <c r="H150" s="14"/>
       <c r="I150" s="7"/>
-      <c r="J150" s="16" t="s">
+      <c r="J150" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K150" s="17"/>
-      <c r="L150" s="17"/>
-      <c r="M150" s="17"/>
-      <c r="N150" s="18"/>
+      <c r="K150" s="21"/>
+      <c r="L150" s="21"/>
+      <c r="M150" s="21"/>
+      <c r="N150" s="22"/>
       <c r="O150" s="2"/>
     </row>
     <row r="151" spans="2:15" x14ac:dyDescent="0.25">
@@ -5140,20 +5143,20 @@
       <c r="O155" s="2"/>
     </row>
     <row r="156" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B156" s="19" t="s">
+      <c r="B156" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C156" s="20"/>
-      <c r="D156" s="20"/>
+      <c r="C156" s="18"/>
+      <c r="D156" s="18"/>
       <c r="E156" s="14"/>
       <c r="F156" s="4"/>
       <c r="G156" s="15"/>
       <c r="H156" s="14"/>
-      <c r="I156" s="19" t="s">
+      <c r="I156" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J156" s="20"/>
-      <c r="K156" s="20"/>
+      <c r="J156" s="18"/>
+      <c r="K156" s="18"/>
       <c r="L156" s="14"/>
       <c r="M156" s="4"/>
       <c r="N156" s="15"/>
@@ -5209,62 +5212,62 @@
     </row>
     <row r="160" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
-      <c r="C160" s="21" t="s">
+      <c r="C160" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D160" s="20"/>
-      <c r="E160" s="20"/>
-      <c r="F160" s="20"/>
-      <c r="G160" s="22"/>
+      <c r="D160" s="18"/>
+      <c r="E160" s="18"/>
+      <c r="F160" s="18"/>
+      <c r="G160" s="19"/>
       <c r="H160" s="14"/>
       <c r="I160" s="6"/>
-      <c r="J160" s="21" t="s">
+      <c r="J160" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K160" s="20"/>
-      <c r="L160" s="20"/>
-      <c r="M160" s="20"/>
-      <c r="N160" s="22"/>
+      <c r="K160" s="18"/>
+      <c r="L160" s="18"/>
+      <c r="M160" s="18"/>
+      <c r="N160" s="19"/>
       <c r="O160" s="2"/>
     </row>
     <row r="161" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B161" s="7"/>
-      <c r="C161" s="23" t="s">
+      <c r="C161" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D161" s="17"/>
-      <c r="E161" s="17"/>
-      <c r="F161" s="17"/>
-      <c r="G161" s="18"/>
+      <c r="D161" s="21"/>
+      <c r="E161" s="21"/>
+      <c r="F161" s="21"/>
+      <c r="G161" s="22"/>
       <c r="H161" s="14"/>
       <c r="I161" s="7"/>
-      <c r="J161" s="23" t="s">
+      <c r="J161" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K161" s="17"/>
-      <c r="L161" s="17"/>
-      <c r="M161" s="17"/>
-      <c r="N161" s="18"/>
+      <c r="K161" s="21"/>
+      <c r="L161" s="21"/>
+      <c r="M161" s="21"/>
+      <c r="N161" s="22"/>
       <c r="O161" s="2"/>
     </row>
     <row r="162" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B162" s="7"/>
-      <c r="C162" s="23" t="s">
+      <c r="C162" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D162" s="17"/>
-      <c r="E162" s="17"/>
-      <c r="F162" s="17"/>
-      <c r="G162" s="18"/>
+      <c r="D162" s="21"/>
+      <c r="E162" s="21"/>
+      <c r="F162" s="21"/>
+      <c r="G162" s="22"/>
       <c r="H162" s="14"/>
       <c r="I162" s="7"/>
-      <c r="J162" s="23" t="s">
+      <c r="J162" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K162" s="17"/>
-      <c r="L162" s="17"/>
-      <c r="M162" s="17"/>
-      <c r="N162" s="18"/>
+      <c r="K162" s="21"/>
+      <c r="L162" s="21"/>
+      <c r="M162" s="21"/>
+      <c r="N162" s="22"/>
       <c r="O162" s="2"/>
     </row>
     <row r="163" spans="2:15" x14ac:dyDescent="0.25">
@@ -5272,39 +5275,39 @@
       <c r="C163" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D163" s="17"/>
-      <c r="E163" s="17"/>
-      <c r="F163" s="17"/>
-      <c r="G163" s="18"/>
+      <c r="D163" s="21"/>
+      <c r="E163" s="21"/>
+      <c r="F163" s="21"/>
+      <c r="G163" s="22"/>
       <c r="H163" s="14"/>
       <c r="I163" s="7"/>
       <c r="J163" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K163" s="17"/>
-      <c r="L163" s="17"/>
-      <c r="M163" s="17"/>
-      <c r="N163" s="18"/>
+      <c r="K163" s="21"/>
+      <c r="L163" s="21"/>
+      <c r="M163" s="21"/>
+      <c r="N163" s="22"/>
       <c r="O163" s="2"/>
     </row>
     <row r="164" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B164" s="7"/>
-      <c r="C164" s="16" t="s">
+      <c r="C164" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D164" s="17"/>
-      <c r="E164" s="17"/>
-      <c r="F164" s="17"/>
-      <c r="G164" s="18"/>
+      <c r="D164" s="21"/>
+      <c r="E164" s="21"/>
+      <c r="F164" s="21"/>
+      <c r="G164" s="22"/>
       <c r="H164" s="14"/>
       <c r="I164" s="7"/>
-      <c r="J164" s="16" t="s">
+      <c r="J164" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K164" s="17"/>
-      <c r="L164" s="17"/>
-      <c r="M164" s="17"/>
-      <c r="N164" s="18"/>
+      <c r="K164" s="21"/>
+      <c r="L164" s="21"/>
+      <c r="M164" s="21"/>
+      <c r="N164" s="22"/>
       <c r="O164" s="2"/>
     </row>
     <row r="165" spans="2:15" x14ac:dyDescent="0.25">
@@ -5404,20 +5407,20 @@
       <c r="O169" s="2"/>
     </row>
     <row r="170" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B170" s="19" t="s">
+      <c r="B170" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C170" s="20"/>
-      <c r="D170" s="20"/>
+      <c r="C170" s="18"/>
+      <c r="D170" s="18"/>
       <c r="E170" s="14"/>
       <c r="F170" s="4"/>
       <c r="G170" s="15"/>
       <c r="H170" s="14"/>
-      <c r="I170" s="19" t="s">
+      <c r="I170" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J170" s="20"/>
-      <c r="K170" s="20"/>
+      <c r="J170" s="18"/>
+      <c r="K170" s="18"/>
       <c r="L170" s="14"/>
       <c r="M170" s="4"/>
       <c r="N170" s="15"/>
@@ -5459,103 +5462,103 @@
       <c r="O173" s="2"/>
     </row>
     <row r="174" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B174" s="25"/>
-      <c r="C174" s="21" t="s">
+      <c r="B174" s="26"/>
+      <c r="C174" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D174" s="20"/>
-      <c r="E174" s="20"/>
-      <c r="F174" s="20"/>
-      <c r="G174" s="22"/>
+      <c r="D174" s="18"/>
+      <c r="E174" s="18"/>
+      <c r="F174" s="18"/>
+      <c r="G174" s="19"/>
       <c r="H174" s="14"/>
       <c r="I174" s="6"/>
-      <c r="J174" s="21" t="s">
+      <c r="J174" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K174" s="20"/>
-      <c r="L174" s="20"/>
-      <c r="M174" s="20"/>
-      <c r="N174" s="22"/>
+      <c r="K174" s="18"/>
+      <c r="L174" s="18"/>
+      <c r="M174" s="18"/>
+      <c r="N174" s="19"/>
       <c r="O174" s="2"/>
     </row>
     <row r="175" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B175" s="26"/>
-      <c r="C175" s="23" t="s">
+      <c r="B175" s="27"/>
+      <c r="C175" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D175" s="17"/>
-      <c r="E175" s="17"/>
-      <c r="F175" s="17"/>
-      <c r="G175" s="18"/>
+      <c r="D175" s="21"/>
+      <c r="E175" s="21"/>
+      <c r="F175" s="21"/>
+      <c r="G175" s="22"/>
       <c r="H175" s="14"/>
       <c r="I175" s="7"/>
-      <c r="J175" s="23" t="s">
+      <c r="J175" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K175" s="17"/>
-      <c r="L175" s="17"/>
-      <c r="M175" s="17"/>
-      <c r="N175" s="18"/>
+      <c r="K175" s="21"/>
+      <c r="L175" s="21"/>
+      <c r="M175" s="21"/>
+      <c r="N175" s="22"/>
       <c r="O175" s="2"/>
     </row>
     <row r="176" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B176" s="26"/>
-      <c r="C176" s="23" t="s">
+      <c r="B176" s="27"/>
+      <c r="C176" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D176" s="17"/>
-      <c r="E176" s="17"/>
-      <c r="F176" s="17"/>
-      <c r="G176" s="18"/>
+      <c r="D176" s="21"/>
+      <c r="E176" s="21"/>
+      <c r="F176" s="21"/>
+      <c r="G176" s="22"/>
       <c r="H176" s="14"/>
       <c r="I176" s="7"/>
-      <c r="J176" s="23" t="s">
+      <c r="J176" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K176" s="17"/>
-      <c r="L176" s="17"/>
-      <c r="M176" s="17"/>
-      <c r="N176" s="18"/>
+      <c r="K176" s="21"/>
+      <c r="L176" s="21"/>
+      <c r="M176" s="21"/>
+      <c r="N176" s="22"/>
       <c r="O176" s="2"/>
     </row>
     <row r="177" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B177" s="26"/>
+      <c r="B177" s="27"/>
       <c r="C177" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D177" s="17"/>
-      <c r="E177" s="17"/>
-      <c r="F177" s="17"/>
-      <c r="G177" s="18"/>
+      <c r="D177" s="21"/>
+      <c r="E177" s="21"/>
+      <c r="F177" s="21"/>
+      <c r="G177" s="22"/>
       <c r="H177" s="14"/>
       <c r="I177" s="7"/>
       <c r="J177" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K177" s="17"/>
-      <c r="L177" s="17"/>
-      <c r="M177" s="17"/>
-      <c r="N177" s="18"/>
+      <c r="K177" s="21"/>
+      <c r="L177" s="21"/>
+      <c r="M177" s="21"/>
+      <c r="N177" s="22"/>
       <c r="O177" s="2"/>
     </row>
     <row r="178" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B178" s="26"/>
-      <c r="C178" s="16" t="s">
+      <c r="B178" s="27"/>
+      <c r="C178" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D178" s="17"/>
-      <c r="E178" s="17"/>
-      <c r="F178" s="17"/>
-      <c r="G178" s="18"/>
+      <c r="D178" s="21"/>
+      <c r="E178" s="21"/>
+      <c r="F178" s="21"/>
+      <c r="G178" s="22"/>
       <c r="H178" s="14"/>
       <c r="I178" s="7"/>
-      <c r="J178" s="16" t="s">
+      <c r="J178" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K178" s="17"/>
-      <c r="L178" s="17"/>
-      <c r="M178" s="17"/>
-      <c r="N178" s="18"/>
+      <c r="K178" s="21"/>
+      <c r="L178" s="21"/>
+      <c r="M178" s="21"/>
+      <c r="N178" s="22"/>
       <c r="O178" s="2"/>
     </row>
     <row r="179" spans="2:15" x14ac:dyDescent="0.25">
@@ -5655,20 +5658,20 @@
       <c r="O183" s="2"/>
     </row>
     <row r="184" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B184" s="19" t="s">
+      <c r="B184" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C184" s="20"/>
-      <c r="D184" s="20"/>
+      <c r="C184" s="18"/>
+      <c r="D184" s="18"/>
       <c r="E184" s="14"/>
       <c r="F184" s="4"/>
       <c r="G184" s="15"/>
       <c r="H184" s="14"/>
-      <c r="I184" s="19" t="s">
+      <c r="I184" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J184" s="20"/>
-      <c r="K184" s="20"/>
+      <c r="J184" s="18"/>
+      <c r="K184" s="18"/>
       <c r="L184" s="14"/>
       <c r="M184" s="4"/>
       <c r="N184" s="15"/>
@@ -5724,62 +5727,62 @@
     </row>
     <row r="188" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
-      <c r="C188" s="21" t="s">
+      <c r="C188" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D188" s="20"/>
-      <c r="E188" s="20"/>
-      <c r="F188" s="20"/>
-      <c r="G188" s="22"/>
+      <c r="D188" s="18"/>
+      <c r="E188" s="18"/>
+      <c r="F188" s="18"/>
+      <c r="G188" s="19"/>
       <c r="H188" s="14"/>
       <c r="I188" s="6"/>
-      <c r="J188" s="21" t="s">
+      <c r="J188" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K188" s="20"/>
-      <c r="L188" s="20"/>
-      <c r="M188" s="20"/>
-      <c r="N188" s="22"/>
+      <c r="K188" s="18"/>
+      <c r="L188" s="18"/>
+      <c r="M188" s="18"/>
+      <c r="N188" s="19"/>
       <c r="O188" s="2"/>
     </row>
     <row r="189" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B189" s="7"/>
-      <c r="C189" s="23" t="s">
+      <c r="C189" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D189" s="17"/>
-      <c r="E189" s="17"/>
-      <c r="F189" s="17"/>
-      <c r="G189" s="18"/>
+      <c r="D189" s="21"/>
+      <c r="E189" s="21"/>
+      <c r="F189" s="21"/>
+      <c r="G189" s="22"/>
       <c r="H189" s="14"/>
       <c r="I189" s="7"/>
-      <c r="J189" s="23" t="s">
+      <c r="J189" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K189" s="17"/>
-      <c r="L189" s="17"/>
-      <c r="M189" s="17"/>
-      <c r="N189" s="18"/>
+      <c r="K189" s="21"/>
+      <c r="L189" s="21"/>
+      <c r="M189" s="21"/>
+      <c r="N189" s="22"/>
       <c r="O189" s="2"/>
     </row>
     <row r="190" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B190" s="7"/>
-      <c r="C190" s="23" t="s">
+      <c r="C190" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D190" s="17"/>
-      <c r="E190" s="17"/>
-      <c r="F190" s="17"/>
-      <c r="G190" s="18"/>
+      <c r="D190" s="21"/>
+      <c r="E190" s="21"/>
+      <c r="F190" s="21"/>
+      <c r="G190" s="22"/>
       <c r="H190" s="14"/>
       <c r="I190" s="7"/>
-      <c r="J190" s="23" t="s">
+      <c r="J190" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K190" s="17"/>
-      <c r="L190" s="17"/>
-      <c r="M190" s="17"/>
-      <c r="N190" s="18"/>
+      <c r="K190" s="21"/>
+      <c r="L190" s="21"/>
+      <c r="M190" s="21"/>
+      <c r="N190" s="22"/>
       <c r="O190" s="2"/>
     </row>
     <row r="191" spans="2:15" x14ac:dyDescent="0.25">
@@ -5787,39 +5790,39 @@
       <c r="C191" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D191" s="17"/>
-      <c r="E191" s="17"/>
-      <c r="F191" s="17"/>
-      <c r="G191" s="18"/>
+      <c r="D191" s="21"/>
+      <c r="E191" s="21"/>
+      <c r="F191" s="21"/>
+      <c r="G191" s="22"/>
       <c r="H191" s="14"/>
       <c r="I191" s="7"/>
       <c r="J191" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K191" s="17"/>
-      <c r="L191" s="17"/>
-      <c r="M191" s="17"/>
-      <c r="N191" s="18"/>
+      <c r="K191" s="21"/>
+      <c r="L191" s="21"/>
+      <c r="M191" s="21"/>
+      <c r="N191" s="22"/>
       <c r="O191" s="2"/>
     </row>
     <row r="192" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B192" s="7"/>
-      <c r="C192" s="16" t="s">
+      <c r="C192" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D192" s="17"/>
-      <c r="E192" s="17"/>
-      <c r="F192" s="17"/>
-      <c r="G192" s="18"/>
+      <c r="D192" s="21"/>
+      <c r="E192" s="21"/>
+      <c r="F192" s="21"/>
+      <c r="G192" s="22"/>
       <c r="H192" s="14"/>
       <c r="I192" s="7"/>
-      <c r="J192" s="16" t="s">
+      <c r="J192" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K192" s="17"/>
-      <c r="L192" s="17"/>
-      <c r="M192" s="17"/>
-      <c r="N192" s="18"/>
+      <c r="K192" s="21"/>
+      <c r="L192" s="21"/>
+      <c r="M192" s="21"/>
+      <c r="N192" s="22"/>
       <c r="O192" s="2"/>
     </row>
     <row r="193" spans="2:15" x14ac:dyDescent="0.25">
@@ -5919,20 +5922,20 @@
       <c r="O197" s="2"/>
     </row>
     <row r="198" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B198" s="19" t="s">
+      <c r="B198" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C198" s="20"/>
-      <c r="D198" s="20"/>
+      <c r="C198" s="18"/>
+      <c r="D198" s="18"/>
       <c r="E198" s="14"/>
       <c r="F198" s="4"/>
       <c r="G198" s="15"/>
       <c r="H198" s="14"/>
-      <c r="I198" s="19" t="s">
+      <c r="I198" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J198" s="20"/>
-      <c r="K198" s="20"/>
+      <c r="J198" s="18"/>
+      <c r="K198" s="18"/>
       <c r="L198" s="14"/>
       <c r="M198" s="4"/>
       <c r="N198" s="15"/>
@@ -5974,103 +5977,103 @@
       <c r="O201" s="2"/>
     </row>
     <row r="202" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B202" s="25"/>
-      <c r="C202" s="21" t="s">
+      <c r="B202" s="26"/>
+      <c r="C202" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D202" s="20"/>
-      <c r="E202" s="20"/>
-      <c r="F202" s="20"/>
-      <c r="G202" s="22"/>
+      <c r="D202" s="18"/>
+      <c r="E202" s="18"/>
+      <c r="F202" s="18"/>
+      <c r="G202" s="19"/>
       <c r="H202" s="14"/>
       <c r="I202" s="6"/>
-      <c r="J202" s="21" t="s">
+      <c r="J202" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K202" s="20"/>
-      <c r="L202" s="20"/>
-      <c r="M202" s="20"/>
-      <c r="N202" s="22"/>
+      <c r="K202" s="18"/>
+      <c r="L202" s="18"/>
+      <c r="M202" s="18"/>
+      <c r="N202" s="19"/>
       <c r="O202" s="2"/>
     </row>
     <row r="203" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B203" s="26"/>
-      <c r="C203" s="23" t="s">
+      <c r="B203" s="27"/>
+      <c r="C203" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D203" s="17"/>
-      <c r="E203" s="17"/>
-      <c r="F203" s="17"/>
-      <c r="G203" s="18"/>
+      <c r="D203" s="21"/>
+      <c r="E203" s="21"/>
+      <c r="F203" s="21"/>
+      <c r="G203" s="22"/>
       <c r="H203" s="14"/>
       <c r="I203" s="7"/>
-      <c r="J203" s="23" t="s">
+      <c r="J203" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K203" s="17"/>
-      <c r="L203" s="17"/>
-      <c r="M203" s="17"/>
-      <c r="N203" s="18"/>
+      <c r="K203" s="21"/>
+      <c r="L203" s="21"/>
+      <c r="M203" s="21"/>
+      <c r="N203" s="22"/>
       <c r="O203" s="2"/>
     </row>
     <row r="204" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B204" s="26"/>
-      <c r="C204" s="23" t="s">
+      <c r="B204" s="27"/>
+      <c r="C204" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D204" s="17"/>
-      <c r="E204" s="17"/>
-      <c r="F204" s="17"/>
-      <c r="G204" s="18"/>
+      <c r="D204" s="21"/>
+      <c r="E204" s="21"/>
+      <c r="F204" s="21"/>
+      <c r="G204" s="22"/>
       <c r="H204" s="14"/>
       <c r="I204" s="7"/>
-      <c r="J204" s="23" t="s">
+      <c r="J204" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K204" s="17"/>
-      <c r="L204" s="17"/>
-      <c r="M204" s="17"/>
-      <c r="N204" s="18"/>
+      <c r="K204" s="21"/>
+      <c r="L204" s="21"/>
+      <c r="M204" s="21"/>
+      <c r="N204" s="22"/>
       <c r="O204" s="2"/>
     </row>
     <row r="205" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B205" s="26"/>
+      <c r="B205" s="27"/>
       <c r="C205" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D205" s="17"/>
-      <c r="E205" s="17"/>
-      <c r="F205" s="17"/>
-      <c r="G205" s="18"/>
+      <c r="D205" s="21"/>
+      <c r="E205" s="21"/>
+      <c r="F205" s="21"/>
+      <c r="G205" s="22"/>
       <c r="H205" s="14"/>
       <c r="I205" s="7"/>
       <c r="J205" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K205" s="17"/>
-      <c r="L205" s="17"/>
-      <c r="M205" s="17"/>
-      <c r="N205" s="18"/>
+      <c r="K205" s="21"/>
+      <c r="L205" s="21"/>
+      <c r="M205" s="21"/>
+      <c r="N205" s="22"/>
       <c r="O205" s="2"/>
     </row>
     <row r="206" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B206" s="26"/>
-      <c r="C206" s="16" t="s">
+      <c r="B206" s="27"/>
+      <c r="C206" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D206" s="17"/>
-      <c r="E206" s="17"/>
-      <c r="F206" s="17"/>
-      <c r="G206" s="18"/>
+      <c r="D206" s="21"/>
+      <c r="E206" s="21"/>
+      <c r="F206" s="21"/>
+      <c r="G206" s="22"/>
       <c r="H206" s="14"/>
       <c r="I206" s="7"/>
-      <c r="J206" s="16" t="s">
+      <c r="J206" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K206" s="17"/>
-      <c r="L206" s="17"/>
-      <c r="M206" s="17"/>
-      <c r="N206" s="18"/>
+      <c r="K206" s="21"/>
+      <c r="L206" s="21"/>
+      <c r="M206" s="21"/>
+      <c r="N206" s="22"/>
       <c r="O206" s="2"/>
     </row>
     <row r="207" spans="2:15" x14ac:dyDescent="0.25">
@@ -6170,20 +6173,20 @@
       <c r="O211" s="2"/>
     </row>
     <row r="212" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B212" s="19" t="s">
+      <c r="B212" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C212" s="20"/>
-      <c r="D212" s="20"/>
+      <c r="C212" s="18"/>
+      <c r="D212" s="18"/>
       <c r="E212" s="14"/>
       <c r="F212" s="4"/>
       <c r="G212" s="15"/>
       <c r="H212" s="14"/>
-      <c r="I212" s="19" t="s">
+      <c r="I212" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J212" s="20"/>
-      <c r="K212" s="20"/>
+      <c r="J212" s="18"/>
+      <c r="K212" s="18"/>
       <c r="L212" s="14"/>
       <c r="M212" s="4"/>
       <c r="N212" s="15"/>
@@ -6239,62 +6242,62 @@
     </row>
     <row r="216" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B216" s="6"/>
-      <c r="C216" s="21" t="s">
+      <c r="C216" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D216" s="20"/>
-      <c r="E216" s="20"/>
-      <c r="F216" s="20"/>
-      <c r="G216" s="22"/>
+      <c r="D216" s="18"/>
+      <c r="E216" s="18"/>
+      <c r="F216" s="18"/>
+      <c r="G216" s="19"/>
       <c r="H216" s="14"/>
       <c r="I216" s="6"/>
-      <c r="J216" s="21" t="s">
+      <c r="J216" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K216" s="20"/>
-      <c r="L216" s="20"/>
-      <c r="M216" s="20"/>
-      <c r="N216" s="22"/>
+      <c r="K216" s="18"/>
+      <c r="L216" s="18"/>
+      <c r="M216" s="18"/>
+      <c r="N216" s="19"/>
       <c r="O216" s="2"/>
     </row>
     <row r="217" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B217" s="7"/>
-      <c r="C217" s="23" t="s">
+      <c r="C217" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D217" s="17"/>
-      <c r="E217" s="17"/>
-      <c r="F217" s="17"/>
-      <c r="G217" s="18"/>
+      <c r="D217" s="21"/>
+      <c r="E217" s="21"/>
+      <c r="F217" s="21"/>
+      <c r="G217" s="22"/>
       <c r="H217" s="14"/>
       <c r="I217" s="7"/>
-      <c r="J217" s="23" t="s">
+      <c r="J217" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K217" s="17"/>
-      <c r="L217" s="17"/>
-      <c r="M217" s="17"/>
-      <c r="N217" s="18"/>
+      <c r="K217" s="21"/>
+      <c r="L217" s="21"/>
+      <c r="M217" s="21"/>
+      <c r="N217" s="22"/>
       <c r="O217" s="2"/>
     </row>
     <row r="218" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B218" s="7"/>
-      <c r="C218" s="23" t="s">
+      <c r="C218" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D218" s="17"/>
-      <c r="E218" s="17"/>
-      <c r="F218" s="17"/>
-      <c r="G218" s="18"/>
+      <c r="D218" s="21"/>
+      <c r="E218" s="21"/>
+      <c r="F218" s="21"/>
+      <c r="G218" s="22"/>
       <c r="H218" s="14"/>
       <c r="I218" s="7"/>
-      <c r="J218" s="23" t="s">
+      <c r="J218" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K218" s="17"/>
-      <c r="L218" s="17"/>
-      <c r="M218" s="17"/>
-      <c r="N218" s="18"/>
+      <c r="K218" s="21"/>
+      <c r="L218" s="21"/>
+      <c r="M218" s="21"/>
+      <c r="N218" s="22"/>
       <c r="O218" s="2"/>
     </row>
     <row r="219" spans="2:15" x14ac:dyDescent="0.25">
@@ -6302,39 +6305,39 @@
       <c r="C219" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D219" s="17"/>
-      <c r="E219" s="17"/>
-      <c r="F219" s="17"/>
-      <c r="G219" s="18"/>
+      <c r="D219" s="21"/>
+      <c r="E219" s="21"/>
+      <c r="F219" s="21"/>
+      <c r="G219" s="22"/>
       <c r="H219" s="14"/>
       <c r="I219" s="7"/>
       <c r="J219" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K219" s="17"/>
-      <c r="L219" s="17"/>
-      <c r="M219" s="17"/>
-      <c r="N219" s="18"/>
+      <c r="K219" s="21"/>
+      <c r="L219" s="21"/>
+      <c r="M219" s="21"/>
+      <c r="N219" s="22"/>
       <c r="O219" s="2"/>
     </row>
     <row r="220" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B220" s="7"/>
-      <c r="C220" s="16" t="s">
+      <c r="C220" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D220" s="17"/>
-      <c r="E220" s="17"/>
-      <c r="F220" s="17"/>
-      <c r="G220" s="18"/>
+      <c r="D220" s="21"/>
+      <c r="E220" s="21"/>
+      <c r="F220" s="21"/>
+      <c r="G220" s="22"/>
       <c r="H220" s="14"/>
       <c r="I220" s="7"/>
-      <c r="J220" s="16" t="s">
+      <c r="J220" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K220" s="17"/>
-      <c r="L220" s="17"/>
-      <c r="M220" s="17"/>
-      <c r="N220" s="18"/>
+      <c r="K220" s="21"/>
+      <c r="L220" s="21"/>
+      <c r="M220" s="21"/>
+      <c r="N220" s="22"/>
       <c r="O220" s="2"/>
     </row>
     <row r="221" spans="2:15" x14ac:dyDescent="0.25">
@@ -6434,20 +6437,20 @@
       <c r="O225" s="2"/>
     </row>
     <row r="226" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B226" s="19" t="s">
+      <c r="B226" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C226" s="20"/>
-      <c r="D226" s="20"/>
+      <c r="C226" s="18"/>
+      <c r="D226" s="18"/>
       <c r="E226" s="14"/>
       <c r="F226" s="4"/>
       <c r="G226" s="15"/>
       <c r="H226" s="14"/>
-      <c r="I226" s="19" t="s">
+      <c r="I226" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J226" s="20"/>
-      <c r="K226" s="20"/>
+      <c r="J226" s="18"/>
+      <c r="K226" s="18"/>
       <c r="L226" s="14"/>
       <c r="M226" s="4"/>
       <c r="N226" s="15"/>
@@ -6489,103 +6492,103 @@
       <c r="O229" s="2"/>
     </row>
     <row r="230" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B230" s="25"/>
-      <c r="C230" s="21" t="s">
+      <c r="B230" s="26"/>
+      <c r="C230" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D230" s="20"/>
-      <c r="E230" s="20"/>
-      <c r="F230" s="20"/>
-      <c r="G230" s="22"/>
+      <c r="D230" s="18"/>
+      <c r="E230" s="18"/>
+      <c r="F230" s="18"/>
+      <c r="G230" s="19"/>
       <c r="H230" s="14"/>
       <c r="I230" s="6"/>
-      <c r="J230" s="21" t="s">
+      <c r="J230" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K230" s="20"/>
-      <c r="L230" s="20"/>
-      <c r="M230" s="20"/>
-      <c r="N230" s="22"/>
+      <c r="K230" s="18"/>
+      <c r="L230" s="18"/>
+      <c r="M230" s="18"/>
+      <c r="N230" s="19"/>
       <c r="O230" s="2"/>
     </row>
     <row r="231" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B231" s="26"/>
-      <c r="C231" s="23" t="s">
+      <c r="B231" s="27"/>
+      <c r="C231" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D231" s="17"/>
-      <c r="E231" s="17"/>
-      <c r="F231" s="17"/>
-      <c r="G231" s="18"/>
+      <c r="D231" s="21"/>
+      <c r="E231" s="21"/>
+      <c r="F231" s="21"/>
+      <c r="G231" s="22"/>
       <c r="H231" s="14"/>
       <c r="I231" s="7"/>
-      <c r="J231" s="23" t="s">
+      <c r="J231" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K231" s="17"/>
-      <c r="L231" s="17"/>
-      <c r="M231" s="17"/>
-      <c r="N231" s="18"/>
+      <c r="K231" s="21"/>
+      <c r="L231" s="21"/>
+      <c r="M231" s="21"/>
+      <c r="N231" s="22"/>
       <c r="O231" s="2"/>
     </row>
     <row r="232" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B232" s="26"/>
-      <c r="C232" s="23" t="s">
+      <c r="B232" s="27"/>
+      <c r="C232" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D232" s="17"/>
-      <c r="E232" s="17"/>
-      <c r="F232" s="17"/>
-      <c r="G232" s="18"/>
+      <c r="D232" s="21"/>
+      <c r="E232" s="21"/>
+      <c r="F232" s="21"/>
+      <c r="G232" s="22"/>
       <c r="H232" s="14"/>
       <c r="I232" s="7"/>
-      <c r="J232" s="23" t="s">
+      <c r="J232" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K232" s="17"/>
-      <c r="L232" s="17"/>
-      <c r="M232" s="17"/>
-      <c r="N232" s="18"/>
+      <c r="K232" s="21"/>
+      <c r="L232" s="21"/>
+      <c r="M232" s="21"/>
+      <c r="N232" s="22"/>
       <c r="O232" s="2"/>
     </row>
     <row r="233" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B233" s="26"/>
+      <c r="B233" s="27"/>
       <c r="C233" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D233" s="17"/>
-      <c r="E233" s="17"/>
-      <c r="F233" s="17"/>
-      <c r="G233" s="18"/>
+      <c r="D233" s="21"/>
+      <c r="E233" s="21"/>
+      <c r="F233" s="21"/>
+      <c r="G233" s="22"/>
       <c r="H233" s="14"/>
       <c r="I233" s="7"/>
       <c r="J233" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K233" s="17"/>
-      <c r="L233" s="17"/>
-      <c r="M233" s="17"/>
-      <c r="N233" s="18"/>
+      <c r="K233" s="21"/>
+      <c r="L233" s="21"/>
+      <c r="M233" s="21"/>
+      <c r="N233" s="22"/>
       <c r="O233" s="2"/>
     </row>
     <row r="234" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B234" s="26"/>
-      <c r="C234" s="16" t="s">
+      <c r="B234" s="27"/>
+      <c r="C234" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D234" s="17"/>
-      <c r="E234" s="17"/>
-      <c r="F234" s="17"/>
-      <c r="G234" s="18"/>
+      <c r="D234" s="21"/>
+      <c r="E234" s="21"/>
+      <c r="F234" s="21"/>
+      <c r="G234" s="22"/>
       <c r="H234" s="14"/>
       <c r="I234" s="7"/>
-      <c r="J234" s="16" t="s">
+      <c r="J234" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K234" s="17"/>
-      <c r="L234" s="17"/>
-      <c r="M234" s="17"/>
-      <c r="N234" s="18"/>
+      <c r="K234" s="21"/>
+      <c r="L234" s="21"/>
+      <c r="M234" s="21"/>
+      <c r="N234" s="22"/>
       <c r="O234" s="2"/>
     </row>
     <row r="235" spans="2:15" x14ac:dyDescent="0.25">
@@ -6685,20 +6688,20 @@
       <c r="O239" s="2"/>
     </row>
     <row r="240" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B240" s="19" t="s">
+      <c r="B240" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C240" s="20"/>
-      <c r="D240" s="20"/>
+      <c r="C240" s="18"/>
+      <c r="D240" s="18"/>
       <c r="E240" s="14"/>
       <c r="F240" s="4"/>
       <c r="G240" s="15"/>
       <c r="H240" s="14"/>
-      <c r="I240" s="19" t="s">
+      <c r="I240" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J240" s="20"/>
-      <c r="K240" s="20"/>
+      <c r="J240" s="18"/>
+      <c r="K240" s="18"/>
       <c r="L240" s="14"/>
       <c r="M240" s="4"/>
       <c r="N240" s="15"/>
@@ -6754,62 +6757,62 @@
     </row>
     <row r="244" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B244" s="6"/>
-      <c r="C244" s="21" t="s">
+      <c r="C244" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D244" s="20"/>
-      <c r="E244" s="20"/>
-      <c r="F244" s="20"/>
-      <c r="G244" s="22"/>
+      <c r="D244" s="18"/>
+      <c r="E244" s="18"/>
+      <c r="F244" s="18"/>
+      <c r="G244" s="19"/>
       <c r="H244" s="14"/>
       <c r="I244" s="6"/>
-      <c r="J244" s="21" t="s">
+      <c r="J244" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K244" s="20"/>
-      <c r="L244" s="20"/>
-      <c r="M244" s="20"/>
-      <c r="N244" s="22"/>
+      <c r="K244" s="18"/>
+      <c r="L244" s="18"/>
+      <c r="M244" s="18"/>
+      <c r="N244" s="19"/>
       <c r="O244" s="2"/>
     </row>
     <row r="245" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B245" s="7"/>
-      <c r="C245" s="23" t="s">
+      <c r="C245" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D245" s="17"/>
-      <c r="E245" s="17"/>
-      <c r="F245" s="17"/>
-      <c r="G245" s="18"/>
+      <c r="D245" s="21"/>
+      <c r="E245" s="21"/>
+      <c r="F245" s="21"/>
+      <c r="G245" s="22"/>
       <c r="H245" s="14"/>
       <c r="I245" s="7"/>
-      <c r="J245" s="23" t="s">
+      <c r="J245" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K245" s="17"/>
-      <c r="L245" s="17"/>
-      <c r="M245" s="17"/>
-      <c r="N245" s="18"/>
+      <c r="K245" s="21"/>
+      <c r="L245" s="21"/>
+      <c r="M245" s="21"/>
+      <c r="N245" s="22"/>
       <c r="O245" s="2"/>
     </row>
     <row r="246" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B246" s="7"/>
-      <c r="C246" s="23" t="s">
+      <c r="C246" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D246" s="17"/>
-      <c r="E246" s="17"/>
-      <c r="F246" s="17"/>
-      <c r="G246" s="18"/>
+      <c r="D246" s="21"/>
+      <c r="E246" s="21"/>
+      <c r="F246" s="21"/>
+      <c r="G246" s="22"/>
       <c r="H246" s="14"/>
       <c r="I246" s="7"/>
-      <c r="J246" s="23" t="s">
+      <c r="J246" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K246" s="17"/>
-      <c r="L246" s="17"/>
-      <c r="M246" s="17"/>
-      <c r="N246" s="18"/>
+      <c r="K246" s="21"/>
+      <c r="L246" s="21"/>
+      <c r="M246" s="21"/>
+      <c r="N246" s="22"/>
       <c r="O246" s="2"/>
     </row>
     <row r="247" spans="2:15" x14ac:dyDescent="0.25">
@@ -6817,39 +6820,39 @@
       <c r="C247" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D247" s="17"/>
-      <c r="E247" s="17"/>
-      <c r="F247" s="17"/>
-      <c r="G247" s="18"/>
+      <c r="D247" s="21"/>
+      <c r="E247" s="21"/>
+      <c r="F247" s="21"/>
+      <c r="G247" s="22"/>
       <c r="H247" s="14"/>
       <c r="I247" s="7"/>
       <c r="J247" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K247" s="17"/>
-      <c r="L247" s="17"/>
-      <c r="M247" s="17"/>
-      <c r="N247" s="18"/>
+      <c r="K247" s="21"/>
+      <c r="L247" s="21"/>
+      <c r="M247" s="21"/>
+      <c r="N247" s="22"/>
       <c r="O247" s="2"/>
     </row>
     <row r="248" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B248" s="7"/>
-      <c r="C248" s="16" t="s">
+      <c r="C248" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D248" s="17"/>
-      <c r="E248" s="17"/>
-      <c r="F248" s="17"/>
-      <c r="G248" s="18"/>
+      <c r="D248" s="21"/>
+      <c r="E248" s="21"/>
+      <c r="F248" s="21"/>
+      <c r="G248" s="22"/>
       <c r="H248" s="14"/>
       <c r="I248" s="7"/>
-      <c r="J248" s="16" t="s">
+      <c r="J248" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K248" s="17"/>
-      <c r="L248" s="17"/>
-      <c r="M248" s="17"/>
-      <c r="N248" s="18"/>
+      <c r="K248" s="21"/>
+      <c r="L248" s="21"/>
+      <c r="M248" s="21"/>
+      <c r="N248" s="22"/>
       <c r="O248" s="2"/>
     </row>
     <row r="249" spans="2:15" x14ac:dyDescent="0.25">
@@ -6949,20 +6952,20 @@
       <c r="O253" s="2"/>
     </row>
     <row r="254" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B254" s="19" t="s">
+      <c r="B254" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C254" s="20"/>
-      <c r="D254" s="20"/>
+      <c r="C254" s="18"/>
+      <c r="D254" s="18"/>
       <c r="E254" s="14"/>
       <c r="F254" s="4"/>
       <c r="G254" s="15"/>
       <c r="H254" s="14"/>
-      <c r="I254" s="19" t="s">
+      <c r="I254" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J254" s="20"/>
-      <c r="K254" s="20"/>
+      <c r="J254" s="18"/>
+      <c r="K254" s="18"/>
       <c r="L254" s="14"/>
       <c r="M254" s="4"/>
       <c r="N254" s="15"/>
@@ -7004,103 +7007,103 @@
       <c r="O257" s="2"/>
     </row>
     <row r="258" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B258" s="25"/>
-      <c r="C258" s="21" t="s">
+      <c r="B258" s="26"/>
+      <c r="C258" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D258" s="20"/>
-      <c r="E258" s="20"/>
-      <c r="F258" s="20"/>
-      <c r="G258" s="22"/>
+      <c r="D258" s="18"/>
+      <c r="E258" s="18"/>
+      <c r="F258" s="18"/>
+      <c r="G258" s="19"/>
       <c r="H258" s="14"/>
       <c r="I258" s="6"/>
-      <c r="J258" s="21" t="s">
+      <c r="J258" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K258" s="20"/>
-      <c r="L258" s="20"/>
-      <c r="M258" s="20"/>
-      <c r="N258" s="22"/>
+      <c r="K258" s="18"/>
+      <c r="L258" s="18"/>
+      <c r="M258" s="18"/>
+      <c r="N258" s="19"/>
       <c r="O258" s="2"/>
     </row>
     <row r="259" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B259" s="26"/>
-      <c r="C259" s="23" t="s">
+      <c r="B259" s="27"/>
+      <c r="C259" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D259" s="17"/>
-      <c r="E259" s="17"/>
-      <c r="F259" s="17"/>
-      <c r="G259" s="18"/>
+      <c r="D259" s="21"/>
+      <c r="E259" s="21"/>
+      <c r="F259" s="21"/>
+      <c r="G259" s="22"/>
       <c r="H259" s="14"/>
       <c r="I259" s="7"/>
-      <c r="J259" s="23" t="s">
+      <c r="J259" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K259" s="17"/>
-      <c r="L259" s="17"/>
-      <c r="M259" s="17"/>
-      <c r="N259" s="18"/>
+      <c r="K259" s="21"/>
+      <c r="L259" s="21"/>
+      <c r="M259" s="21"/>
+      <c r="N259" s="22"/>
       <c r="O259" s="2"/>
     </row>
     <row r="260" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B260" s="26"/>
-      <c r="C260" s="23" t="s">
+      <c r="B260" s="27"/>
+      <c r="C260" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D260" s="17"/>
-      <c r="E260" s="17"/>
-      <c r="F260" s="17"/>
-      <c r="G260" s="18"/>
+      <c r="D260" s="21"/>
+      <c r="E260" s="21"/>
+      <c r="F260" s="21"/>
+      <c r="G260" s="22"/>
       <c r="H260" s="14"/>
       <c r="I260" s="7"/>
-      <c r="J260" s="23" t="s">
+      <c r="J260" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K260" s="17"/>
-      <c r="L260" s="17"/>
-      <c r="M260" s="17"/>
-      <c r="N260" s="18"/>
+      <c r="K260" s="21"/>
+      <c r="L260" s="21"/>
+      <c r="M260" s="21"/>
+      <c r="N260" s="22"/>
       <c r="O260" s="2"/>
     </row>
     <row r="261" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B261" s="26"/>
+      <c r="B261" s="27"/>
       <c r="C261" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D261" s="17"/>
-      <c r="E261" s="17"/>
-      <c r="F261" s="17"/>
-      <c r="G261" s="18"/>
+      <c r="D261" s="21"/>
+      <c r="E261" s="21"/>
+      <c r="F261" s="21"/>
+      <c r="G261" s="22"/>
       <c r="H261" s="14"/>
       <c r="I261" s="7"/>
       <c r="J261" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K261" s="17"/>
-      <c r="L261" s="17"/>
-      <c r="M261" s="17"/>
-      <c r="N261" s="18"/>
+      <c r="K261" s="21"/>
+      <c r="L261" s="21"/>
+      <c r="M261" s="21"/>
+      <c r="N261" s="22"/>
       <c r="O261" s="2"/>
     </row>
     <row r="262" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B262" s="26"/>
-      <c r="C262" s="16" t="s">
+      <c r="B262" s="27"/>
+      <c r="C262" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D262" s="17"/>
-      <c r="E262" s="17"/>
-      <c r="F262" s="17"/>
-      <c r="G262" s="18"/>
+      <c r="D262" s="21"/>
+      <c r="E262" s="21"/>
+      <c r="F262" s="21"/>
+      <c r="G262" s="22"/>
       <c r="H262" s="14"/>
       <c r="I262" s="7"/>
-      <c r="J262" s="16" t="s">
+      <c r="J262" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K262" s="17"/>
-      <c r="L262" s="17"/>
-      <c r="M262" s="17"/>
-      <c r="N262" s="18"/>
+      <c r="K262" s="21"/>
+      <c r="L262" s="21"/>
+      <c r="M262" s="21"/>
+      <c r="N262" s="22"/>
       <c r="O262" s="2"/>
     </row>
     <row r="263" spans="2:15" x14ac:dyDescent="0.25">
@@ -7200,20 +7203,20 @@
       <c r="O267" s="2"/>
     </row>
     <row r="268" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B268" s="19" t="s">
+      <c r="B268" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C268" s="20"/>
-      <c r="D268" s="20"/>
+      <c r="C268" s="18"/>
+      <c r="D268" s="18"/>
       <c r="E268" s="14"/>
       <c r="F268" s="4"/>
       <c r="G268" s="15"/>
       <c r="H268" s="14"/>
-      <c r="I268" s="19" t="s">
+      <c r="I268" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J268" s="20"/>
-      <c r="K268" s="20"/>
+      <c r="J268" s="18"/>
+      <c r="K268" s="18"/>
       <c r="L268" s="14"/>
       <c r="M268" s="4"/>
       <c r="N268" s="15"/>
@@ -7269,62 +7272,62 @@
     </row>
     <row r="272" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B272" s="6"/>
-      <c r="C272" s="21" t="s">
+      <c r="C272" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D272" s="20"/>
-      <c r="E272" s="20"/>
-      <c r="F272" s="20"/>
-      <c r="G272" s="22"/>
+      <c r="D272" s="18"/>
+      <c r="E272" s="18"/>
+      <c r="F272" s="18"/>
+      <c r="G272" s="19"/>
       <c r="H272" s="14"/>
       <c r="I272" s="6"/>
-      <c r="J272" s="21" t="s">
+      <c r="J272" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K272" s="20"/>
-      <c r="L272" s="20"/>
-      <c r="M272" s="20"/>
-      <c r="N272" s="22"/>
+      <c r="K272" s="18"/>
+      <c r="L272" s="18"/>
+      <c r="M272" s="18"/>
+      <c r="N272" s="19"/>
       <c r="O272" s="2"/>
     </row>
     <row r="273" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B273" s="7"/>
-      <c r="C273" s="23" t="s">
+      <c r="C273" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D273" s="17"/>
-      <c r="E273" s="17"/>
-      <c r="F273" s="17"/>
-      <c r="G273" s="18"/>
+      <c r="D273" s="21"/>
+      <c r="E273" s="21"/>
+      <c r="F273" s="21"/>
+      <c r="G273" s="22"/>
       <c r="H273" s="14"/>
       <c r="I273" s="7"/>
-      <c r="J273" s="23" t="s">
+      <c r="J273" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K273" s="17"/>
-      <c r="L273" s="17"/>
-      <c r="M273" s="17"/>
-      <c r="N273" s="18"/>
+      <c r="K273" s="21"/>
+      <c r="L273" s="21"/>
+      <c r="M273" s="21"/>
+      <c r="N273" s="22"/>
       <c r="O273" s="2"/>
     </row>
     <row r="274" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B274" s="7"/>
-      <c r="C274" s="23" t="s">
+      <c r="C274" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D274" s="17"/>
-      <c r="E274" s="17"/>
-      <c r="F274" s="17"/>
-      <c r="G274" s="18"/>
+      <c r="D274" s="21"/>
+      <c r="E274" s="21"/>
+      <c r="F274" s="21"/>
+      <c r="G274" s="22"/>
       <c r="H274" s="14"/>
       <c r="I274" s="7"/>
-      <c r="J274" s="23" t="s">
+      <c r="J274" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K274" s="17"/>
-      <c r="L274" s="17"/>
-      <c r="M274" s="17"/>
-      <c r="N274" s="18"/>
+      <c r="K274" s="21"/>
+      <c r="L274" s="21"/>
+      <c r="M274" s="21"/>
+      <c r="N274" s="22"/>
       <c r="O274" s="2"/>
     </row>
     <row r="275" spans="2:15" x14ac:dyDescent="0.25">
@@ -7332,39 +7335,39 @@
       <c r="C275" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D275" s="17"/>
-      <c r="E275" s="17"/>
-      <c r="F275" s="17"/>
-      <c r="G275" s="18"/>
+      <c r="D275" s="21"/>
+      <c r="E275" s="21"/>
+      <c r="F275" s="21"/>
+      <c r="G275" s="22"/>
       <c r="H275" s="14"/>
       <c r="I275" s="7"/>
       <c r="J275" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K275" s="17"/>
-      <c r="L275" s="17"/>
-      <c r="M275" s="17"/>
-      <c r="N275" s="18"/>
+      <c r="K275" s="21"/>
+      <c r="L275" s="21"/>
+      <c r="M275" s="21"/>
+      <c r="N275" s="22"/>
       <c r="O275" s="2"/>
     </row>
     <row r="276" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B276" s="7"/>
-      <c r="C276" s="16" t="s">
+      <c r="C276" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D276" s="17"/>
-      <c r="E276" s="17"/>
-      <c r="F276" s="17"/>
-      <c r="G276" s="18"/>
+      <c r="D276" s="21"/>
+      <c r="E276" s="21"/>
+      <c r="F276" s="21"/>
+      <c r="G276" s="22"/>
       <c r="H276" s="14"/>
       <c r="I276" s="7"/>
-      <c r="J276" s="16" t="s">
+      <c r="J276" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K276" s="17"/>
-      <c r="L276" s="17"/>
-      <c r="M276" s="17"/>
-      <c r="N276" s="18"/>
+      <c r="K276" s="21"/>
+      <c r="L276" s="21"/>
+      <c r="M276" s="21"/>
+      <c r="N276" s="22"/>
       <c r="O276" s="2"/>
     </row>
     <row r="277" spans="2:15" x14ac:dyDescent="0.25">
@@ -7464,20 +7467,20 @@
       <c r="O281" s="2"/>
     </row>
     <row r="282" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B282" s="19" t="s">
+      <c r="B282" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C282" s="20"/>
-      <c r="D282" s="20"/>
+      <c r="C282" s="18"/>
+      <c r="D282" s="18"/>
       <c r="E282" s="14"/>
       <c r="F282" s="4"/>
       <c r="G282" s="15"/>
       <c r="H282" s="14"/>
-      <c r="I282" s="19" t="s">
+      <c r="I282" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J282" s="20"/>
-      <c r="K282" s="20"/>
+      <c r="J282" s="18"/>
+      <c r="K282" s="18"/>
       <c r="L282" s="14"/>
       <c r="M282" s="4"/>
       <c r="N282" s="15"/>
@@ -7516,6 +7519,232 @@
     </row>
   </sheetData>
   <mergeCells count="250">
+    <mergeCell ref="C276:G276"/>
+    <mergeCell ref="J276:N276"/>
+    <mergeCell ref="B282:D282"/>
+    <mergeCell ref="I282:K282"/>
+    <mergeCell ref="B268:D268"/>
+    <mergeCell ref="I268:K268"/>
+    <mergeCell ref="C272:G272"/>
+    <mergeCell ref="J272:N272"/>
+    <mergeCell ref="C273:G273"/>
+    <mergeCell ref="J273:N273"/>
+    <mergeCell ref="C274:G274"/>
+    <mergeCell ref="J274:N274"/>
+    <mergeCell ref="C275:G275"/>
+    <mergeCell ref="J275:N275"/>
+    <mergeCell ref="C248:G248"/>
+    <mergeCell ref="J248:N248"/>
+    <mergeCell ref="B254:D254"/>
+    <mergeCell ref="I254:K254"/>
+    <mergeCell ref="B258:B262"/>
+    <mergeCell ref="C258:G258"/>
+    <mergeCell ref="J258:N258"/>
+    <mergeCell ref="C259:G259"/>
+    <mergeCell ref="J259:N259"/>
+    <mergeCell ref="C260:G260"/>
+    <mergeCell ref="J260:N260"/>
+    <mergeCell ref="C261:G261"/>
+    <mergeCell ref="J261:N261"/>
+    <mergeCell ref="C262:G262"/>
+    <mergeCell ref="J262:N262"/>
+    <mergeCell ref="B240:D240"/>
+    <mergeCell ref="I240:K240"/>
+    <mergeCell ref="C244:G244"/>
+    <mergeCell ref="J244:N244"/>
+    <mergeCell ref="C245:G245"/>
+    <mergeCell ref="J245:N245"/>
+    <mergeCell ref="C246:G246"/>
+    <mergeCell ref="J246:N246"/>
+    <mergeCell ref="C247:G247"/>
+    <mergeCell ref="J247:N247"/>
+    <mergeCell ref="B230:B234"/>
+    <mergeCell ref="C230:G230"/>
+    <mergeCell ref="J230:N230"/>
+    <mergeCell ref="C231:G231"/>
+    <mergeCell ref="J231:N231"/>
+    <mergeCell ref="C232:G232"/>
+    <mergeCell ref="J232:N232"/>
+    <mergeCell ref="C233:G233"/>
+    <mergeCell ref="J233:N233"/>
+    <mergeCell ref="C234:G234"/>
+    <mergeCell ref="J234:N234"/>
+    <mergeCell ref="C217:G217"/>
+    <mergeCell ref="J217:N217"/>
+    <mergeCell ref="C218:G218"/>
+    <mergeCell ref="J218:N218"/>
+    <mergeCell ref="C219:G219"/>
+    <mergeCell ref="J219:N219"/>
+    <mergeCell ref="C220:G220"/>
+    <mergeCell ref="J220:N220"/>
+    <mergeCell ref="B226:D226"/>
+    <mergeCell ref="I226:K226"/>
+    <mergeCell ref="B202:B206"/>
+    <mergeCell ref="J202:N202"/>
+    <mergeCell ref="J203:N203"/>
+    <mergeCell ref="J204:N204"/>
+    <mergeCell ref="J205:N205"/>
+    <mergeCell ref="J206:N206"/>
+    <mergeCell ref="B212:D212"/>
+    <mergeCell ref="I212:K212"/>
+    <mergeCell ref="C216:G216"/>
+    <mergeCell ref="J216:N216"/>
+    <mergeCell ref="C204:G204"/>
+    <mergeCell ref="C206:G206"/>
+    <mergeCell ref="C205:G205"/>
+    <mergeCell ref="C202:G202"/>
+    <mergeCell ref="C203:G203"/>
+    <mergeCell ref="B184:D184"/>
+    <mergeCell ref="I184:K184"/>
+    <mergeCell ref="C188:G188"/>
+    <mergeCell ref="J188:N188"/>
+    <mergeCell ref="C189:G189"/>
+    <mergeCell ref="C191:G191"/>
+    <mergeCell ref="C192:G192"/>
+    <mergeCell ref="J192:N192"/>
+    <mergeCell ref="B198:D198"/>
+    <mergeCell ref="I198:K198"/>
+    <mergeCell ref="C190:G190"/>
+    <mergeCell ref="J189:N189"/>
+    <mergeCell ref="C164:G164"/>
+    <mergeCell ref="J164:N164"/>
+    <mergeCell ref="B170:D170"/>
+    <mergeCell ref="I170:K170"/>
+    <mergeCell ref="B174:B178"/>
+    <mergeCell ref="C175:G175"/>
+    <mergeCell ref="C176:G176"/>
+    <mergeCell ref="C177:G177"/>
+    <mergeCell ref="C178:G178"/>
+    <mergeCell ref="J178:N178"/>
+    <mergeCell ref="B156:D156"/>
+    <mergeCell ref="I156:K156"/>
+    <mergeCell ref="C160:G160"/>
+    <mergeCell ref="J160:N160"/>
+    <mergeCell ref="C161:G161"/>
+    <mergeCell ref="J161:N161"/>
+    <mergeCell ref="C162:G162"/>
+    <mergeCell ref="J162:N162"/>
+    <mergeCell ref="C163:G163"/>
+    <mergeCell ref="J163:N163"/>
+    <mergeCell ref="B142:D142"/>
+    <mergeCell ref="I142:K142"/>
+    <mergeCell ref="B146:B150"/>
+    <mergeCell ref="C146:G146"/>
+    <mergeCell ref="J146:N146"/>
+    <mergeCell ref="C147:G147"/>
+    <mergeCell ref="J147:N147"/>
+    <mergeCell ref="C148:G148"/>
+    <mergeCell ref="J148:N148"/>
+    <mergeCell ref="C149:G149"/>
+    <mergeCell ref="J149:N149"/>
+    <mergeCell ref="C150:G150"/>
+    <mergeCell ref="J150:N150"/>
+    <mergeCell ref="C132:G132"/>
+    <mergeCell ref="J132:N132"/>
+    <mergeCell ref="C133:G133"/>
+    <mergeCell ref="J133:N133"/>
+    <mergeCell ref="C134:G134"/>
+    <mergeCell ref="J134:N134"/>
+    <mergeCell ref="C135:G135"/>
+    <mergeCell ref="J135:N135"/>
+    <mergeCell ref="C136:G136"/>
+    <mergeCell ref="J136:N136"/>
+    <mergeCell ref="B118:B122"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="J118:N118"/>
+    <mergeCell ref="C119:G119"/>
+    <mergeCell ref="J119:N119"/>
+    <mergeCell ref="J120:N120"/>
+    <mergeCell ref="C121:G121"/>
+    <mergeCell ref="B128:D128"/>
+    <mergeCell ref="I128:K128"/>
+    <mergeCell ref="B100:D100"/>
+    <mergeCell ref="I100:K100"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="J104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="J105:N105"/>
+    <mergeCell ref="J106:N106"/>
+    <mergeCell ref="J108:N108"/>
+    <mergeCell ref="B114:D114"/>
+    <mergeCell ref="I114:K114"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="I86:K86"/>
+    <mergeCell ref="B90:B94"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="J90:N90"/>
+    <mergeCell ref="J91:N91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="J92:N92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="J93:N93"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="J94:N94"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="I72:K72"/>
+    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="J78:N78"/>
+    <mergeCell ref="C79:G79"/>
+    <mergeCell ref="J79:N79"/>
+    <mergeCell ref="C80:G80"/>
+    <mergeCell ref="J80:N80"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="J191:N191"/>
+    <mergeCell ref="J176:N176"/>
+    <mergeCell ref="J177:N177"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="J52:N52"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="J107:N107"/>
+    <mergeCell ref="J122:N122"/>
+    <mergeCell ref="C122:G122"/>
+    <mergeCell ref="J175:N175"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C107:G107"/>
+    <mergeCell ref="J190:N190"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="J48:N48"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="J49:N49"/>
+    <mergeCell ref="J62:N62"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="C65:G65"/>
+    <mergeCell ref="J65:N65"/>
+    <mergeCell ref="C66:G66"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="J50:N50"/>
+    <mergeCell ref="C51:G51"/>
+    <mergeCell ref="J51:N51"/>
+    <mergeCell ref="J66:N66"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="J34:N34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="J35:N35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="J36:N36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="J37:N37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="J38:N38"/>
+    <mergeCell ref="C62:G62"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="J63:N63"/>
+    <mergeCell ref="C64:G64"/>
+    <mergeCell ref="J64:N64"/>
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="J7:N7"/>
     <mergeCell ref="C22:G22"/>
@@ -7540,232 +7769,6 @@
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="J121:N121"/>
     <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C62:G62"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="C63:G63"/>
-    <mergeCell ref="J63:N63"/>
-    <mergeCell ref="C64:G64"/>
-    <mergeCell ref="J64:N64"/>
-    <mergeCell ref="C65:G65"/>
-    <mergeCell ref="J65:N65"/>
-    <mergeCell ref="C66:G66"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="J50:N50"/>
-    <mergeCell ref="C51:G51"/>
-    <mergeCell ref="J51:N51"/>
-    <mergeCell ref="J66:N66"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="J191:N191"/>
-    <mergeCell ref="J176:N176"/>
-    <mergeCell ref="J177:N177"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="J52:N52"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="I58:K58"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="J107:N107"/>
-    <mergeCell ref="J122:N122"/>
-    <mergeCell ref="C122:G122"/>
-    <mergeCell ref="J175:N175"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C107:G107"/>
-    <mergeCell ref="J190:N190"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="J48:N48"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="J49:N49"/>
-    <mergeCell ref="J62:N62"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="J34:N34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="J35:N35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="J36:N36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="J37:N37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="J38:N38"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="I72:K72"/>
-    <mergeCell ref="C77:G77"/>
-    <mergeCell ref="C78:G78"/>
-    <mergeCell ref="J78:N78"/>
-    <mergeCell ref="C79:G79"/>
-    <mergeCell ref="J79:N79"/>
-    <mergeCell ref="C80:G80"/>
-    <mergeCell ref="J80:N80"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="I86:K86"/>
-    <mergeCell ref="B90:B94"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="J90:N90"/>
-    <mergeCell ref="J91:N91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="J92:N92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="J93:N93"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="J94:N94"/>
-    <mergeCell ref="B100:D100"/>
-    <mergeCell ref="I100:K100"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="J104:N104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="J105:N105"/>
-    <mergeCell ref="J106:N106"/>
-    <mergeCell ref="J108:N108"/>
-    <mergeCell ref="B114:D114"/>
-    <mergeCell ref="I114:K114"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="B118:B122"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="J118:N118"/>
-    <mergeCell ref="C119:G119"/>
-    <mergeCell ref="J119:N119"/>
-    <mergeCell ref="J120:N120"/>
-    <mergeCell ref="C121:G121"/>
-    <mergeCell ref="B128:D128"/>
-    <mergeCell ref="I128:K128"/>
-    <mergeCell ref="C132:G132"/>
-    <mergeCell ref="J132:N132"/>
-    <mergeCell ref="C133:G133"/>
-    <mergeCell ref="J133:N133"/>
-    <mergeCell ref="C134:G134"/>
-    <mergeCell ref="J134:N134"/>
-    <mergeCell ref="C135:G135"/>
-    <mergeCell ref="J135:N135"/>
-    <mergeCell ref="C136:G136"/>
-    <mergeCell ref="J136:N136"/>
-    <mergeCell ref="B142:D142"/>
-    <mergeCell ref="I142:K142"/>
-    <mergeCell ref="B146:B150"/>
-    <mergeCell ref="C146:G146"/>
-    <mergeCell ref="J146:N146"/>
-    <mergeCell ref="C147:G147"/>
-    <mergeCell ref="J147:N147"/>
-    <mergeCell ref="C148:G148"/>
-    <mergeCell ref="J148:N148"/>
-    <mergeCell ref="C149:G149"/>
-    <mergeCell ref="J149:N149"/>
-    <mergeCell ref="C150:G150"/>
-    <mergeCell ref="J150:N150"/>
-    <mergeCell ref="B156:D156"/>
-    <mergeCell ref="I156:K156"/>
-    <mergeCell ref="C160:G160"/>
-    <mergeCell ref="J160:N160"/>
-    <mergeCell ref="C161:G161"/>
-    <mergeCell ref="J161:N161"/>
-    <mergeCell ref="C162:G162"/>
-    <mergeCell ref="J162:N162"/>
-    <mergeCell ref="C163:G163"/>
-    <mergeCell ref="J163:N163"/>
-    <mergeCell ref="C164:G164"/>
-    <mergeCell ref="J164:N164"/>
-    <mergeCell ref="B170:D170"/>
-    <mergeCell ref="I170:K170"/>
-    <mergeCell ref="B174:B178"/>
-    <mergeCell ref="C175:G175"/>
-    <mergeCell ref="C176:G176"/>
-    <mergeCell ref="C177:G177"/>
-    <mergeCell ref="C178:G178"/>
-    <mergeCell ref="J178:N178"/>
-    <mergeCell ref="B184:D184"/>
-    <mergeCell ref="I184:K184"/>
-    <mergeCell ref="C188:G188"/>
-    <mergeCell ref="J188:N188"/>
-    <mergeCell ref="C189:G189"/>
-    <mergeCell ref="C191:G191"/>
-    <mergeCell ref="C192:G192"/>
-    <mergeCell ref="J192:N192"/>
-    <mergeCell ref="B198:D198"/>
-    <mergeCell ref="I198:K198"/>
-    <mergeCell ref="C190:G190"/>
-    <mergeCell ref="J189:N189"/>
-    <mergeCell ref="B202:B206"/>
-    <mergeCell ref="J202:N202"/>
-    <mergeCell ref="J203:N203"/>
-    <mergeCell ref="J204:N204"/>
-    <mergeCell ref="J205:N205"/>
-    <mergeCell ref="J206:N206"/>
-    <mergeCell ref="B212:D212"/>
-    <mergeCell ref="I212:K212"/>
-    <mergeCell ref="C216:G216"/>
-    <mergeCell ref="J216:N216"/>
-    <mergeCell ref="C204:G204"/>
-    <mergeCell ref="C206:G206"/>
-    <mergeCell ref="C205:G205"/>
-    <mergeCell ref="C202:G202"/>
-    <mergeCell ref="C203:G203"/>
-    <mergeCell ref="C217:G217"/>
-    <mergeCell ref="J217:N217"/>
-    <mergeCell ref="C218:G218"/>
-    <mergeCell ref="J218:N218"/>
-    <mergeCell ref="C219:G219"/>
-    <mergeCell ref="J219:N219"/>
-    <mergeCell ref="C220:G220"/>
-    <mergeCell ref="J220:N220"/>
-    <mergeCell ref="B226:D226"/>
-    <mergeCell ref="I226:K226"/>
-    <mergeCell ref="B230:B234"/>
-    <mergeCell ref="C230:G230"/>
-    <mergeCell ref="J230:N230"/>
-    <mergeCell ref="C231:G231"/>
-    <mergeCell ref="J231:N231"/>
-    <mergeCell ref="C232:G232"/>
-    <mergeCell ref="J232:N232"/>
-    <mergeCell ref="C233:G233"/>
-    <mergeCell ref="J233:N233"/>
-    <mergeCell ref="C234:G234"/>
-    <mergeCell ref="J234:N234"/>
-    <mergeCell ref="B240:D240"/>
-    <mergeCell ref="I240:K240"/>
-    <mergeCell ref="C244:G244"/>
-    <mergeCell ref="J244:N244"/>
-    <mergeCell ref="C245:G245"/>
-    <mergeCell ref="J245:N245"/>
-    <mergeCell ref="C246:G246"/>
-    <mergeCell ref="J246:N246"/>
-    <mergeCell ref="C247:G247"/>
-    <mergeCell ref="J247:N247"/>
-    <mergeCell ref="C248:G248"/>
-    <mergeCell ref="J248:N248"/>
-    <mergeCell ref="B254:D254"/>
-    <mergeCell ref="I254:K254"/>
-    <mergeCell ref="B258:B262"/>
-    <mergeCell ref="C258:G258"/>
-    <mergeCell ref="J258:N258"/>
-    <mergeCell ref="C259:G259"/>
-    <mergeCell ref="J259:N259"/>
-    <mergeCell ref="C260:G260"/>
-    <mergeCell ref="J260:N260"/>
-    <mergeCell ref="C261:G261"/>
-    <mergeCell ref="J261:N261"/>
-    <mergeCell ref="C262:G262"/>
-    <mergeCell ref="J262:N262"/>
-    <mergeCell ref="C276:G276"/>
-    <mergeCell ref="J276:N276"/>
-    <mergeCell ref="B282:D282"/>
-    <mergeCell ref="I282:K282"/>
-    <mergeCell ref="B268:D268"/>
-    <mergeCell ref="I268:K268"/>
-    <mergeCell ref="C272:G272"/>
-    <mergeCell ref="J272:N272"/>
-    <mergeCell ref="C273:G273"/>
-    <mergeCell ref="J273:N273"/>
-    <mergeCell ref="C274:G274"/>
-    <mergeCell ref="J274:N274"/>
-    <mergeCell ref="C275:G275"/>
-    <mergeCell ref="J275:N275"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
:fire: REMOVENDO ARQUIVOS INUTÉIS
</commit_message>
<xml_diff>
--- a/ModeloCarteirinha.xlsx
+++ b/ModeloCarteirinha.xlsx
@@ -53,7 +53,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +74,20 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -213,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -234,25 +248,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -260,6 +273,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2449,7 +2464,7 @@
   <dimension ref="A5:O284"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2473,98 +2488,98 @@
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
-      <c r="C6" s="17" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="22"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="19"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="22"/>
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="27"/>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="22"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="18"/>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="27"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="22"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="18"/>
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="27"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
       <c r="I9" s="7"/>
       <c r="J9" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="22"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="18"/>
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="27"/>
-      <c r="C10" s="25" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="22"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="18"/>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2606,16 +2621,17 @@
       <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="28"/>
       <c r="D14"/>
+      <c r="E14" s="28"/>
       <c r="F14" s="3"/>
       <c r="G14" s="8"/>
       <c r="I14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J14" s="16"/>
+      <c r="J14" s="28"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="L14" s="27"/>
       <c r="M14" s="3"/>
       <c r="N14" s="8"/>
       <c r="O14" s="2"/>
@@ -2632,18 +2648,18 @@
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
       <c r="F16" s="4"/>
       <c r="G16" s="8"/>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
       <c r="L16" s="2"/>
       <c r="M16" s="4"/>
       <c r="N16" s="8"/>
@@ -2680,59 +2696,59 @@
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="22"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="17" t="s">
+      <c r="J20" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="19"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="22"/>
       <c r="O20" s="2"/>
     </row>
     <row r="21" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="20" t="s">
+      <c r="J21" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="22"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="18"/>
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="18"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="22"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="18"/>
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
@@ -2740,37 +2756,37 @@
       <c r="C23" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18"/>
       <c r="I23" s="7"/>
       <c r="J23" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="22"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="18"/>
       <c r="O23" s="2"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="22"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="18"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="25" t="s">
+      <c r="J24" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="22"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="18"/>
       <c r="O24" s="2"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -2840,18 +2856,18 @@
       <c r="O29" s="2"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
       <c r="F30" s="4"/>
       <c r="G30" s="8"/>
-      <c r="I30" s="23" t="s">
+      <c r="I30" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
       <c r="L30" s="2"/>
       <c r="M30" s="4"/>
       <c r="N30" s="8"/>
@@ -2887,103 +2903,103 @@
       <c r="O33" s="2"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="26"/>
-      <c r="C34" s="17" t="s">
+      <c r="B34" s="25"/>
+      <c r="C34" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="22"/>
       <c r="H34" s="14"/>
       <c r="I34" s="6"/>
-      <c r="J34" s="17" t="s">
+      <c r="J34" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="19"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="22"/>
       <c r="O34" s="2"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="27"/>
-      <c r="C35" s="20" t="s">
+      <c r="B35" s="26"/>
+      <c r="C35" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="22"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="18"/>
       <c r="H35" s="14"/>
       <c r="I35" s="7"/>
-      <c r="J35" s="20" t="s">
+      <c r="J35" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="22"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="18"/>
       <c r="O35" s="2"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="27"/>
-      <c r="C36" s="20" t="s">
+      <c r="B36" s="26"/>
+      <c r="C36" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="22"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="18"/>
       <c r="H36" s="14"/>
       <c r="I36" s="7"/>
-      <c r="J36" s="20" t="s">
+      <c r="J36" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="21"/>
-      <c r="N36" s="22"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="18"/>
       <c r="O36" s="2"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="27"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="22"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="18"/>
       <c r="H37" s="14"/>
       <c r="I37" s="7"/>
       <c r="J37" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="21"/>
-      <c r="N37" s="22"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="18"/>
       <c r="O37" s="2"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="27"/>
-      <c r="C38" s="25" t="s">
+      <c r="B38" s="26"/>
+      <c r="C38" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="22"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="18"/>
       <c r="H38" s="14"/>
       <c r="I38" s="7"/>
-      <c r="J38" s="25" t="s">
+      <c r="J38" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K38" s="21"/>
-      <c r="L38" s="21"/>
-      <c r="M38" s="21"/>
-      <c r="N38" s="22"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="18"/>
       <c r="O38" s="2"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
@@ -3083,20 +3099,20 @@
       <c r="O43" s="2"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
       <c r="E44" s="14"/>
       <c r="F44" s="4"/>
       <c r="G44" s="15"/>
       <c r="H44" s="14"/>
-      <c r="I44" s="23" t="s">
+      <c r="I44" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
       <c r="L44" s="14"/>
       <c r="M44" s="4"/>
       <c r="N44" s="15"/>
@@ -3152,62 +3168,62 @@
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="19"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="22"/>
       <c r="H48" s="14"/>
       <c r="I48" s="6"/>
-      <c r="J48" s="17" t="s">
+      <c r="J48" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="19"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="22"/>
       <c r="O48" s="2"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="20" t="s">
+      <c r="C49" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="22"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="18"/>
       <c r="H49" s="14"/>
       <c r="I49" s="7"/>
-      <c r="J49" s="20" t="s">
+      <c r="J49" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K49" s="21"/>
-      <c r="L49" s="21"/>
-      <c r="M49" s="21"/>
-      <c r="N49" s="22"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="18"/>
       <c r="O49" s="2"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="20" t="s">
+      <c r="C50" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="22"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="18"/>
       <c r="H50" s="14"/>
       <c r="I50" s="7"/>
-      <c r="J50" s="20" t="s">
+      <c r="J50" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K50" s="21"/>
-      <c r="L50" s="21"/>
-      <c r="M50" s="21"/>
-      <c r="N50" s="22"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="18"/>
       <c r="O50" s="2"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
@@ -3215,39 +3231,39 @@
       <c r="C51" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="22"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="18"/>
       <c r="H51" s="14"/>
       <c r="I51" s="7"/>
       <c r="J51" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K51" s="21"/>
-      <c r="L51" s="21"/>
-      <c r="M51" s="21"/>
-      <c r="N51" s="22"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="18"/>
       <c r="O51" s="2"/>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
-      <c r="C52" s="25" t="s">
+      <c r="C52" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="22"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="18"/>
       <c r="H52" s="14"/>
       <c r="I52" s="7"/>
-      <c r="J52" s="25" t="s">
+      <c r="J52" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K52" s="21"/>
-      <c r="L52" s="21"/>
-      <c r="M52" s="21"/>
-      <c r="N52" s="22"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="17"/>
+      <c r="N52" s="18"/>
       <c r="O52" s="2"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
@@ -3347,20 +3363,20 @@
       <c r="O57" s="2"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="23" t="s">
+      <c r="B58" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
       <c r="E58" s="14"/>
       <c r="F58" s="4"/>
       <c r="G58" s="15"/>
       <c r="H58" s="14"/>
-      <c r="I58" s="23" t="s">
+      <c r="I58" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J58" s="18"/>
-      <c r="K58" s="18"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="20"/>
       <c r="L58" s="14"/>
       <c r="M58" s="4"/>
       <c r="N58" s="15"/>
@@ -3402,103 +3418,103 @@
       <c r="O61" s="2"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="26"/>
-      <c r="C62" s="17" t="s">
+      <c r="B62" s="25"/>
+      <c r="C62" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="19"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="22"/>
       <c r="H62" s="14"/>
       <c r="I62" s="6"/>
-      <c r="J62" s="17" t="s">
+      <c r="J62" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K62" s="18"/>
-      <c r="L62" s="18"/>
-      <c r="M62" s="18"/>
-      <c r="N62" s="19"/>
+      <c r="K62" s="20"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="22"/>
       <c r="O62" s="2"/>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="27"/>
-      <c r="C63" s="20" t="s">
+      <c r="B63" s="26"/>
+      <c r="C63" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D63" s="21"/>
-      <c r="E63" s="21"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="22"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="18"/>
       <c r="H63" s="14"/>
       <c r="I63" s="7"/>
-      <c r="J63" s="20" t="s">
+      <c r="J63" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K63" s="21"/>
-      <c r="L63" s="21"/>
-      <c r="M63" s="21"/>
-      <c r="N63" s="22"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="18"/>
       <c r="O63" s="2"/>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="27"/>
-      <c r="C64" s="20" t="s">
+      <c r="B64" s="26"/>
+      <c r="C64" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D64" s="21"/>
-      <c r="E64" s="21"/>
-      <c r="F64" s="21"/>
-      <c r="G64" s="22"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="18"/>
       <c r="H64" s="14"/>
       <c r="I64" s="7"/>
-      <c r="J64" s="20" t="s">
+      <c r="J64" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K64" s="21"/>
-      <c r="L64" s="21"/>
-      <c r="M64" s="21"/>
-      <c r="N64" s="22"/>
+      <c r="K64" s="17"/>
+      <c r="L64" s="17"/>
+      <c r="M64" s="17"/>
+      <c r="N64" s="18"/>
       <c r="O64" s="2"/>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="27"/>
+      <c r="B65" s="26"/>
       <c r="C65" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="21"/>
-      <c r="E65" s="21"/>
-      <c r="F65" s="21"/>
-      <c r="G65" s="22"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="18"/>
       <c r="H65" s="14"/>
       <c r="I65" s="7"/>
       <c r="J65" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K65" s="21"/>
-      <c r="L65" s="21"/>
-      <c r="M65" s="21"/>
-      <c r="N65" s="22"/>
+      <c r="K65" s="17"/>
+      <c r="L65" s="17"/>
+      <c r="M65" s="17"/>
+      <c r="N65" s="18"/>
       <c r="O65" s="2"/>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="27"/>
-      <c r="C66" s="25" t="s">
+      <c r="B66" s="26"/>
+      <c r="C66" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="21"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="22"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="18"/>
       <c r="H66" s="14"/>
       <c r="I66" s="7"/>
-      <c r="J66" s="25" t="s">
+      <c r="J66" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K66" s="21"/>
-      <c r="L66" s="21"/>
-      <c r="M66" s="21"/>
-      <c r="N66" s="22"/>
+      <c r="K66" s="17"/>
+      <c r="L66" s="17"/>
+      <c r="M66" s="17"/>
+      <c r="N66" s="18"/>
       <c r="O66" s="2"/>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
@@ -3598,20 +3614,20 @@
       <c r="O71" s="2"/>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="23" t="s">
+      <c r="B72" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="20"/>
       <c r="E72" s="14"/>
       <c r="F72" s="4"/>
       <c r="G72" s="15"/>
       <c r="H72" s="14"/>
-      <c r="I72" s="23" t="s">
+      <c r="I72" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J72" s="18"/>
-      <c r="K72" s="18"/>
+      <c r="J72" s="20"/>
+      <c r="K72" s="20"/>
       <c r="L72" s="14"/>
       <c r="M72" s="4"/>
       <c r="N72" s="15"/>
@@ -3667,62 +3683,62 @@
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
-      <c r="C76" s="17" t="s">
+      <c r="C76" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D76" s="18"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="19"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="22"/>
       <c r="H76" s="14"/>
       <c r="I76" s="6"/>
-      <c r="J76" s="17" t="s">
+      <c r="J76" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K76" s="18"/>
-      <c r="L76" s="18"/>
-      <c r="M76" s="18"/>
-      <c r="N76" s="19"/>
+      <c r="K76" s="20"/>
+      <c r="L76" s="20"/>
+      <c r="M76" s="20"/>
+      <c r="N76" s="22"/>
       <c r="O76" s="2"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B77" s="7"/>
-      <c r="C77" s="20" t="s">
+      <c r="C77" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D77" s="21"/>
-      <c r="E77" s="21"/>
-      <c r="F77" s="21"/>
-      <c r="G77" s="22"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="18"/>
       <c r="H77" s="14"/>
       <c r="I77" s="7"/>
-      <c r="J77" s="20" t="s">
+      <c r="J77" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K77" s="21"/>
-      <c r="L77" s="21"/>
-      <c r="M77" s="21"/>
-      <c r="N77" s="22"/>
+      <c r="K77" s="17"/>
+      <c r="L77" s="17"/>
+      <c r="M77" s="17"/>
+      <c r="N77" s="18"/>
       <c r="O77" s="2"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B78" s="7"/>
-      <c r="C78" s="20" t="s">
+      <c r="C78" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D78" s="21"/>
-      <c r="E78" s="21"/>
-      <c r="F78" s="21"/>
-      <c r="G78" s="22"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="18"/>
       <c r="H78" s="14"/>
       <c r="I78" s="7"/>
-      <c r="J78" s="20" t="s">
+      <c r="J78" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K78" s="21"/>
-      <c r="L78" s="21"/>
-      <c r="M78" s="21"/>
-      <c r="N78" s="22"/>
+      <c r="K78" s="17"/>
+      <c r="L78" s="17"/>
+      <c r="M78" s="17"/>
+      <c r="N78" s="18"/>
       <c r="O78" s="2"/>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
@@ -3730,39 +3746,39 @@
       <c r="C79" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D79" s="21"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="21"/>
-      <c r="G79" s="22"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="18"/>
       <c r="H79" s="14"/>
       <c r="I79" s="7"/>
       <c r="J79" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K79" s="21"/>
-      <c r="L79" s="21"/>
-      <c r="M79" s="21"/>
-      <c r="N79" s="22"/>
+      <c r="K79" s="17"/>
+      <c r="L79" s="17"/>
+      <c r="M79" s="17"/>
+      <c r="N79" s="18"/>
       <c r="O79" s="2"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B80" s="7"/>
-      <c r="C80" s="25" t="s">
+      <c r="C80" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D80" s="21"/>
-      <c r="E80" s="21"/>
-      <c r="F80" s="21"/>
-      <c r="G80" s="22"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="18"/>
       <c r="H80" s="14"/>
       <c r="I80" s="7"/>
-      <c r="J80" s="25" t="s">
+      <c r="J80" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K80" s="21"/>
-      <c r="L80" s="21"/>
-      <c r="M80" s="21"/>
-      <c r="N80" s="22"/>
+      <c r="K80" s="17"/>
+      <c r="L80" s="17"/>
+      <c r="M80" s="17"/>
+      <c r="N80" s="18"/>
       <c r="O80" s="2"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
@@ -3862,20 +3878,20 @@
       <c r="O85" s="2"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B86" s="23" t="s">
+      <c r="B86" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C86" s="18"/>
-      <c r="D86" s="18"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="20"/>
       <c r="E86" s="14"/>
       <c r="F86" s="4"/>
       <c r="G86" s="15"/>
       <c r="H86" s="14"/>
-      <c r="I86" s="23" t="s">
+      <c r="I86" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J86" s="18"/>
-      <c r="K86" s="18"/>
+      <c r="J86" s="20"/>
+      <c r="K86" s="20"/>
       <c r="L86" s="14"/>
       <c r="M86" s="4"/>
       <c r="N86" s="15"/>
@@ -3917,103 +3933,103 @@
       <c r="O89" s="2"/>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B90" s="26"/>
-      <c r="C90" s="17" t="s">
+      <c r="B90" s="25"/>
+      <c r="C90" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="18"/>
-      <c r="G90" s="19"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="20"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="22"/>
       <c r="H90" s="14"/>
       <c r="I90" s="6"/>
-      <c r="J90" s="17" t="s">
+      <c r="J90" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K90" s="18"/>
-      <c r="L90" s="18"/>
-      <c r="M90" s="18"/>
-      <c r="N90" s="19"/>
+      <c r="K90" s="20"/>
+      <c r="L90" s="20"/>
+      <c r="M90" s="20"/>
+      <c r="N90" s="22"/>
       <c r="O90" s="2"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B91" s="27"/>
-      <c r="C91" s="20" t="s">
+      <c r="B91" s="26"/>
+      <c r="C91" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D91" s="21"/>
-      <c r="E91" s="21"/>
-      <c r="F91" s="21"/>
-      <c r="G91" s="22"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="17"/>
+      <c r="F91" s="17"/>
+      <c r="G91" s="18"/>
       <c r="H91" s="14"/>
       <c r="I91" s="7"/>
-      <c r="J91" s="20" t="s">
+      <c r="J91" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K91" s="21"/>
-      <c r="L91" s="21"/>
-      <c r="M91" s="21"/>
-      <c r="N91" s="22"/>
+      <c r="K91" s="17"/>
+      <c r="L91" s="17"/>
+      <c r="M91" s="17"/>
+      <c r="N91" s="18"/>
       <c r="O91" s="2"/>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B92" s="27"/>
-      <c r="C92" s="20" t="s">
+      <c r="B92" s="26"/>
+      <c r="C92" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D92" s="21"/>
-      <c r="E92" s="21"/>
-      <c r="F92" s="21"/>
-      <c r="G92" s="22"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="18"/>
       <c r="H92" s="14"/>
       <c r="I92" s="7"/>
-      <c r="J92" s="20" t="s">
+      <c r="J92" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K92" s="21"/>
-      <c r="L92" s="21"/>
-      <c r="M92" s="21"/>
-      <c r="N92" s="22"/>
+      <c r="K92" s="17"/>
+      <c r="L92" s="17"/>
+      <c r="M92" s="17"/>
+      <c r="N92" s="18"/>
       <c r="O92" s="2"/>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B93" s="27"/>
+      <c r="B93" s="26"/>
       <c r="C93" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D93" s="21"/>
-      <c r="E93" s="21"/>
-      <c r="F93" s="21"/>
-      <c r="G93" s="22"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="17"/>
+      <c r="F93" s="17"/>
+      <c r="G93" s="18"/>
       <c r="H93" s="14"/>
       <c r="I93" s="7"/>
       <c r="J93" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K93" s="21"/>
-      <c r="L93" s="21"/>
-      <c r="M93" s="21"/>
-      <c r="N93" s="22"/>
+      <c r="K93" s="17"/>
+      <c r="L93" s="17"/>
+      <c r="M93" s="17"/>
+      <c r="N93" s="18"/>
       <c r="O93" s="2"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B94" s="27"/>
-      <c r="C94" s="25" t="s">
+      <c r="B94" s="26"/>
+      <c r="C94" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D94" s="21"/>
-      <c r="E94" s="21"/>
-      <c r="F94" s="21"/>
-      <c r="G94" s="22"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="17"/>
+      <c r="F94" s="17"/>
+      <c r="G94" s="18"/>
       <c r="H94" s="14"/>
       <c r="I94" s="7"/>
-      <c r="J94" s="25" t="s">
+      <c r="J94" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K94" s="21"/>
-      <c r="L94" s="21"/>
-      <c r="M94" s="21"/>
-      <c r="N94" s="22"/>
+      <c r="K94" s="17"/>
+      <c r="L94" s="17"/>
+      <c r="M94" s="17"/>
+      <c r="N94" s="18"/>
       <c r="O94" s="2"/>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
@@ -4113,20 +4129,20 @@
       <c r="O99" s="2"/>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B100" s="23" t="s">
+      <c r="B100" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C100" s="18"/>
-      <c r="D100" s="18"/>
+      <c r="C100" s="20"/>
+      <c r="D100" s="20"/>
       <c r="E100" s="14"/>
       <c r="F100" s="4"/>
       <c r="G100" s="15"/>
       <c r="H100" s="14"/>
-      <c r="I100" s="23" t="s">
+      <c r="I100" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J100" s="18"/>
-      <c r="K100" s="18"/>
+      <c r="J100" s="20"/>
+      <c r="K100" s="20"/>
       <c r="L100" s="14"/>
       <c r="M100" s="4"/>
       <c r="N100" s="15"/>
@@ -4182,62 +4198,62 @@
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104" s="6"/>
-      <c r="C104" s="17" t="s">
+      <c r="C104" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D104" s="18"/>
-      <c r="E104" s="18"/>
-      <c r="F104" s="18"/>
-      <c r="G104" s="19"/>
+      <c r="D104" s="20"/>
+      <c r="E104" s="20"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="22"/>
       <c r="H104" s="14"/>
       <c r="I104" s="6"/>
-      <c r="J104" s="17" t="s">
+      <c r="J104" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K104" s="18"/>
-      <c r="L104" s="18"/>
-      <c r="M104" s="18"/>
-      <c r="N104" s="19"/>
+      <c r="K104" s="20"/>
+      <c r="L104" s="20"/>
+      <c r="M104" s="20"/>
+      <c r="N104" s="22"/>
       <c r="O104" s="2"/>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B105" s="7"/>
-      <c r="C105" s="20" t="s">
+      <c r="C105" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D105" s="21"/>
-      <c r="E105" s="21"/>
-      <c r="F105" s="21"/>
-      <c r="G105" s="22"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="17"/>
+      <c r="F105" s="17"/>
+      <c r="G105" s="18"/>
       <c r="H105" s="14"/>
       <c r="I105" s="7"/>
-      <c r="J105" s="20" t="s">
+      <c r="J105" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K105" s="21"/>
-      <c r="L105" s="21"/>
-      <c r="M105" s="21"/>
-      <c r="N105" s="22"/>
+      <c r="K105" s="17"/>
+      <c r="L105" s="17"/>
+      <c r="M105" s="17"/>
+      <c r="N105" s="18"/>
       <c r="O105" s="2"/>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106" s="7"/>
-      <c r="C106" s="20" t="s">
+      <c r="C106" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D106" s="21"/>
-      <c r="E106" s="21"/>
-      <c r="F106" s="21"/>
-      <c r="G106" s="22"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="17"/>
+      <c r="G106" s="18"/>
       <c r="H106" s="14"/>
       <c r="I106" s="7"/>
-      <c r="J106" s="20" t="s">
+      <c r="J106" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K106" s="21"/>
-      <c r="L106" s="21"/>
-      <c r="M106" s="21"/>
-      <c r="N106" s="22"/>
+      <c r="K106" s="17"/>
+      <c r="L106" s="17"/>
+      <c r="M106" s="17"/>
+      <c r="N106" s="18"/>
       <c r="O106" s="2"/>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
@@ -4245,39 +4261,39 @@
       <c r="C107" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D107" s="21"/>
-      <c r="E107" s="21"/>
-      <c r="F107" s="21"/>
-      <c r="G107" s="22"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
+      <c r="F107" s="17"/>
+      <c r="G107" s="18"/>
       <c r="H107" s="14"/>
       <c r="I107" s="7"/>
       <c r="J107" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K107" s="21"/>
-      <c r="L107" s="21"/>
-      <c r="M107" s="21"/>
-      <c r="N107" s="22"/>
+      <c r="K107" s="17"/>
+      <c r="L107" s="17"/>
+      <c r="M107" s="17"/>
+      <c r="N107" s="18"/>
       <c r="O107" s="2"/>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B108" s="7"/>
-      <c r="C108" s="25" t="s">
+      <c r="C108" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D108" s="21"/>
-      <c r="E108" s="21"/>
-      <c r="F108" s="21"/>
-      <c r="G108" s="22"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="17"/>
+      <c r="F108" s="17"/>
+      <c r="G108" s="18"/>
       <c r="H108" s="14"/>
       <c r="I108" s="7"/>
-      <c r="J108" s="25" t="s">
+      <c r="J108" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K108" s="21"/>
-      <c r="L108" s="21"/>
-      <c r="M108" s="21"/>
-      <c r="N108" s="22"/>
+      <c r="K108" s="17"/>
+      <c r="L108" s="17"/>
+      <c r="M108" s="17"/>
+      <c r="N108" s="18"/>
       <c r="O108" s="2"/>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.25">
@@ -4377,20 +4393,20 @@
       <c r="O113" s="2"/>
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B114" s="23" t="s">
+      <c r="B114" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C114" s="18"/>
-      <c r="D114" s="18"/>
+      <c r="C114" s="20"/>
+      <c r="D114" s="20"/>
       <c r="E114" s="14"/>
       <c r="F114" s="4"/>
       <c r="G114" s="15"/>
       <c r="H114" s="14"/>
-      <c r="I114" s="23" t="s">
+      <c r="I114" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J114" s="18"/>
-      <c r="K114" s="18"/>
+      <c r="J114" s="20"/>
+      <c r="K114" s="20"/>
       <c r="L114" s="14"/>
       <c r="M114" s="4"/>
       <c r="N114" s="15"/>
@@ -4432,103 +4448,103 @@
       <c r="O117" s="2"/>
     </row>
     <row r="118" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B118" s="26"/>
-      <c r="C118" s="17" t="s">
+      <c r="B118" s="25"/>
+      <c r="C118" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D118" s="18"/>
-      <c r="E118" s="18"/>
-      <c r="F118" s="18"/>
-      <c r="G118" s="19"/>
+      <c r="D118" s="20"/>
+      <c r="E118" s="20"/>
+      <c r="F118" s="20"/>
+      <c r="G118" s="22"/>
       <c r="H118" s="14"/>
       <c r="I118" s="6"/>
-      <c r="J118" s="17" t="s">
+      <c r="J118" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K118" s="18"/>
-      <c r="L118" s="18"/>
-      <c r="M118" s="18"/>
-      <c r="N118" s="19"/>
+      <c r="K118" s="20"/>
+      <c r="L118" s="20"/>
+      <c r="M118" s="20"/>
+      <c r="N118" s="22"/>
       <c r="O118" s="2"/>
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B119" s="27"/>
-      <c r="C119" s="20" t="s">
+      <c r="B119" s="26"/>
+      <c r="C119" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D119" s="21"/>
-      <c r="E119" s="21"/>
-      <c r="F119" s="21"/>
-      <c r="G119" s="22"/>
+      <c r="D119" s="17"/>
+      <c r="E119" s="17"/>
+      <c r="F119" s="17"/>
+      <c r="G119" s="18"/>
       <c r="H119" s="14"/>
       <c r="I119" s="7"/>
-      <c r="J119" s="20" t="s">
+      <c r="J119" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K119" s="21"/>
-      <c r="L119" s="21"/>
-      <c r="M119" s="21"/>
-      <c r="N119" s="22"/>
+      <c r="K119" s="17"/>
+      <c r="L119" s="17"/>
+      <c r="M119" s="17"/>
+      <c r="N119" s="18"/>
       <c r="O119" s="2"/>
     </row>
     <row r="120" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B120" s="27"/>
-      <c r="C120" s="20" t="s">
+      <c r="B120" s="26"/>
+      <c r="C120" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D120" s="21"/>
-      <c r="E120" s="21"/>
-      <c r="F120" s="21"/>
-      <c r="G120" s="22"/>
+      <c r="D120" s="17"/>
+      <c r="E120" s="17"/>
+      <c r="F120" s="17"/>
+      <c r="G120" s="18"/>
       <c r="H120" s="14"/>
       <c r="I120" s="7"/>
-      <c r="J120" s="20" t="s">
+      <c r="J120" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K120" s="21"/>
-      <c r="L120" s="21"/>
-      <c r="M120" s="21"/>
-      <c r="N120" s="22"/>
+      <c r="K120" s="17"/>
+      <c r="L120" s="17"/>
+      <c r="M120" s="17"/>
+      <c r="N120" s="18"/>
       <c r="O120" s="2"/>
     </row>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B121" s="27"/>
+      <c r="B121" s="26"/>
       <c r="C121" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D121" s="21"/>
-      <c r="E121" s="21"/>
-      <c r="F121" s="21"/>
-      <c r="G121" s="22"/>
+      <c r="D121" s="17"/>
+      <c r="E121" s="17"/>
+      <c r="F121" s="17"/>
+      <c r="G121" s="18"/>
       <c r="H121" s="14"/>
       <c r="I121" s="7"/>
       <c r="J121" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K121" s="21"/>
-      <c r="L121" s="21"/>
-      <c r="M121" s="21"/>
-      <c r="N121" s="22"/>
+      <c r="K121" s="17"/>
+      <c r="L121" s="17"/>
+      <c r="M121" s="17"/>
+      <c r="N121" s="18"/>
       <c r="O121" s="2"/>
     </row>
     <row r="122" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B122" s="27"/>
-      <c r="C122" s="25" t="s">
+      <c r="B122" s="26"/>
+      <c r="C122" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D122" s="21"/>
-      <c r="E122" s="21"/>
-      <c r="F122" s="21"/>
-      <c r="G122" s="22"/>
+      <c r="D122" s="17"/>
+      <c r="E122" s="17"/>
+      <c r="F122" s="17"/>
+      <c r="G122" s="18"/>
       <c r="H122" s="14"/>
       <c r="I122" s="7"/>
-      <c r="J122" s="25" t="s">
+      <c r="J122" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K122" s="21"/>
-      <c r="L122" s="21"/>
-      <c r="M122" s="21"/>
-      <c r="N122" s="22"/>
+      <c r="K122" s="17"/>
+      <c r="L122" s="17"/>
+      <c r="M122" s="17"/>
+      <c r="N122" s="18"/>
       <c r="O122" s="2"/>
     </row>
     <row r="123" spans="2:15" x14ac:dyDescent="0.25">
@@ -4628,20 +4644,20 @@
       <c r="O127" s="2"/>
     </row>
     <row r="128" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B128" s="23" t="s">
+      <c r="B128" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C128" s="18"/>
-      <c r="D128" s="18"/>
+      <c r="C128" s="20"/>
+      <c r="D128" s="20"/>
       <c r="E128" s="14"/>
       <c r="F128" s="4"/>
       <c r="G128" s="15"/>
       <c r="H128" s="14"/>
-      <c r="I128" s="23" t="s">
+      <c r="I128" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J128" s="18"/>
-      <c r="K128" s="18"/>
+      <c r="J128" s="20"/>
+      <c r="K128" s="20"/>
       <c r="L128" s="14"/>
       <c r="M128" s="4"/>
       <c r="N128" s="15"/>
@@ -4697,62 +4713,62 @@
     </row>
     <row r="132" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
-      <c r="C132" s="17" t="s">
+      <c r="C132" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D132" s="18"/>
-      <c r="E132" s="18"/>
-      <c r="F132" s="18"/>
-      <c r="G132" s="19"/>
+      <c r="D132" s="20"/>
+      <c r="E132" s="20"/>
+      <c r="F132" s="20"/>
+      <c r="G132" s="22"/>
       <c r="H132" s="14"/>
       <c r="I132" s="6"/>
-      <c r="J132" s="17" t="s">
+      <c r="J132" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K132" s="18"/>
-      <c r="L132" s="18"/>
-      <c r="M132" s="18"/>
-      <c r="N132" s="19"/>
+      <c r="K132" s="20"/>
+      <c r="L132" s="20"/>
+      <c r="M132" s="20"/>
+      <c r="N132" s="22"/>
       <c r="O132" s="2"/>
     </row>
     <row r="133" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B133" s="7"/>
-      <c r="C133" s="20" t="s">
+      <c r="C133" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D133" s="21"/>
-      <c r="E133" s="21"/>
-      <c r="F133" s="21"/>
-      <c r="G133" s="22"/>
+      <c r="D133" s="17"/>
+      <c r="E133" s="17"/>
+      <c r="F133" s="17"/>
+      <c r="G133" s="18"/>
       <c r="H133" s="14"/>
       <c r="I133" s="7"/>
-      <c r="J133" s="20" t="s">
+      <c r="J133" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K133" s="21"/>
-      <c r="L133" s="21"/>
-      <c r="M133" s="21"/>
-      <c r="N133" s="22"/>
+      <c r="K133" s="17"/>
+      <c r="L133" s="17"/>
+      <c r="M133" s="17"/>
+      <c r="N133" s="18"/>
       <c r="O133" s="2"/>
     </row>
     <row r="134" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B134" s="7"/>
-      <c r="C134" s="20" t="s">
+      <c r="C134" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D134" s="21"/>
-      <c r="E134" s="21"/>
-      <c r="F134" s="21"/>
-      <c r="G134" s="22"/>
+      <c r="D134" s="17"/>
+      <c r="E134" s="17"/>
+      <c r="F134" s="17"/>
+      <c r="G134" s="18"/>
       <c r="H134" s="14"/>
       <c r="I134" s="7"/>
-      <c r="J134" s="20" t="s">
+      <c r="J134" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K134" s="21"/>
-      <c r="L134" s="21"/>
-      <c r="M134" s="21"/>
-      <c r="N134" s="22"/>
+      <c r="K134" s="17"/>
+      <c r="L134" s="17"/>
+      <c r="M134" s="17"/>
+      <c r="N134" s="18"/>
       <c r="O134" s="2"/>
     </row>
     <row r="135" spans="2:15" x14ac:dyDescent="0.25">
@@ -4760,39 +4776,39 @@
       <c r="C135" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D135" s="21"/>
-      <c r="E135" s="21"/>
-      <c r="F135" s="21"/>
-      <c r="G135" s="22"/>
+      <c r="D135" s="17"/>
+      <c r="E135" s="17"/>
+      <c r="F135" s="17"/>
+      <c r="G135" s="18"/>
       <c r="H135" s="14"/>
       <c r="I135" s="7"/>
       <c r="J135" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K135" s="21"/>
-      <c r="L135" s="21"/>
-      <c r="M135" s="21"/>
-      <c r="N135" s="22"/>
+      <c r="K135" s="17"/>
+      <c r="L135" s="17"/>
+      <c r="M135" s="17"/>
+      <c r="N135" s="18"/>
       <c r="O135" s="2"/>
     </row>
     <row r="136" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B136" s="7"/>
-      <c r="C136" s="25" t="s">
+      <c r="C136" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D136" s="21"/>
-      <c r="E136" s="21"/>
-      <c r="F136" s="21"/>
-      <c r="G136" s="22"/>
+      <c r="D136" s="17"/>
+      <c r="E136" s="17"/>
+      <c r="F136" s="17"/>
+      <c r="G136" s="18"/>
       <c r="H136" s="14"/>
       <c r="I136" s="7"/>
-      <c r="J136" s="25" t="s">
+      <c r="J136" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K136" s="21"/>
-      <c r="L136" s="21"/>
-      <c r="M136" s="21"/>
-      <c r="N136" s="22"/>
+      <c r="K136" s="17"/>
+      <c r="L136" s="17"/>
+      <c r="M136" s="17"/>
+      <c r="N136" s="18"/>
       <c r="O136" s="2"/>
     </row>
     <row r="137" spans="2:15" x14ac:dyDescent="0.25">
@@ -4892,20 +4908,20 @@
       <c r="O141" s="2"/>
     </row>
     <row r="142" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B142" s="23" t="s">
+      <c r="B142" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C142" s="18"/>
-      <c r="D142" s="18"/>
+      <c r="C142" s="20"/>
+      <c r="D142" s="20"/>
       <c r="E142" s="14"/>
       <c r="F142" s="4"/>
       <c r="G142" s="15"/>
       <c r="H142" s="14"/>
-      <c r="I142" s="23" t="s">
+      <c r="I142" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J142" s="18"/>
-      <c r="K142" s="18"/>
+      <c r="J142" s="20"/>
+      <c r="K142" s="20"/>
       <c r="L142" s="14"/>
       <c r="M142" s="4"/>
       <c r="N142" s="15"/>
@@ -4947,103 +4963,103 @@
       <c r="O145" s="2"/>
     </row>
     <row r="146" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B146" s="26"/>
-      <c r="C146" s="17" t="s">
+      <c r="B146" s="25"/>
+      <c r="C146" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D146" s="18"/>
-      <c r="E146" s="18"/>
-      <c r="F146" s="18"/>
-      <c r="G146" s="19"/>
+      <c r="D146" s="20"/>
+      <c r="E146" s="20"/>
+      <c r="F146" s="20"/>
+      <c r="G146" s="22"/>
       <c r="H146" s="14"/>
       <c r="I146" s="6"/>
-      <c r="J146" s="17" t="s">
+      <c r="J146" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K146" s="18"/>
-      <c r="L146" s="18"/>
-      <c r="M146" s="18"/>
-      <c r="N146" s="19"/>
+      <c r="K146" s="20"/>
+      <c r="L146" s="20"/>
+      <c r="M146" s="20"/>
+      <c r="N146" s="22"/>
       <c r="O146" s="2"/>
     </row>
     <row r="147" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B147" s="27"/>
-      <c r="C147" s="20" t="s">
+      <c r="B147" s="26"/>
+      <c r="C147" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D147" s="21"/>
-      <c r="E147" s="21"/>
-      <c r="F147" s="21"/>
-      <c r="G147" s="22"/>
+      <c r="D147" s="17"/>
+      <c r="E147" s="17"/>
+      <c r="F147" s="17"/>
+      <c r="G147" s="18"/>
       <c r="H147" s="14"/>
       <c r="I147" s="7"/>
-      <c r="J147" s="20" t="s">
+      <c r="J147" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K147" s="21"/>
-      <c r="L147" s="21"/>
-      <c r="M147" s="21"/>
-      <c r="N147" s="22"/>
+      <c r="K147" s="17"/>
+      <c r="L147" s="17"/>
+      <c r="M147" s="17"/>
+      <c r="N147" s="18"/>
       <c r="O147" s="2"/>
     </row>
     <row r="148" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B148" s="27"/>
-      <c r="C148" s="20" t="s">
+      <c r="B148" s="26"/>
+      <c r="C148" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D148" s="21"/>
-      <c r="E148" s="21"/>
-      <c r="F148" s="21"/>
-      <c r="G148" s="22"/>
+      <c r="D148" s="17"/>
+      <c r="E148" s="17"/>
+      <c r="F148" s="17"/>
+      <c r="G148" s="18"/>
       <c r="H148" s="14"/>
       <c r="I148" s="7"/>
-      <c r="J148" s="20" t="s">
+      <c r="J148" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K148" s="21"/>
-      <c r="L148" s="21"/>
-      <c r="M148" s="21"/>
-      <c r="N148" s="22"/>
+      <c r="K148" s="17"/>
+      <c r="L148" s="17"/>
+      <c r="M148" s="17"/>
+      <c r="N148" s="18"/>
       <c r="O148" s="2"/>
     </row>
     <row r="149" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B149" s="27"/>
+      <c r="B149" s="26"/>
       <c r="C149" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D149" s="21"/>
-      <c r="E149" s="21"/>
-      <c r="F149" s="21"/>
-      <c r="G149" s="22"/>
+      <c r="D149" s="17"/>
+      <c r="E149" s="17"/>
+      <c r="F149" s="17"/>
+      <c r="G149" s="18"/>
       <c r="H149" s="14"/>
       <c r="I149" s="7"/>
       <c r="J149" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K149" s="21"/>
-      <c r="L149" s="21"/>
-      <c r="M149" s="21"/>
-      <c r="N149" s="22"/>
+      <c r="K149" s="17"/>
+      <c r="L149" s="17"/>
+      <c r="M149" s="17"/>
+      <c r="N149" s="18"/>
       <c r="O149" s="2"/>
     </row>
     <row r="150" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B150" s="27"/>
-      <c r="C150" s="25" t="s">
+      <c r="B150" s="26"/>
+      <c r="C150" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D150" s="21"/>
-      <c r="E150" s="21"/>
-      <c r="F150" s="21"/>
-      <c r="G150" s="22"/>
+      <c r="D150" s="17"/>
+      <c r="E150" s="17"/>
+      <c r="F150" s="17"/>
+      <c r="G150" s="18"/>
       <c r="H150" s="14"/>
       <c r="I150" s="7"/>
-      <c r="J150" s="25" t="s">
+      <c r="J150" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K150" s="21"/>
-      <c r="L150" s="21"/>
-      <c r="M150" s="21"/>
-      <c r="N150" s="22"/>
+      <c r="K150" s="17"/>
+      <c r="L150" s="17"/>
+      <c r="M150" s="17"/>
+      <c r="N150" s="18"/>
       <c r="O150" s="2"/>
     </row>
     <row r="151" spans="2:15" x14ac:dyDescent="0.25">
@@ -5143,20 +5159,20 @@
       <c r="O155" s="2"/>
     </row>
     <row r="156" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B156" s="23" t="s">
+      <c r="B156" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C156" s="18"/>
-      <c r="D156" s="18"/>
+      <c r="C156" s="20"/>
+      <c r="D156" s="20"/>
       <c r="E156" s="14"/>
       <c r="F156" s="4"/>
       <c r="G156" s="15"/>
       <c r="H156" s="14"/>
-      <c r="I156" s="23" t="s">
+      <c r="I156" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J156" s="18"/>
-      <c r="K156" s="18"/>
+      <c r="J156" s="20"/>
+      <c r="K156" s="20"/>
       <c r="L156" s="14"/>
       <c r="M156" s="4"/>
       <c r="N156" s="15"/>
@@ -5212,62 +5228,62 @@
     </row>
     <row r="160" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
-      <c r="C160" s="17" t="s">
+      <c r="C160" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D160" s="18"/>
-      <c r="E160" s="18"/>
-      <c r="F160" s="18"/>
-      <c r="G160" s="19"/>
+      <c r="D160" s="20"/>
+      <c r="E160" s="20"/>
+      <c r="F160" s="20"/>
+      <c r="G160" s="22"/>
       <c r="H160" s="14"/>
       <c r="I160" s="6"/>
-      <c r="J160" s="17" t="s">
+      <c r="J160" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K160" s="18"/>
-      <c r="L160" s="18"/>
-      <c r="M160" s="18"/>
-      <c r="N160" s="19"/>
+      <c r="K160" s="20"/>
+      <c r="L160" s="20"/>
+      <c r="M160" s="20"/>
+      <c r="N160" s="22"/>
       <c r="O160" s="2"/>
     </row>
     <row r="161" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B161" s="7"/>
-      <c r="C161" s="20" t="s">
+      <c r="C161" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D161" s="21"/>
-      <c r="E161" s="21"/>
-      <c r="F161" s="21"/>
-      <c r="G161" s="22"/>
+      <c r="D161" s="17"/>
+      <c r="E161" s="17"/>
+      <c r="F161" s="17"/>
+      <c r="G161" s="18"/>
       <c r="H161" s="14"/>
       <c r="I161" s="7"/>
-      <c r="J161" s="20" t="s">
+      <c r="J161" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K161" s="21"/>
-      <c r="L161" s="21"/>
-      <c r="M161" s="21"/>
-      <c r="N161" s="22"/>
+      <c r="K161" s="17"/>
+      <c r="L161" s="17"/>
+      <c r="M161" s="17"/>
+      <c r="N161" s="18"/>
       <c r="O161" s="2"/>
     </row>
     <row r="162" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B162" s="7"/>
-      <c r="C162" s="20" t="s">
+      <c r="C162" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D162" s="21"/>
-      <c r="E162" s="21"/>
-      <c r="F162" s="21"/>
-      <c r="G162" s="22"/>
+      <c r="D162" s="17"/>
+      <c r="E162" s="17"/>
+      <c r="F162" s="17"/>
+      <c r="G162" s="18"/>
       <c r="H162" s="14"/>
       <c r="I162" s="7"/>
-      <c r="J162" s="20" t="s">
+      <c r="J162" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K162" s="21"/>
-      <c r="L162" s="21"/>
-      <c r="M162" s="21"/>
-      <c r="N162" s="22"/>
+      <c r="K162" s="17"/>
+      <c r="L162" s="17"/>
+      <c r="M162" s="17"/>
+      <c r="N162" s="18"/>
       <c r="O162" s="2"/>
     </row>
     <row r="163" spans="2:15" x14ac:dyDescent="0.25">
@@ -5275,39 +5291,39 @@
       <c r="C163" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D163" s="21"/>
-      <c r="E163" s="21"/>
-      <c r="F163" s="21"/>
-      <c r="G163" s="22"/>
+      <c r="D163" s="17"/>
+      <c r="E163" s="17"/>
+      <c r="F163" s="17"/>
+      <c r="G163" s="18"/>
       <c r="H163" s="14"/>
       <c r="I163" s="7"/>
       <c r="J163" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K163" s="21"/>
-      <c r="L163" s="21"/>
-      <c r="M163" s="21"/>
-      <c r="N163" s="22"/>
+      <c r="K163" s="17"/>
+      <c r="L163" s="17"/>
+      <c r="M163" s="17"/>
+      <c r="N163" s="18"/>
       <c r="O163" s="2"/>
     </row>
     <row r="164" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B164" s="7"/>
-      <c r="C164" s="25" t="s">
+      <c r="C164" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D164" s="21"/>
-      <c r="E164" s="21"/>
-      <c r="F164" s="21"/>
-      <c r="G164" s="22"/>
+      <c r="D164" s="17"/>
+      <c r="E164" s="17"/>
+      <c r="F164" s="17"/>
+      <c r="G164" s="18"/>
       <c r="H164" s="14"/>
       <c r="I164" s="7"/>
-      <c r="J164" s="25" t="s">
+      <c r="J164" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K164" s="21"/>
-      <c r="L164" s="21"/>
-      <c r="M164" s="21"/>
-      <c r="N164" s="22"/>
+      <c r="K164" s="17"/>
+      <c r="L164" s="17"/>
+      <c r="M164" s="17"/>
+      <c r="N164" s="18"/>
       <c r="O164" s="2"/>
     </row>
     <row r="165" spans="2:15" x14ac:dyDescent="0.25">
@@ -5407,20 +5423,20 @@
       <c r="O169" s="2"/>
     </row>
     <row r="170" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B170" s="23" t="s">
+      <c r="B170" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C170" s="18"/>
-      <c r="D170" s="18"/>
+      <c r="C170" s="20"/>
+      <c r="D170" s="20"/>
       <c r="E170" s="14"/>
       <c r="F170" s="4"/>
       <c r="G170" s="15"/>
       <c r="H170" s="14"/>
-      <c r="I170" s="23" t="s">
+      <c r="I170" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J170" s="18"/>
-      <c r="K170" s="18"/>
+      <c r="J170" s="20"/>
+      <c r="K170" s="20"/>
       <c r="L170" s="14"/>
       <c r="M170" s="4"/>
       <c r="N170" s="15"/>
@@ -5462,103 +5478,103 @@
       <c r="O173" s="2"/>
     </row>
     <row r="174" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B174" s="26"/>
-      <c r="C174" s="17" t="s">
+      <c r="B174" s="25"/>
+      <c r="C174" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D174" s="18"/>
-      <c r="E174" s="18"/>
-      <c r="F174" s="18"/>
-      <c r="G174" s="19"/>
+      <c r="D174" s="20"/>
+      <c r="E174" s="20"/>
+      <c r="F174" s="20"/>
+      <c r="G174" s="22"/>
       <c r="H174" s="14"/>
       <c r="I174" s="6"/>
-      <c r="J174" s="17" t="s">
+      <c r="J174" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K174" s="18"/>
-      <c r="L174" s="18"/>
-      <c r="M174" s="18"/>
-      <c r="N174" s="19"/>
+      <c r="K174" s="20"/>
+      <c r="L174" s="20"/>
+      <c r="M174" s="20"/>
+      <c r="N174" s="22"/>
       <c r="O174" s="2"/>
     </row>
     <row r="175" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B175" s="27"/>
-      <c r="C175" s="20" t="s">
+      <c r="B175" s="26"/>
+      <c r="C175" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D175" s="21"/>
-      <c r="E175" s="21"/>
-      <c r="F175" s="21"/>
-      <c r="G175" s="22"/>
+      <c r="D175" s="17"/>
+      <c r="E175" s="17"/>
+      <c r="F175" s="17"/>
+      <c r="G175" s="18"/>
       <c r="H175" s="14"/>
       <c r="I175" s="7"/>
-      <c r="J175" s="20" t="s">
+      <c r="J175" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K175" s="21"/>
-      <c r="L175" s="21"/>
-      <c r="M175" s="21"/>
-      <c r="N175" s="22"/>
+      <c r="K175" s="17"/>
+      <c r="L175" s="17"/>
+      <c r="M175" s="17"/>
+      <c r="N175" s="18"/>
       <c r="O175" s="2"/>
     </row>
     <row r="176" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B176" s="27"/>
-      <c r="C176" s="20" t="s">
+      <c r="B176" s="26"/>
+      <c r="C176" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D176" s="21"/>
-      <c r="E176" s="21"/>
-      <c r="F176" s="21"/>
-      <c r="G176" s="22"/>
+      <c r="D176" s="17"/>
+      <c r="E176" s="17"/>
+      <c r="F176" s="17"/>
+      <c r="G176" s="18"/>
       <c r="H176" s="14"/>
       <c r="I176" s="7"/>
-      <c r="J176" s="20" t="s">
+      <c r="J176" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K176" s="21"/>
-      <c r="L176" s="21"/>
-      <c r="M176" s="21"/>
-      <c r="N176" s="22"/>
+      <c r="K176" s="17"/>
+      <c r="L176" s="17"/>
+      <c r="M176" s="17"/>
+      <c r="N176" s="18"/>
       <c r="O176" s="2"/>
     </row>
     <row r="177" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B177" s="27"/>
+      <c r="B177" s="26"/>
       <c r="C177" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D177" s="21"/>
-      <c r="E177" s="21"/>
-      <c r="F177" s="21"/>
-      <c r="G177" s="22"/>
+      <c r="D177" s="17"/>
+      <c r="E177" s="17"/>
+      <c r="F177" s="17"/>
+      <c r="G177" s="18"/>
       <c r="H177" s="14"/>
       <c r="I177" s="7"/>
       <c r="J177" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K177" s="21"/>
-      <c r="L177" s="21"/>
-      <c r="M177" s="21"/>
-      <c r="N177" s="22"/>
+      <c r="K177" s="17"/>
+      <c r="L177" s="17"/>
+      <c r="M177" s="17"/>
+      <c r="N177" s="18"/>
       <c r="O177" s="2"/>
     </row>
     <row r="178" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B178" s="27"/>
-      <c r="C178" s="25" t="s">
+      <c r="B178" s="26"/>
+      <c r="C178" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D178" s="21"/>
-      <c r="E178" s="21"/>
-      <c r="F178" s="21"/>
-      <c r="G178" s="22"/>
+      <c r="D178" s="17"/>
+      <c r="E178" s="17"/>
+      <c r="F178" s="17"/>
+      <c r="G178" s="18"/>
       <c r="H178" s="14"/>
       <c r="I178" s="7"/>
-      <c r="J178" s="25" t="s">
+      <c r="J178" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K178" s="21"/>
-      <c r="L178" s="21"/>
-      <c r="M178" s="21"/>
-      <c r="N178" s="22"/>
+      <c r="K178" s="17"/>
+      <c r="L178" s="17"/>
+      <c r="M178" s="17"/>
+      <c r="N178" s="18"/>
       <c r="O178" s="2"/>
     </row>
     <row r="179" spans="2:15" x14ac:dyDescent="0.25">
@@ -5658,20 +5674,20 @@
       <c r="O183" s="2"/>
     </row>
     <row r="184" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B184" s="23" t="s">
+      <c r="B184" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C184" s="18"/>
-      <c r="D184" s="18"/>
+      <c r="C184" s="20"/>
+      <c r="D184" s="20"/>
       <c r="E184" s="14"/>
       <c r="F184" s="4"/>
       <c r="G184" s="15"/>
       <c r="H184" s="14"/>
-      <c r="I184" s="23" t="s">
+      <c r="I184" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J184" s="18"/>
-      <c r="K184" s="18"/>
+      <c r="J184" s="20"/>
+      <c r="K184" s="20"/>
       <c r="L184" s="14"/>
       <c r="M184" s="4"/>
       <c r="N184" s="15"/>
@@ -5727,62 +5743,62 @@
     </row>
     <row r="188" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
-      <c r="C188" s="17" t="s">
+      <c r="C188" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D188" s="18"/>
-      <c r="E188" s="18"/>
-      <c r="F188" s="18"/>
-      <c r="G188" s="19"/>
+      <c r="D188" s="20"/>
+      <c r="E188" s="20"/>
+      <c r="F188" s="20"/>
+      <c r="G188" s="22"/>
       <c r="H188" s="14"/>
       <c r="I188" s="6"/>
-      <c r="J188" s="17" t="s">
+      <c r="J188" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K188" s="18"/>
-      <c r="L188" s="18"/>
-      <c r="M188" s="18"/>
-      <c r="N188" s="19"/>
+      <c r="K188" s="20"/>
+      <c r="L188" s="20"/>
+      <c r="M188" s="20"/>
+      <c r="N188" s="22"/>
       <c r="O188" s="2"/>
     </row>
     <row r="189" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B189" s="7"/>
-      <c r="C189" s="20" t="s">
+      <c r="C189" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D189" s="21"/>
-      <c r="E189" s="21"/>
-      <c r="F189" s="21"/>
-      <c r="G189" s="22"/>
+      <c r="D189" s="17"/>
+      <c r="E189" s="17"/>
+      <c r="F189" s="17"/>
+      <c r="G189" s="18"/>
       <c r="H189" s="14"/>
       <c r="I189" s="7"/>
-      <c r="J189" s="20" t="s">
+      <c r="J189" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K189" s="21"/>
-      <c r="L189" s="21"/>
-      <c r="M189" s="21"/>
-      <c r="N189" s="22"/>
+      <c r="K189" s="17"/>
+      <c r="L189" s="17"/>
+      <c r="M189" s="17"/>
+      <c r="N189" s="18"/>
       <c r="O189" s="2"/>
     </row>
     <row r="190" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B190" s="7"/>
-      <c r="C190" s="20" t="s">
+      <c r="C190" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D190" s="21"/>
-      <c r="E190" s="21"/>
-      <c r="F190" s="21"/>
-      <c r="G190" s="22"/>
+      <c r="D190" s="17"/>
+      <c r="E190" s="17"/>
+      <c r="F190" s="17"/>
+      <c r="G190" s="18"/>
       <c r="H190" s="14"/>
       <c r="I190" s="7"/>
-      <c r="J190" s="20" t="s">
+      <c r="J190" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K190" s="21"/>
-      <c r="L190" s="21"/>
-      <c r="M190" s="21"/>
-      <c r="N190" s="22"/>
+      <c r="K190" s="17"/>
+      <c r="L190" s="17"/>
+      <c r="M190" s="17"/>
+      <c r="N190" s="18"/>
       <c r="O190" s="2"/>
     </row>
     <row r="191" spans="2:15" x14ac:dyDescent="0.25">
@@ -5790,39 +5806,39 @@
       <c r="C191" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D191" s="21"/>
-      <c r="E191" s="21"/>
-      <c r="F191" s="21"/>
-      <c r="G191" s="22"/>
+      <c r="D191" s="17"/>
+      <c r="E191" s="17"/>
+      <c r="F191" s="17"/>
+      <c r="G191" s="18"/>
       <c r="H191" s="14"/>
       <c r="I191" s="7"/>
       <c r="J191" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K191" s="21"/>
-      <c r="L191" s="21"/>
-      <c r="M191" s="21"/>
-      <c r="N191" s="22"/>
+      <c r="K191" s="17"/>
+      <c r="L191" s="17"/>
+      <c r="M191" s="17"/>
+      <c r="N191" s="18"/>
       <c r="O191" s="2"/>
     </row>
     <row r="192" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B192" s="7"/>
-      <c r="C192" s="25" t="s">
+      <c r="C192" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D192" s="21"/>
-      <c r="E192" s="21"/>
-      <c r="F192" s="21"/>
-      <c r="G192" s="22"/>
+      <c r="D192" s="17"/>
+      <c r="E192" s="17"/>
+      <c r="F192" s="17"/>
+      <c r="G192" s="18"/>
       <c r="H192" s="14"/>
       <c r="I192" s="7"/>
-      <c r="J192" s="25" t="s">
+      <c r="J192" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K192" s="21"/>
-      <c r="L192" s="21"/>
-      <c r="M192" s="21"/>
-      <c r="N192" s="22"/>
+      <c r="K192" s="17"/>
+      <c r="L192" s="17"/>
+      <c r="M192" s="17"/>
+      <c r="N192" s="18"/>
       <c r="O192" s="2"/>
     </row>
     <row r="193" spans="2:15" x14ac:dyDescent="0.25">
@@ -5922,20 +5938,20 @@
       <c r="O197" s="2"/>
     </row>
     <row r="198" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B198" s="23" t="s">
+      <c r="B198" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C198" s="18"/>
-      <c r="D198" s="18"/>
+      <c r="C198" s="20"/>
+      <c r="D198" s="20"/>
       <c r="E198" s="14"/>
       <c r="F198" s="4"/>
       <c r="G198" s="15"/>
       <c r="H198" s="14"/>
-      <c r="I198" s="23" t="s">
+      <c r="I198" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J198" s="18"/>
-      <c r="K198" s="18"/>
+      <c r="J198" s="20"/>
+      <c r="K198" s="20"/>
       <c r="L198" s="14"/>
       <c r="M198" s="4"/>
       <c r="N198" s="15"/>
@@ -5977,103 +5993,103 @@
       <c r="O201" s="2"/>
     </row>
     <row r="202" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B202" s="26"/>
-      <c r="C202" s="17" t="s">
+      <c r="B202" s="25"/>
+      <c r="C202" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D202" s="18"/>
-      <c r="E202" s="18"/>
-      <c r="F202" s="18"/>
-      <c r="G202" s="19"/>
+      <c r="D202" s="20"/>
+      <c r="E202" s="20"/>
+      <c r="F202" s="20"/>
+      <c r="G202" s="22"/>
       <c r="H202" s="14"/>
       <c r="I202" s="6"/>
-      <c r="J202" s="17" t="s">
+      <c r="J202" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K202" s="18"/>
-      <c r="L202" s="18"/>
-      <c r="M202" s="18"/>
-      <c r="N202" s="19"/>
+      <c r="K202" s="20"/>
+      <c r="L202" s="20"/>
+      <c r="M202" s="20"/>
+      <c r="N202" s="22"/>
       <c r="O202" s="2"/>
     </row>
     <row r="203" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B203" s="27"/>
-      <c r="C203" s="20" t="s">
+      <c r="B203" s="26"/>
+      <c r="C203" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D203" s="21"/>
-      <c r="E203" s="21"/>
-      <c r="F203" s="21"/>
-      <c r="G203" s="22"/>
+      <c r="D203" s="17"/>
+      <c r="E203" s="17"/>
+      <c r="F203" s="17"/>
+      <c r="G203" s="18"/>
       <c r="H203" s="14"/>
       <c r="I203" s="7"/>
-      <c r="J203" s="20" t="s">
+      <c r="J203" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K203" s="21"/>
-      <c r="L203" s="21"/>
-      <c r="M203" s="21"/>
-      <c r="N203" s="22"/>
+      <c r="K203" s="17"/>
+      <c r="L203" s="17"/>
+      <c r="M203" s="17"/>
+      <c r="N203" s="18"/>
       <c r="O203" s="2"/>
     </row>
     <row r="204" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B204" s="27"/>
-      <c r="C204" s="20" t="s">
+      <c r="B204" s="26"/>
+      <c r="C204" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D204" s="21"/>
-      <c r="E204" s="21"/>
-      <c r="F204" s="21"/>
-      <c r="G204" s="22"/>
+      <c r="D204" s="17"/>
+      <c r="E204" s="17"/>
+      <c r="F204" s="17"/>
+      <c r="G204" s="18"/>
       <c r="H204" s="14"/>
       <c r="I204" s="7"/>
-      <c r="J204" s="20" t="s">
+      <c r="J204" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K204" s="21"/>
-      <c r="L204" s="21"/>
-      <c r="M204" s="21"/>
-      <c r="N204" s="22"/>
+      <c r="K204" s="17"/>
+      <c r="L204" s="17"/>
+      <c r="M204" s="17"/>
+      <c r="N204" s="18"/>
       <c r="O204" s="2"/>
     </row>
     <row r="205" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B205" s="27"/>
+      <c r="B205" s="26"/>
       <c r="C205" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D205" s="21"/>
-      <c r="E205" s="21"/>
-      <c r="F205" s="21"/>
-      <c r="G205" s="22"/>
+      <c r="D205" s="17"/>
+      <c r="E205" s="17"/>
+      <c r="F205" s="17"/>
+      <c r="G205" s="18"/>
       <c r="H205" s="14"/>
       <c r="I205" s="7"/>
       <c r="J205" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K205" s="21"/>
-      <c r="L205" s="21"/>
-      <c r="M205" s="21"/>
-      <c r="N205" s="22"/>
+      <c r="K205" s="17"/>
+      <c r="L205" s="17"/>
+      <c r="M205" s="17"/>
+      <c r="N205" s="18"/>
       <c r="O205" s="2"/>
     </row>
     <row r="206" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B206" s="27"/>
-      <c r="C206" s="25" t="s">
+      <c r="B206" s="26"/>
+      <c r="C206" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D206" s="21"/>
-      <c r="E206" s="21"/>
-      <c r="F206" s="21"/>
-      <c r="G206" s="22"/>
+      <c r="D206" s="17"/>
+      <c r="E206" s="17"/>
+      <c r="F206" s="17"/>
+      <c r="G206" s="18"/>
       <c r="H206" s="14"/>
       <c r="I206" s="7"/>
-      <c r="J206" s="25" t="s">
+      <c r="J206" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K206" s="21"/>
-      <c r="L206" s="21"/>
-      <c r="M206" s="21"/>
-      <c r="N206" s="22"/>
+      <c r="K206" s="17"/>
+      <c r="L206" s="17"/>
+      <c r="M206" s="17"/>
+      <c r="N206" s="18"/>
       <c r="O206" s="2"/>
     </row>
     <row r="207" spans="2:15" x14ac:dyDescent="0.25">
@@ -6173,20 +6189,20 @@
       <c r="O211" s="2"/>
     </row>
     <row r="212" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B212" s="23" t="s">
+      <c r="B212" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C212" s="18"/>
-      <c r="D212" s="18"/>
+      <c r="C212" s="20"/>
+      <c r="D212" s="20"/>
       <c r="E212" s="14"/>
       <c r="F212" s="4"/>
       <c r="G212" s="15"/>
       <c r="H212" s="14"/>
-      <c r="I212" s="23" t="s">
+      <c r="I212" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J212" s="18"/>
-      <c r="K212" s="18"/>
+      <c r="J212" s="20"/>
+      <c r="K212" s="20"/>
       <c r="L212" s="14"/>
       <c r="M212" s="4"/>
       <c r="N212" s="15"/>
@@ -6242,62 +6258,62 @@
     </row>
     <row r="216" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B216" s="6"/>
-      <c r="C216" s="17" t="s">
+      <c r="C216" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D216" s="18"/>
-      <c r="E216" s="18"/>
-      <c r="F216" s="18"/>
-      <c r="G216" s="19"/>
+      <c r="D216" s="20"/>
+      <c r="E216" s="20"/>
+      <c r="F216" s="20"/>
+      <c r="G216" s="22"/>
       <c r="H216" s="14"/>
       <c r="I216" s="6"/>
-      <c r="J216" s="17" t="s">
+      <c r="J216" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K216" s="18"/>
-      <c r="L216" s="18"/>
-      <c r="M216" s="18"/>
-      <c r="N216" s="19"/>
+      <c r="K216" s="20"/>
+      <c r="L216" s="20"/>
+      <c r="M216" s="20"/>
+      <c r="N216" s="22"/>
       <c r="O216" s="2"/>
     </row>
     <row r="217" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B217" s="7"/>
-      <c r="C217" s="20" t="s">
+      <c r="C217" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D217" s="21"/>
-      <c r="E217" s="21"/>
-      <c r="F217" s="21"/>
-      <c r="G217" s="22"/>
+      <c r="D217" s="17"/>
+      <c r="E217" s="17"/>
+      <c r="F217" s="17"/>
+      <c r="G217" s="18"/>
       <c r="H217" s="14"/>
       <c r="I217" s="7"/>
-      <c r="J217" s="20" t="s">
+      <c r="J217" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K217" s="21"/>
-      <c r="L217" s="21"/>
-      <c r="M217" s="21"/>
-      <c r="N217" s="22"/>
+      <c r="K217" s="17"/>
+      <c r="L217" s="17"/>
+      <c r="M217" s="17"/>
+      <c r="N217" s="18"/>
       <c r="O217" s="2"/>
     </row>
     <row r="218" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B218" s="7"/>
-      <c r="C218" s="20" t="s">
+      <c r="C218" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D218" s="21"/>
-      <c r="E218" s="21"/>
-      <c r="F218" s="21"/>
-      <c r="G218" s="22"/>
+      <c r="D218" s="17"/>
+      <c r="E218" s="17"/>
+      <c r="F218" s="17"/>
+      <c r="G218" s="18"/>
       <c r="H218" s="14"/>
       <c r="I218" s="7"/>
-      <c r="J218" s="20" t="s">
+      <c r="J218" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K218" s="21"/>
-      <c r="L218" s="21"/>
-      <c r="M218" s="21"/>
-      <c r="N218" s="22"/>
+      <c r="K218" s="17"/>
+      <c r="L218" s="17"/>
+      <c r="M218" s="17"/>
+      <c r="N218" s="18"/>
       <c r="O218" s="2"/>
     </row>
     <row r="219" spans="2:15" x14ac:dyDescent="0.25">
@@ -6305,39 +6321,39 @@
       <c r="C219" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D219" s="21"/>
-      <c r="E219" s="21"/>
-      <c r="F219" s="21"/>
-      <c r="G219" s="22"/>
+      <c r="D219" s="17"/>
+      <c r="E219" s="17"/>
+      <c r="F219" s="17"/>
+      <c r="G219" s="18"/>
       <c r="H219" s="14"/>
       <c r="I219" s="7"/>
       <c r="J219" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K219" s="21"/>
-      <c r="L219" s="21"/>
-      <c r="M219" s="21"/>
-      <c r="N219" s="22"/>
+      <c r="K219" s="17"/>
+      <c r="L219" s="17"/>
+      <c r="M219" s="17"/>
+      <c r="N219" s="18"/>
       <c r="O219" s="2"/>
     </row>
     <row r="220" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B220" s="7"/>
-      <c r="C220" s="25" t="s">
+      <c r="C220" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D220" s="21"/>
-      <c r="E220" s="21"/>
-      <c r="F220" s="21"/>
-      <c r="G220" s="22"/>
+      <c r="D220" s="17"/>
+      <c r="E220" s="17"/>
+      <c r="F220" s="17"/>
+      <c r="G220" s="18"/>
       <c r="H220" s="14"/>
       <c r="I220" s="7"/>
-      <c r="J220" s="25" t="s">
+      <c r="J220" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K220" s="21"/>
-      <c r="L220" s="21"/>
-      <c r="M220" s="21"/>
-      <c r="N220" s="22"/>
+      <c r="K220" s="17"/>
+      <c r="L220" s="17"/>
+      <c r="M220" s="17"/>
+      <c r="N220" s="18"/>
       <c r="O220" s="2"/>
     </row>
     <row r="221" spans="2:15" x14ac:dyDescent="0.25">
@@ -6437,20 +6453,20 @@
       <c r="O225" s="2"/>
     </row>
     <row r="226" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B226" s="23" t="s">
+      <c r="B226" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C226" s="18"/>
-      <c r="D226" s="18"/>
+      <c r="C226" s="20"/>
+      <c r="D226" s="20"/>
       <c r="E226" s="14"/>
       <c r="F226" s="4"/>
       <c r="G226" s="15"/>
       <c r="H226" s="14"/>
-      <c r="I226" s="23" t="s">
+      <c r="I226" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J226" s="18"/>
-      <c r="K226" s="18"/>
+      <c r="J226" s="20"/>
+      <c r="K226" s="20"/>
       <c r="L226" s="14"/>
       <c r="M226" s="4"/>
       <c r="N226" s="15"/>
@@ -6492,103 +6508,103 @@
       <c r="O229" s="2"/>
     </row>
     <row r="230" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B230" s="26"/>
-      <c r="C230" s="17" t="s">
+      <c r="B230" s="25"/>
+      <c r="C230" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D230" s="18"/>
-      <c r="E230" s="18"/>
-      <c r="F230" s="18"/>
-      <c r="G230" s="19"/>
+      <c r="D230" s="20"/>
+      <c r="E230" s="20"/>
+      <c r="F230" s="20"/>
+      <c r="G230" s="22"/>
       <c r="H230" s="14"/>
       <c r="I230" s="6"/>
-      <c r="J230" s="17" t="s">
+      <c r="J230" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K230" s="18"/>
-      <c r="L230" s="18"/>
-      <c r="M230" s="18"/>
-      <c r="N230" s="19"/>
+      <c r="K230" s="20"/>
+      <c r="L230" s="20"/>
+      <c r="M230" s="20"/>
+      <c r="N230" s="22"/>
       <c r="O230" s="2"/>
     </row>
     <row r="231" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B231" s="27"/>
-      <c r="C231" s="20" t="s">
+      <c r="B231" s="26"/>
+      <c r="C231" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D231" s="21"/>
-      <c r="E231" s="21"/>
-      <c r="F231" s="21"/>
-      <c r="G231" s="22"/>
+      <c r="D231" s="17"/>
+      <c r="E231" s="17"/>
+      <c r="F231" s="17"/>
+      <c r="G231" s="18"/>
       <c r="H231" s="14"/>
       <c r="I231" s="7"/>
-      <c r="J231" s="20" t="s">
+      <c r="J231" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K231" s="21"/>
-      <c r="L231" s="21"/>
-      <c r="M231" s="21"/>
-      <c r="N231" s="22"/>
+      <c r="K231" s="17"/>
+      <c r="L231" s="17"/>
+      <c r="M231" s="17"/>
+      <c r="N231" s="18"/>
       <c r="O231" s="2"/>
     </row>
     <row r="232" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B232" s="27"/>
-      <c r="C232" s="20" t="s">
+      <c r="B232" s="26"/>
+      <c r="C232" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D232" s="21"/>
-      <c r="E232" s="21"/>
-      <c r="F232" s="21"/>
-      <c r="G232" s="22"/>
+      <c r="D232" s="17"/>
+      <c r="E232" s="17"/>
+      <c r="F232" s="17"/>
+      <c r="G232" s="18"/>
       <c r="H232" s="14"/>
       <c r="I232" s="7"/>
-      <c r="J232" s="20" t="s">
+      <c r="J232" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K232" s="21"/>
-      <c r="L232" s="21"/>
-      <c r="M232" s="21"/>
-      <c r="N232" s="22"/>
+      <c r="K232" s="17"/>
+      <c r="L232" s="17"/>
+      <c r="M232" s="17"/>
+      <c r="N232" s="18"/>
       <c r="O232" s="2"/>
     </row>
     <row r="233" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B233" s="27"/>
+      <c r="B233" s="26"/>
       <c r="C233" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D233" s="21"/>
-      <c r="E233" s="21"/>
-      <c r="F233" s="21"/>
-      <c r="G233" s="22"/>
+      <c r="D233" s="17"/>
+      <c r="E233" s="17"/>
+      <c r="F233" s="17"/>
+      <c r="G233" s="18"/>
       <c r="H233" s="14"/>
       <c r="I233" s="7"/>
       <c r="J233" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K233" s="21"/>
-      <c r="L233" s="21"/>
-      <c r="M233" s="21"/>
-      <c r="N233" s="22"/>
+      <c r="K233" s="17"/>
+      <c r="L233" s="17"/>
+      <c r="M233" s="17"/>
+      <c r="N233" s="18"/>
       <c r="O233" s="2"/>
     </row>
     <row r="234" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B234" s="27"/>
-      <c r="C234" s="25" t="s">
+      <c r="B234" s="26"/>
+      <c r="C234" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D234" s="21"/>
-      <c r="E234" s="21"/>
-      <c r="F234" s="21"/>
-      <c r="G234" s="22"/>
+      <c r="D234" s="17"/>
+      <c r="E234" s="17"/>
+      <c r="F234" s="17"/>
+      <c r="G234" s="18"/>
       <c r="H234" s="14"/>
       <c r="I234" s="7"/>
-      <c r="J234" s="25" t="s">
+      <c r="J234" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K234" s="21"/>
-      <c r="L234" s="21"/>
-      <c r="M234" s="21"/>
-      <c r="N234" s="22"/>
+      <c r="K234" s="17"/>
+      <c r="L234" s="17"/>
+      <c r="M234" s="17"/>
+      <c r="N234" s="18"/>
       <c r="O234" s="2"/>
     </row>
     <row r="235" spans="2:15" x14ac:dyDescent="0.25">
@@ -6688,20 +6704,20 @@
       <c r="O239" s="2"/>
     </row>
     <row r="240" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B240" s="23" t="s">
+      <c r="B240" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C240" s="18"/>
-      <c r="D240" s="18"/>
+      <c r="C240" s="20"/>
+      <c r="D240" s="20"/>
       <c r="E240" s="14"/>
       <c r="F240" s="4"/>
       <c r="G240" s="15"/>
       <c r="H240" s="14"/>
-      <c r="I240" s="23" t="s">
+      <c r="I240" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J240" s="18"/>
-      <c r="K240" s="18"/>
+      <c r="J240" s="20"/>
+      <c r="K240" s="20"/>
       <c r="L240" s="14"/>
       <c r="M240" s="4"/>
       <c r="N240" s="15"/>
@@ -6757,62 +6773,62 @@
     </row>
     <row r="244" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B244" s="6"/>
-      <c r="C244" s="17" t="s">
+      <c r="C244" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D244" s="18"/>
-      <c r="E244" s="18"/>
-      <c r="F244" s="18"/>
-      <c r="G244" s="19"/>
+      <c r="D244" s="20"/>
+      <c r="E244" s="20"/>
+      <c r="F244" s="20"/>
+      <c r="G244" s="22"/>
       <c r="H244" s="14"/>
       <c r="I244" s="6"/>
-      <c r="J244" s="17" t="s">
+      <c r="J244" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K244" s="18"/>
-      <c r="L244" s="18"/>
-      <c r="M244" s="18"/>
-      <c r="N244" s="19"/>
+      <c r="K244" s="20"/>
+      <c r="L244" s="20"/>
+      <c r="M244" s="20"/>
+      <c r="N244" s="22"/>
       <c r="O244" s="2"/>
     </row>
     <row r="245" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B245" s="7"/>
-      <c r="C245" s="20" t="s">
+      <c r="C245" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D245" s="21"/>
-      <c r="E245" s="21"/>
-      <c r="F245" s="21"/>
-      <c r="G245" s="22"/>
+      <c r="D245" s="17"/>
+      <c r="E245" s="17"/>
+      <c r="F245" s="17"/>
+      <c r="G245" s="18"/>
       <c r="H245" s="14"/>
       <c r="I245" s="7"/>
-      <c r="J245" s="20" t="s">
+      <c r="J245" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K245" s="21"/>
-      <c r="L245" s="21"/>
-      <c r="M245" s="21"/>
-      <c r="N245" s="22"/>
+      <c r="K245" s="17"/>
+      <c r="L245" s="17"/>
+      <c r="M245" s="17"/>
+      <c r="N245" s="18"/>
       <c r="O245" s="2"/>
     </row>
     <row r="246" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B246" s="7"/>
-      <c r="C246" s="20" t="s">
+      <c r="C246" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D246" s="21"/>
-      <c r="E246" s="21"/>
-      <c r="F246" s="21"/>
-      <c r="G246" s="22"/>
+      <c r="D246" s="17"/>
+      <c r="E246" s="17"/>
+      <c r="F246" s="17"/>
+      <c r="G246" s="18"/>
       <c r="H246" s="14"/>
       <c r="I246" s="7"/>
-      <c r="J246" s="20" t="s">
+      <c r="J246" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K246" s="21"/>
-      <c r="L246" s="21"/>
-      <c r="M246" s="21"/>
-      <c r="N246" s="22"/>
+      <c r="K246" s="17"/>
+      <c r="L246" s="17"/>
+      <c r="M246" s="17"/>
+      <c r="N246" s="18"/>
       <c r="O246" s="2"/>
     </row>
     <row r="247" spans="2:15" x14ac:dyDescent="0.25">
@@ -6820,39 +6836,39 @@
       <c r="C247" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D247" s="21"/>
-      <c r="E247" s="21"/>
-      <c r="F247" s="21"/>
-      <c r="G247" s="22"/>
+      <c r="D247" s="17"/>
+      <c r="E247" s="17"/>
+      <c r="F247" s="17"/>
+      <c r="G247" s="18"/>
       <c r="H247" s="14"/>
       <c r="I247" s="7"/>
       <c r="J247" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K247" s="21"/>
-      <c r="L247" s="21"/>
-      <c r="M247" s="21"/>
-      <c r="N247" s="22"/>
+      <c r="K247" s="17"/>
+      <c r="L247" s="17"/>
+      <c r="M247" s="17"/>
+      <c r="N247" s="18"/>
       <c r="O247" s="2"/>
     </row>
     <row r="248" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B248" s="7"/>
-      <c r="C248" s="25" t="s">
+      <c r="C248" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D248" s="21"/>
-      <c r="E248" s="21"/>
-      <c r="F248" s="21"/>
-      <c r="G248" s="22"/>
+      <c r="D248" s="17"/>
+      <c r="E248" s="17"/>
+      <c r="F248" s="17"/>
+      <c r="G248" s="18"/>
       <c r="H248" s="14"/>
       <c r="I248" s="7"/>
-      <c r="J248" s="25" t="s">
+      <c r="J248" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K248" s="21"/>
-      <c r="L248" s="21"/>
-      <c r="M248" s="21"/>
-      <c r="N248" s="22"/>
+      <c r="K248" s="17"/>
+      <c r="L248" s="17"/>
+      <c r="M248" s="17"/>
+      <c r="N248" s="18"/>
       <c r="O248" s="2"/>
     </row>
     <row r="249" spans="2:15" x14ac:dyDescent="0.25">
@@ -6952,20 +6968,20 @@
       <c r="O253" s="2"/>
     </row>
     <row r="254" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B254" s="23" t="s">
+      <c r="B254" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C254" s="18"/>
-      <c r="D254" s="18"/>
+      <c r="C254" s="20"/>
+      <c r="D254" s="20"/>
       <c r="E254" s="14"/>
       <c r="F254" s="4"/>
       <c r="G254" s="15"/>
       <c r="H254" s="14"/>
-      <c r="I254" s="23" t="s">
+      <c r="I254" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J254" s="18"/>
-      <c r="K254" s="18"/>
+      <c r="J254" s="20"/>
+      <c r="K254" s="20"/>
       <c r="L254" s="14"/>
       <c r="M254" s="4"/>
       <c r="N254" s="15"/>
@@ -7007,103 +7023,103 @@
       <c r="O257" s="2"/>
     </row>
     <row r="258" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B258" s="26"/>
-      <c r="C258" s="17" t="s">
+      <c r="B258" s="25"/>
+      <c r="C258" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D258" s="18"/>
-      <c r="E258" s="18"/>
-      <c r="F258" s="18"/>
-      <c r="G258" s="19"/>
+      <c r="D258" s="20"/>
+      <c r="E258" s="20"/>
+      <c r="F258" s="20"/>
+      <c r="G258" s="22"/>
       <c r="H258" s="14"/>
       <c r="I258" s="6"/>
-      <c r="J258" s="17" t="s">
+      <c r="J258" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K258" s="18"/>
-      <c r="L258" s="18"/>
-      <c r="M258" s="18"/>
-      <c r="N258" s="19"/>
+      <c r="K258" s="20"/>
+      <c r="L258" s="20"/>
+      <c r="M258" s="20"/>
+      <c r="N258" s="22"/>
       <c r="O258" s="2"/>
     </row>
     <row r="259" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B259" s="27"/>
-      <c r="C259" s="20" t="s">
+      <c r="B259" s="26"/>
+      <c r="C259" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D259" s="21"/>
-      <c r="E259" s="21"/>
-      <c r="F259" s="21"/>
-      <c r="G259" s="22"/>
+      <c r="D259" s="17"/>
+      <c r="E259" s="17"/>
+      <c r="F259" s="17"/>
+      <c r="G259" s="18"/>
       <c r="H259" s="14"/>
       <c r="I259" s="7"/>
-      <c r="J259" s="20" t="s">
+      <c r="J259" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K259" s="21"/>
-      <c r="L259" s="21"/>
-      <c r="M259" s="21"/>
-      <c r="N259" s="22"/>
+      <c r="K259" s="17"/>
+      <c r="L259" s="17"/>
+      <c r="M259" s="17"/>
+      <c r="N259" s="18"/>
       <c r="O259" s="2"/>
     </row>
     <row r="260" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B260" s="27"/>
-      <c r="C260" s="20" t="s">
+      <c r="B260" s="26"/>
+      <c r="C260" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D260" s="21"/>
-      <c r="E260" s="21"/>
-      <c r="F260" s="21"/>
-      <c r="G260" s="22"/>
+      <c r="D260" s="17"/>
+      <c r="E260" s="17"/>
+      <c r="F260" s="17"/>
+      <c r="G260" s="18"/>
       <c r="H260" s="14"/>
       <c r="I260" s="7"/>
-      <c r="J260" s="20" t="s">
+      <c r="J260" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K260" s="21"/>
-      <c r="L260" s="21"/>
-      <c r="M260" s="21"/>
-      <c r="N260" s="22"/>
+      <c r="K260" s="17"/>
+      <c r="L260" s="17"/>
+      <c r="M260" s="17"/>
+      <c r="N260" s="18"/>
       <c r="O260" s="2"/>
     </row>
     <row r="261" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B261" s="27"/>
+      <c r="B261" s="26"/>
       <c r="C261" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D261" s="21"/>
-      <c r="E261" s="21"/>
-      <c r="F261" s="21"/>
-      <c r="G261" s="22"/>
+      <c r="D261" s="17"/>
+      <c r="E261" s="17"/>
+      <c r="F261" s="17"/>
+      <c r="G261" s="18"/>
       <c r="H261" s="14"/>
       <c r="I261" s="7"/>
       <c r="J261" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K261" s="21"/>
-      <c r="L261" s="21"/>
-      <c r="M261" s="21"/>
-      <c r="N261" s="22"/>
+      <c r="K261" s="17"/>
+      <c r="L261" s="17"/>
+      <c r="M261" s="17"/>
+      <c r="N261" s="18"/>
       <c r="O261" s="2"/>
     </row>
     <row r="262" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B262" s="27"/>
-      <c r="C262" s="25" t="s">
+      <c r="B262" s="26"/>
+      <c r="C262" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D262" s="21"/>
-      <c r="E262" s="21"/>
-      <c r="F262" s="21"/>
-      <c r="G262" s="22"/>
+      <c r="D262" s="17"/>
+      <c r="E262" s="17"/>
+      <c r="F262" s="17"/>
+      <c r="G262" s="18"/>
       <c r="H262" s="14"/>
       <c r="I262" s="7"/>
-      <c r="J262" s="25" t="s">
+      <c r="J262" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K262" s="21"/>
-      <c r="L262" s="21"/>
-      <c r="M262" s="21"/>
-      <c r="N262" s="22"/>
+      <c r="K262" s="17"/>
+      <c r="L262" s="17"/>
+      <c r="M262" s="17"/>
+      <c r="N262" s="18"/>
       <c r="O262" s="2"/>
     </row>
     <row r="263" spans="2:15" x14ac:dyDescent="0.25">
@@ -7203,20 +7219,20 @@
       <c r="O267" s="2"/>
     </row>
     <row r="268" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B268" s="23" t="s">
+      <c r="B268" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C268" s="18"/>
-      <c r="D268" s="18"/>
+      <c r="C268" s="20"/>
+      <c r="D268" s="20"/>
       <c r="E268" s="14"/>
       <c r="F268" s="4"/>
       <c r="G268" s="15"/>
       <c r="H268" s="14"/>
-      <c r="I268" s="23" t="s">
+      <c r="I268" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J268" s="18"/>
-      <c r="K268" s="18"/>
+      <c r="J268" s="20"/>
+      <c r="K268" s="20"/>
       <c r="L268" s="14"/>
       <c r="M268" s="4"/>
       <c r="N268" s="15"/>
@@ -7272,62 +7288,62 @@
     </row>
     <row r="272" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B272" s="6"/>
-      <c r="C272" s="17" t="s">
+      <c r="C272" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D272" s="18"/>
-      <c r="E272" s="18"/>
-      <c r="F272" s="18"/>
-      <c r="G272" s="19"/>
+      <c r="D272" s="20"/>
+      <c r="E272" s="20"/>
+      <c r="F272" s="20"/>
+      <c r="G272" s="22"/>
       <c r="H272" s="14"/>
       <c r="I272" s="6"/>
-      <c r="J272" s="17" t="s">
+      <c r="J272" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K272" s="18"/>
-      <c r="L272" s="18"/>
-      <c r="M272" s="18"/>
-      <c r="N272" s="19"/>
+      <c r="K272" s="20"/>
+      <c r="L272" s="20"/>
+      <c r="M272" s="20"/>
+      <c r="N272" s="22"/>
       <c r="O272" s="2"/>
     </row>
     <row r="273" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B273" s="7"/>
-      <c r="C273" s="20" t="s">
+      <c r="C273" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D273" s="21"/>
-      <c r="E273" s="21"/>
-      <c r="F273" s="21"/>
-      <c r="G273" s="22"/>
+      <c r="D273" s="17"/>
+      <c r="E273" s="17"/>
+      <c r="F273" s="17"/>
+      <c r="G273" s="18"/>
       <c r="H273" s="14"/>
       <c r="I273" s="7"/>
-      <c r="J273" s="20" t="s">
+      <c r="J273" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K273" s="21"/>
-      <c r="L273" s="21"/>
-      <c r="M273" s="21"/>
-      <c r="N273" s="22"/>
+      <c r="K273" s="17"/>
+      <c r="L273" s="17"/>
+      <c r="M273" s="17"/>
+      <c r="N273" s="18"/>
       <c r="O273" s="2"/>
     </row>
     <row r="274" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B274" s="7"/>
-      <c r="C274" s="20" t="s">
+      <c r="C274" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D274" s="21"/>
-      <c r="E274" s="21"/>
-      <c r="F274" s="21"/>
-      <c r="G274" s="22"/>
+      <c r="D274" s="17"/>
+      <c r="E274" s="17"/>
+      <c r="F274" s="17"/>
+      <c r="G274" s="18"/>
       <c r="H274" s="14"/>
       <c r="I274" s="7"/>
-      <c r="J274" s="20" t="s">
+      <c r="J274" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K274" s="21"/>
-      <c r="L274" s="21"/>
-      <c r="M274" s="21"/>
-      <c r="N274" s="22"/>
+      <c r="K274" s="17"/>
+      <c r="L274" s="17"/>
+      <c r="M274" s="17"/>
+      <c r="N274" s="18"/>
       <c r="O274" s="2"/>
     </row>
     <row r="275" spans="2:15" x14ac:dyDescent="0.25">
@@ -7335,39 +7351,39 @@
       <c r="C275" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D275" s="21"/>
-      <c r="E275" s="21"/>
-      <c r="F275" s="21"/>
-      <c r="G275" s="22"/>
+      <c r="D275" s="17"/>
+      <c r="E275" s="17"/>
+      <c r="F275" s="17"/>
+      <c r="G275" s="18"/>
       <c r="H275" s="14"/>
       <c r="I275" s="7"/>
       <c r="J275" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K275" s="21"/>
-      <c r="L275" s="21"/>
-      <c r="M275" s="21"/>
-      <c r="N275" s="22"/>
+      <c r="K275" s="17"/>
+      <c r="L275" s="17"/>
+      <c r="M275" s="17"/>
+      <c r="N275" s="18"/>
       <c r="O275" s="2"/>
     </row>
     <row r="276" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B276" s="7"/>
-      <c r="C276" s="25" t="s">
+      <c r="C276" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D276" s="21"/>
-      <c r="E276" s="21"/>
-      <c r="F276" s="21"/>
-      <c r="G276" s="22"/>
+      <c r="D276" s="17"/>
+      <c r="E276" s="17"/>
+      <c r="F276" s="17"/>
+      <c r="G276" s="18"/>
       <c r="H276" s="14"/>
       <c r="I276" s="7"/>
-      <c r="J276" s="25" t="s">
+      <c r="J276" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K276" s="21"/>
-      <c r="L276" s="21"/>
-      <c r="M276" s="21"/>
-      <c r="N276" s="22"/>
+      <c r="K276" s="17"/>
+      <c r="L276" s="17"/>
+      <c r="M276" s="17"/>
+      <c r="N276" s="18"/>
       <c r="O276" s="2"/>
     </row>
     <row r="277" spans="2:15" x14ac:dyDescent="0.25">
@@ -7467,20 +7483,20 @@
       <c r="O281" s="2"/>
     </row>
     <row r="282" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B282" s="23" t="s">
+      <c r="B282" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C282" s="18"/>
-      <c r="D282" s="18"/>
+      <c r="C282" s="20"/>
+      <c r="D282" s="20"/>
       <c r="E282" s="14"/>
       <c r="F282" s="4"/>
       <c r="G282" s="15"/>
       <c r="H282" s="14"/>
-      <c r="I282" s="23" t="s">
+      <c r="I282" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J282" s="18"/>
-      <c r="K282" s="18"/>
+      <c r="J282" s="20"/>
+      <c r="K282" s="20"/>
       <c r="L282" s="14"/>
       <c r="M282" s="4"/>
       <c r="N282" s="15"/>
@@ -7519,205 +7535,30 @@
     </row>
   </sheetData>
   <mergeCells count="250">
-    <mergeCell ref="C276:G276"/>
-    <mergeCell ref="J276:N276"/>
-    <mergeCell ref="B282:D282"/>
-    <mergeCell ref="I282:K282"/>
-    <mergeCell ref="B268:D268"/>
-    <mergeCell ref="I268:K268"/>
-    <mergeCell ref="C272:G272"/>
-    <mergeCell ref="J272:N272"/>
-    <mergeCell ref="C273:G273"/>
-    <mergeCell ref="J273:N273"/>
-    <mergeCell ref="C274:G274"/>
-    <mergeCell ref="J274:N274"/>
-    <mergeCell ref="C275:G275"/>
-    <mergeCell ref="J275:N275"/>
-    <mergeCell ref="C248:G248"/>
-    <mergeCell ref="J248:N248"/>
-    <mergeCell ref="B254:D254"/>
-    <mergeCell ref="I254:K254"/>
-    <mergeCell ref="B258:B262"/>
-    <mergeCell ref="C258:G258"/>
-    <mergeCell ref="J258:N258"/>
-    <mergeCell ref="C259:G259"/>
-    <mergeCell ref="J259:N259"/>
-    <mergeCell ref="C260:G260"/>
-    <mergeCell ref="J260:N260"/>
-    <mergeCell ref="C261:G261"/>
-    <mergeCell ref="J261:N261"/>
-    <mergeCell ref="C262:G262"/>
-    <mergeCell ref="J262:N262"/>
-    <mergeCell ref="B240:D240"/>
-    <mergeCell ref="I240:K240"/>
-    <mergeCell ref="C244:G244"/>
-    <mergeCell ref="J244:N244"/>
-    <mergeCell ref="C245:G245"/>
-    <mergeCell ref="J245:N245"/>
-    <mergeCell ref="C246:G246"/>
-    <mergeCell ref="J246:N246"/>
-    <mergeCell ref="C247:G247"/>
-    <mergeCell ref="J247:N247"/>
-    <mergeCell ref="B230:B234"/>
-    <mergeCell ref="C230:G230"/>
-    <mergeCell ref="J230:N230"/>
-    <mergeCell ref="C231:G231"/>
-    <mergeCell ref="J231:N231"/>
-    <mergeCell ref="C232:G232"/>
-    <mergeCell ref="J232:N232"/>
-    <mergeCell ref="C233:G233"/>
-    <mergeCell ref="J233:N233"/>
-    <mergeCell ref="C234:G234"/>
-    <mergeCell ref="J234:N234"/>
-    <mergeCell ref="C217:G217"/>
-    <mergeCell ref="J217:N217"/>
-    <mergeCell ref="C218:G218"/>
-    <mergeCell ref="J218:N218"/>
-    <mergeCell ref="C219:G219"/>
-    <mergeCell ref="J219:N219"/>
-    <mergeCell ref="C220:G220"/>
-    <mergeCell ref="J220:N220"/>
-    <mergeCell ref="B226:D226"/>
-    <mergeCell ref="I226:K226"/>
-    <mergeCell ref="B202:B206"/>
-    <mergeCell ref="J202:N202"/>
-    <mergeCell ref="J203:N203"/>
-    <mergeCell ref="J204:N204"/>
-    <mergeCell ref="J205:N205"/>
-    <mergeCell ref="J206:N206"/>
-    <mergeCell ref="B212:D212"/>
-    <mergeCell ref="I212:K212"/>
-    <mergeCell ref="C216:G216"/>
-    <mergeCell ref="J216:N216"/>
-    <mergeCell ref="C204:G204"/>
-    <mergeCell ref="C206:G206"/>
-    <mergeCell ref="C205:G205"/>
-    <mergeCell ref="C202:G202"/>
-    <mergeCell ref="C203:G203"/>
-    <mergeCell ref="B184:D184"/>
-    <mergeCell ref="I184:K184"/>
-    <mergeCell ref="C188:G188"/>
-    <mergeCell ref="J188:N188"/>
-    <mergeCell ref="C189:G189"/>
-    <mergeCell ref="C191:G191"/>
-    <mergeCell ref="C192:G192"/>
-    <mergeCell ref="J192:N192"/>
-    <mergeCell ref="B198:D198"/>
-    <mergeCell ref="I198:K198"/>
-    <mergeCell ref="C190:G190"/>
-    <mergeCell ref="J189:N189"/>
-    <mergeCell ref="C164:G164"/>
-    <mergeCell ref="J164:N164"/>
-    <mergeCell ref="B170:D170"/>
-    <mergeCell ref="I170:K170"/>
-    <mergeCell ref="B174:B178"/>
-    <mergeCell ref="C175:G175"/>
-    <mergeCell ref="C176:G176"/>
-    <mergeCell ref="C177:G177"/>
-    <mergeCell ref="C178:G178"/>
-    <mergeCell ref="J178:N178"/>
-    <mergeCell ref="B156:D156"/>
-    <mergeCell ref="I156:K156"/>
-    <mergeCell ref="C160:G160"/>
-    <mergeCell ref="J160:N160"/>
-    <mergeCell ref="C161:G161"/>
-    <mergeCell ref="J161:N161"/>
-    <mergeCell ref="C162:G162"/>
-    <mergeCell ref="J162:N162"/>
-    <mergeCell ref="C163:G163"/>
-    <mergeCell ref="J163:N163"/>
-    <mergeCell ref="B142:D142"/>
-    <mergeCell ref="I142:K142"/>
-    <mergeCell ref="B146:B150"/>
-    <mergeCell ref="C146:G146"/>
-    <mergeCell ref="J146:N146"/>
-    <mergeCell ref="C147:G147"/>
-    <mergeCell ref="J147:N147"/>
-    <mergeCell ref="C148:G148"/>
-    <mergeCell ref="J148:N148"/>
-    <mergeCell ref="C149:G149"/>
-    <mergeCell ref="J149:N149"/>
-    <mergeCell ref="C150:G150"/>
-    <mergeCell ref="J150:N150"/>
-    <mergeCell ref="C132:G132"/>
-    <mergeCell ref="J132:N132"/>
-    <mergeCell ref="C133:G133"/>
-    <mergeCell ref="J133:N133"/>
-    <mergeCell ref="C134:G134"/>
-    <mergeCell ref="J134:N134"/>
-    <mergeCell ref="C135:G135"/>
-    <mergeCell ref="J135:N135"/>
-    <mergeCell ref="C136:G136"/>
-    <mergeCell ref="J136:N136"/>
-    <mergeCell ref="B118:B122"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="J118:N118"/>
-    <mergeCell ref="C119:G119"/>
-    <mergeCell ref="J119:N119"/>
-    <mergeCell ref="J120:N120"/>
-    <mergeCell ref="C121:G121"/>
-    <mergeCell ref="B128:D128"/>
-    <mergeCell ref="I128:K128"/>
-    <mergeCell ref="B100:D100"/>
-    <mergeCell ref="I100:K100"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="J104:N104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="J105:N105"/>
-    <mergeCell ref="J106:N106"/>
-    <mergeCell ref="J108:N108"/>
-    <mergeCell ref="B114:D114"/>
-    <mergeCell ref="I114:K114"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="I86:K86"/>
-    <mergeCell ref="B90:B94"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="J90:N90"/>
-    <mergeCell ref="J91:N91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="J92:N92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="J93:N93"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="J94:N94"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="I72:K72"/>
-    <mergeCell ref="C77:G77"/>
-    <mergeCell ref="C78:G78"/>
-    <mergeCell ref="J78:N78"/>
-    <mergeCell ref="C79:G79"/>
-    <mergeCell ref="J79:N79"/>
-    <mergeCell ref="C80:G80"/>
-    <mergeCell ref="J80:N80"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="J191:N191"/>
-    <mergeCell ref="J176:N176"/>
-    <mergeCell ref="J177:N177"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="J52:N52"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="I58:K58"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="J107:N107"/>
-    <mergeCell ref="J122:N122"/>
-    <mergeCell ref="C122:G122"/>
-    <mergeCell ref="J175:N175"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C107:G107"/>
-    <mergeCell ref="J190:N190"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="J48:N48"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="J49:N49"/>
-    <mergeCell ref="J62:N62"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="C65:G65"/>
-    <mergeCell ref="J65:N65"/>
-    <mergeCell ref="C66:G66"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="J63:N63"/>
+    <mergeCell ref="C64:G64"/>
+    <mergeCell ref="J64:N64"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
     <mergeCell ref="J10:N10"/>
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="J50:N50"/>
@@ -7737,38 +7578,213 @@
     <mergeCell ref="C38:G38"/>
     <mergeCell ref="J38:N38"/>
     <mergeCell ref="C62:G62"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="C63:G63"/>
-    <mergeCell ref="J63:N63"/>
-    <mergeCell ref="C64:G64"/>
-    <mergeCell ref="J64:N64"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="J52:N52"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="J107:N107"/>
+    <mergeCell ref="J122:N122"/>
+    <mergeCell ref="C122:G122"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C107:G107"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="J48:N48"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="J49:N49"/>
+    <mergeCell ref="J62:N62"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="C65:G65"/>
+    <mergeCell ref="J65:N65"/>
+    <mergeCell ref="C66:G66"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="J76:N76"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="I72:K72"/>
+    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="J78:N78"/>
+    <mergeCell ref="C79:G79"/>
+    <mergeCell ref="J79:N79"/>
+    <mergeCell ref="C80:G80"/>
+    <mergeCell ref="J80:N80"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="J77:N77"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="I86:K86"/>
+    <mergeCell ref="B90:B94"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="J90:N90"/>
+    <mergeCell ref="J91:N91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="J92:N92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="J93:N93"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="J94:N94"/>
+    <mergeCell ref="B100:D100"/>
+    <mergeCell ref="I100:K100"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="J104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="J105:N105"/>
+    <mergeCell ref="J106:N106"/>
+    <mergeCell ref="J108:N108"/>
+    <mergeCell ref="B114:D114"/>
+    <mergeCell ref="I114:K114"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="B118:B122"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="J118:N118"/>
+    <mergeCell ref="C119:G119"/>
+    <mergeCell ref="J119:N119"/>
+    <mergeCell ref="J120:N120"/>
+    <mergeCell ref="C121:G121"/>
+    <mergeCell ref="B128:D128"/>
+    <mergeCell ref="I128:K128"/>
+    <mergeCell ref="C120:G120"/>
+    <mergeCell ref="J121:N121"/>
+    <mergeCell ref="C132:G132"/>
+    <mergeCell ref="J132:N132"/>
+    <mergeCell ref="C133:G133"/>
+    <mergeCell ref="J133:N133"/>
+    <mergeCell ref="C134:G134"/>
+    <mergeCell ref="J134:N134"/>
+    <mergeCell ref="C135:G135"/>
+    <mergeCell ref="J135:N135"/>
+    <mergeCell ref="C136:G136"/>
+    <mergeCell ref="J136:N136"/>
+    <mergeCell ref="B142:D142"/>
+    <mergeCell ref="I142:K142"/>
+    <mergeCell ref="B146:B150"/>
+    <mergeCell ref="C146:G146"/>
+    <mergeCell ref="J146:N146"/>
+    <mergeCell ref="C147:G147"/>
+    <mergeCell ref="J147:N147"/>
+    <mergeCell ref="C148:G148"/>
+    <mergeCell ref="J148:N148"/>
+    <mergeCell ref="C149:G149"/>
+    <mergeCell ref="J149:N149"/>
+    <mergeCell ref="C150:G150"/>
+    <mergeCell ref="J150:N150"/>
+    <mergeCell ref="B156:D156"/>
+    <mergeCell ref="I156:K156"/>
+    <mergeCell ref="C160:G160"/>
+    <mergeCell ref="J160:N160"/>
+    <mergeCell ref="C161:G161"/>
+    <mergeCell ref="J161:N161"/>
+    <mergeCell ref="C162:G162"/>
+    <mergeCell ref="J162:N162"/>
+    <mergeCell ref="C163:G163"/>
+    <mergeCell ref="J163:N163"/>
+    <mergeCell ref="C164:G164"/>
+    <mergeCell ref="J164:N164"/>
+    <mergeCell ref="B170:D170"/>
+    <mergeCell ref="I170:K170"/>
+    <mergeCell ref="B174:B178"/>
+    <mergeCell ref="C175:G175"/>
+    <mergeCell ref="C176:G176"/>
+    <mergeCell ref="C177:G177"/>
+    <mergeCell ref="C178:G178"/>
+    <mergeCell ref="J178:N178"/>
+    <mergeCell ref="J176:N176"/>
+    <mergeCell ref="J177:N177"/>
+    <mergeCell ref="J175:N175"/>
     <mergeCell ref="C174:G174"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="J76:N76"/>
-    <mergeCell ref="C120:G120"/>
-    <mergeCell ref="C108:G108"/>
     <mergeCell ref="J174:N174"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="J77:N77"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="J121:N121"/>
-    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="B184:D184"/>
+    <mergeCell ref="I184:K184"/>
+    <mergeCell ref="C188:G188"/>
+    <mergeCell ref="J188:N188"/>
+    <mergeCell ref="C189:G189"/>
+    <mergeCell ref="C191:G191"/>
+    <mergeCell ref="C192:G192"/>
+    <mergeCell ref="J192:N192"/>
+    <mergeCell ref="B198:D198"/>
+    <mergeCell ref="I198:K198"/>
+    <mergeCell ref="C190:G190"/>
+    <mergeCell ref="J189:N189"/>
+    <mergeCell ref="J191:N191"/>
+    <mergeCell ref="J190:N190"/>
+    <mergeCell ref="B202:B206"/>
+    <mergeCell ref="J202:N202"/>
+    <mergeCell ref="J203:N203"/>
+    <mergeCell ref="J204:N204"/>
+    <mergeCell ref="J205:N205"/>
+    <mergeCell ref="J206:N206"/>
+    <mergeCell ref="B212:D212"/>
+    <mergeCell ref="I212:K212"/>
+    <mergeCell ref="C216:G216"/>
+    <mergeCell ref="J216:N216"/>
+    <mergeCell ref="C204:G204"/>
+    <mergeCell ref="C206:G206"/>
+    <mergeCell ref="C205:G205"/>
+    <mergeCell ref="C202:G202"/>
+    <mergeCell ref="C203:G203"/>
+    <mergeCell ref="C217:G217"/>
+    <mergeCell ref="J217:N217"/>
+    <mergeCell ref="C218:G218"/>
+    <mergeCell ref="J218:N218"/>
+    <mergeCell ref="C219:G219"/>
+    <mergeCell ref="J219:N219"/>
+    <mergeCell ref="C220:G220"/>
+    <mergeCell ref="J220:N220"/>
+    <mergeCell ref="B226:D226"/>
+    <mergeCell ref="I226:K226"/>
+    <mergeCell ref="B230:B234"/>
+    <mergeCell ref="C230:G230"/>
+    <mergeCell ref="J230:N230"/>
+    <mergeCell ref="C231:G231"/>
+    <mergeCell ref="J231:N231"/>
+    <mergeCell ref="C232:G232"/>
+    <mergeCell ref="J232:N232"/>
+    <mergeCell ref="C233:G233"/>
+    <mergeCell ref="J233:N233"/>
+    <mergeCell ref="C234:G234"/>
+    <mergeCell ref="J234:N234"/>
+    <mergeCell ref="B240:D240"/>
+    <mergeCell ref="I240:K240"/>
+    <mergeCell ref="C244:G244"/>
+    <mergeCell ref="J244:N244"/>
+    <mergeCell ref="C245:G245"/>
+    <mergeCell ref="J245:N245"/>
+    <mergeCell ref="C246:G246"/>
+    <mergeCell ref="J246:N246"/>
+    <mergeCell ref="C247:G247"/>
+    <mergeCell ref="J247:N247"/>
+    <mergeCell ref="C248:G248"/>
+    <mergeCell ref="J248:N248"/>
+    <mergeCell ref="B254:D254"/>
+    <mergeCell ref="I254:K254"/>
+    <mergeCell ref="B258:B262"/>
+    <mergeCell ref="C258:G258"/>
+    <mergeCell ref="J258:N258"/>
+    <mergeCell ref="C259:G259"/>
+    <mergeCell ref="J259:N259"/>
+    <mergeCell ref="C260:G260"/>
+    <mergeCell ref="J260:N260"/>
+    <mergeCell ref="C261:G261"/>
+    <mergeCell ref="J261:N261"/>
+    <mergeCell ref="C262:G262"/>
+    <mergeCell ref="J262:N262"/>
+    <mergeCell ref="C276:G276"/>
+    <mergeCell ref="J276:N276"/>
+    <mergeCell ref="B282:D282"/>
+    <mergeCell ref="I282:K282"/>
+    <mergeCell ref="B268:D268"/>
+    <mergeCell ref="I268:K268"/>
+    <mergeCell ref="C272:G272"/>
+    <mergeCell ref="J272:N272"/>
+    <mergeCell ref="C273:G273"/>
+    <mergeCell ref="J273:N273"/>
+    <mergeCell ref="C274:G274"/>
+    <mergeCell ref="J274:N274"/>
+    <mergeCell ref="C275:G275"/>
+    <mergeCell ref="J275:N275"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert ":adhesive_bandage: CORRIGINDO ARQUIVO CORROMPIDO"
This reverts commit 8d39024d7029cb5317287b21e643c693cb9399d0.
</commit_message>
<xml_diff>
--- a/ModeloCarteirinha.xlsx
+++ b/ModeloCarteirinha.xlsx
@@ -213,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -234,25 +234,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2449,21 +2448,21 @@
   <dimension ref="A5:O284"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="5.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="3" style="2" customWidth="1"/>
     <col min="9" max="9" width="10.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" style="2" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" customWidth="1"/>
     <col min="13" max="13" width="12.42578125" style="2" customWidth="1"/>
     <col min="14" max="14" width="8" style="2" customWidth="1"/>
@@ -2473,98 +2472,98 @@
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
-      <c r="C6" s="17" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="22"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="19"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="22"/>
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="27"/>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="22"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="18"/>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="27"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="22"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="18"/>
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="27"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
       <c r="I9" s="7"/>
       <c r="J9" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="22"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="18"/>
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="27"/>
-      <c r="C10" s="25" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="22"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="18"/>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2606,14 +2605,12 @@
       <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="16"/>
       <c r="D14"/>
       <c r="F14" s="3"/>
       <c r="G14" s="8"/>
       <c r="I14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J14" s="16"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="3"/>
@@ -2632,18 +2629,18 @@
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
       <c r="F16" s="4"/>
       <c r="G16" s="8"/>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
       <c r="L16" s="2"/>
       <c r="M16" s="4"/>
       <c r="N16" s="8"/>
@@ -2680,59 +2677,59 @@
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="22"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="17" t="s">
+      <c r="J20" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="19"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="22"/>
       <c r="O20" s="2"/>
     </row>
     <row r="21" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="20" t="s">
+      <c r="J21" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="22"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="18"/>
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="18"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="22"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="18"/>
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
@@ -2740,37 +2737,37 @@
       <c r="C23" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18"/>
       <c r="I23" s="7"/>
       <c r="J23" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="22"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="18"/>
       <c r="O23" s="2"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="22"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="18"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="25" t="s">
+      <c r="J24" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="22"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="18"/>
       <c r="O24" s="2"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -2840,18 +2837,18 @@
       <c r="O29" s="2"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
       <c r="F30" s="4"/>
       <c r="G30" s="8"/>
-      <c r="I30" s="23" t="s">
+      <c r="I30" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
       <c r="L30" s="2"/>
       <c r="M30" s="4"/>
       <c r="N30" s="8"/>
@@ -2887,103 +2884,103 @@
       <c r="O33" s="2"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="26"/>
-      <c r="C34" s="17" t="s">
+      <c r="B34" s="25"/>
+      <c r="C34" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="22"/>
       <c r="H34" s="14"/>
       <c r="I34" s="6"/>
-      <c r="J34" s="17" t="s">
+      <c r="J34" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="19"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="22"/>
       <c r="O34" s="2"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="27"/>
-      <c r="C35" s="20" t="s">
+      <c r="B35" s="26"/>
+      <c r="C35" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="22"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="18"/>
       <c r="H35" s="14"/>
       <c r="I35" s="7"/>
-      <c r="J35" s="20" t="s">
+      <c r="J35" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="22"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="18"/>
       <c r="O35" s="2"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="27"/>
-      <c r="C36" s="20" t="s">
+      <c r="B36" s="26"/>
+      <c r="C36" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="22"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="18"/>
       <c r="H36" s="14"/>
       <c r="I36" s="7"/>
-      <c r="J36" s="20" t="s">
+      <c r="J36" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="21"/>
-      <c r="N36" s="22"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="18"/>
       <c r="O36" s="2"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="27"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="22"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="18"/>
       <c r="H37" s="14"/>
       <c r="I37" s="7"/>
       <c r="J37" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="21"/>
-      <c r="N37" s="22"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="18"/>
       <c r="O37" s="2"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="27"/>
-      <c r="C38" s="25" t="s">
+      <c r="B38" s="26"/>
+      <c r="C38" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="22"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="18"/>
       <c r="H38" s="14"/>
       <c r="I38" s="7"/>
-      <c r="J38" s="25" t="s">
+      <c r="J38" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K38" s="21"/>
-      <c r="L38" s="21"/>
-      <c r="M38" s="21"/>
-      <c r="N38" s="22"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="18"/>
       <c r="O38" s="2"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
@@ -3083,20 +3080,20 @@
       <c r="O43" s="2"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
       <c r="E44" s="14"/>
       <c r="F44" s="4"/>
       <c r="G44" s="15"/>
       <c r="H44" s="14"/>
-      <c r="I44" s="23" t="s">
+      <c r="I44" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
       <c r="L44" s="14"/>
       <c r="M44" s="4"/>
       <c r="N44" s="15"/>
@@ -3152,62 +3149,62 @@
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="19"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="22"/>
       <c r="H48" s="14"/>
       <c r="I48" s="6"/>
-      <c r="J48" s="17" t="s">
+      <c r="J48" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="19"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="22"/>
       <c r="O48" s="2"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="20" t="s">
+      <c r="C49" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="22"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="18"/>
       <c r="H49" s="14"/>
       <c r="I49" s="7"/>
-      <c r="J49" s="20" t="s">
+      <c r="J49" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K49" s="21"/>
-      <c r="L49" s="21"/>
-      <c r="M49" s="21"/>
-      <c r="N49" s="22"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="18"/>
       <c r="O49" s="2"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="20" t="s">
+      <c r="C50" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="22"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="18"/>
       <c r="H50" s="14"/>
       <c r="I50" s="7"/>
-      <c r="J50" s="20" t="s">
+      <c r="J50" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K50" s="21"/>
-      <c r="L50" s="21"/>
-      <c r="M50" s="21"/>
-      <c r="N50" s="22"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="18"/>
       <c r="O50" s="2"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
@@ -3215,39 +3212,39 @@
       <c r="C51" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="22"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="18"/>
       <c r="H51" s="14"/>
       <c r="I51" s="7"/>
       <c r="J51" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K51" s="21"/>
-      <c r="L51" s="21"/>
-      <c r="M51" s="21"/>
-      <c r="N51" s="22"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="18"/>
       <c r="O51" s="2"/>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
-      <c r="C52" s="25" t="s">
+      <c r="C52" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="22"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="18"/>
       <c r="H52" s="14"/>
       <c r="I52" s="7"/>
-      <c r="J52" s="25" t="s">
+      <c r="J52" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K52" s="21"/>
-      <c r="L52" s="21"/>
-      <c r="M52" s="21"/>
-      <c r="N52" s="22"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="17"/>
+      <c r="N52" s="18"/>
       <c r="O52" s="2"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
@@ -3347,20 +3344,20 @@
       <c r="O57" s="2"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="23" t="s">
+      <c r="B58" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
       <c r="E58" s="14"/>
       <c r="F58" s="4"/>
       <c r="G58" s="15"/>
       <c r="H58" s="14"/>
-      <c r="I58" s="23" t="s">
+      <c r="I58" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J58" s="18"/>
-      <c r="K58" s="18"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="20"/>
       <c r="L58" s="14"/>
       <c r="M58" s="4"/>
       <c r="N58" s="15"/>
@@ -3402,103 +3399,103 @@
       <c r="O61" s="2"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="26"/>
-      <c r="C62" s="17" t="s">
+      <c r="B62" s="25"/>
+      <c r="C62" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="19"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="22"/>
       <c r="H62" s="14"/>
       <c r="I62" s="6"/>
-      <c r="J62" s="17" t="s">
+      <c r="J62" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K62" s="18"/>
-      <c r="L62" s="18"/>
-      <c r="M62" s="18"/>
-      <c r="N62" s="19"/>
+      <c r="K62" s="20"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="22"/>
       <c r="O62" s="2"/>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="27"/>
-      <c r="C63" s="20" t="s">
+      <c r="B63" s="26"/>
+      <c r="C63" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D63" s="21"/>
-      <c r="E63" s="21"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="22"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="18"/>
       <c r="H63" s="14"/>
       <c r="I63" s="7"/>
-      <c r="J63" s="20" t="s">
+      <c r="J63" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K63" s="21"/>
-      <c r="L63" s="21"/>
-      <c r="M63" s="21"/>
-      <c r="N63" s="22"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="18"/>
       <c r="O63" s="2"/>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="27"/>
-      <c r="C64" s="20" t="s">
+      <c r="B64" s="26"/>
+      <c r="C64" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D64" s="21"/>
-      <c r="E64" s="21"/>
-      <c r="F64" s="21"/>
-      <c r="G64" s="22"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="18"/>
       <c r="H64" s="14"/>
       <c r="I64" s="7"/>
-      <c r="J64" s="20" t="s">
+      <c r="J64" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K64" s="21"/>
-      <c r="L64" s="21"/>
-      <c r="M64" s="21"/>
-      <c r="N64" s="22"/>
+      <c r="K64" s="17"/>
+      <c r="L64" s="17"/>
+      <c r="M64" s="17"/>
+      <c r="N64" s="18"/>
       <c r="O64" s="2"/>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="27"/>
+      <c r="B65" s="26"/>
       <c r="C65" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="21"/>
-      <c r="E65" s="21"/>
-      <c r="F65" s="21"/>
-      <c r="G65" s="22"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="18"/>
       <c r="H65" s="14"/>
       <c r="I65" s="7"/>
       <c r="J65" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K65" s="21"/>
-      <c r="L65" s="21"/>
-      <c r="M65" s="21"/>
-      <c r="N65" s="22"/>
+      <c r="K65" s="17"/>
+      <c r="L65" s="17"/>
+      <c r="M65" s="17"/>
+      <c r="N65" s="18"/>
       <c r="O65" s="2"/>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="27"/>
-      <c r="C66" s="25" t="s">
+      <c r="B66" s="26"/>
+      <c r="C66" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="21"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="22"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="18"/>
       <c r="H66" s="14"/>
       <c r="I66" s="7"/>
-      <c r="J66" s="25" t="s">
+      <c r="J66" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K66" s="21"/>
-      <c r="L66" s="21"/>
-      <c r="M66" s="21"/>
-      <c r="N66" s="22"/>
+      <c r="K66" s="17"/>
+      <c r="L66" s="17"/>
+      <c r="M66" s="17"/>
+      <c r="N66" s="18"/>
       <c r="O66" s="2"/>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
@@ -3598,20 +3595,20 @@
       <c r="O71" s="2"/>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="23" t="s">
+      <c r="B72" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="20"/>
       <c r="E72" s="14"/>
       <c r="F72" s="4"/>
       <c r="G72" s="15"/>
       <c r="H72" s="14"/>
-      <c r="I72" s="23" t="s">
+      <c r="I72" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J72" s="18"/>
-      <c r="K72" s="18"/>
+      <c r="J72" s="20"/>
+      <c r="K72" s="20"/>
       <c r="L72" s="14"/>
       <c r="M72" s="4"/>
       <c r="N72" s="15"/>
@@ -3667,62 +3664,62 @@
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
-      <c r="C76" s="17" t="s">
+      <c r="C76" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D76" s="18"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="19"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="22"/>
       <c r="H76" s="14"/>
       <c r="I76" s="6"/>
-      <c r="J76" s="17" t="s">
+      <c r="J76" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K76" s="18"/>
-      <c r="L76" s="18"/>
-      <c r="M76" s="18"/>
-      <c r="N76" s="19"/>
+      <c r="K76" s="20"/>
+      <c r="L76" s="20"/>
+      <c r="M76" s="20"/>
+      <c r="N76" s="22"/>
       <c r="O76" s="2"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B77" s="7"/>
-      <c r="C77" s="20" t="s">
+      <c r="C77" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D77" s="21"/>
-      <c r="E77" s="21"/>
-      <c r="F77" s="21"/>
-      <c r="G77" s="22"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="18"/>
       <c r="H77" s="14"/>
       <c r="I77" s="7"/>
-      <c r="J77" s="20" t="s">
+      <c r="J77" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K77" s="21"/>
-      <c r="L77" s="21"/>
-      <c r="M77" s="21"/>
-      <c r="N77" s="22"/>
+      <c r="K77" s="17"/>
+      <c r="L77" s="17"/>
+      <c r="M77" s="17"/>
+      <c r="N77" s="18"/>
       <c r="O77" s="2"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B78" s="7"/>
-      <c r="C78" s="20" t="s">
+      <c r="C78" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D78" s="21"/>
-      <c r="E78" s="21"/>
-      <c r="F78" s="21"/>
-      <c r="G78" s="22"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="18"/>
       <c r="H78" s="14"/>
       <c r="I78" s="7"/>
-      <c r="J78" s="20" t="s">
+      <c r="J78" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K78" s="21"/>
-      <c r="L78" s="21"/>
-      <c r="M78" s="21"/>
-      <c r="N78" s="22"/>
+      <c r="K78" s="17"/>
+      <c r="L78" s="17"/>
+      <c r="M78" s="17"/>
+      <c r="N78" s="18"/>
       <c r="O78" s="2"/>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
@@ -3730,39 +3727,39 @@
       <c r="C79" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D79" s="21"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="21"/>
-      <c r="G79" s="22"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="18"/>
       <c r="H79" s="14"/>
       <c r="I79" s="7"/>
       <c r="J79" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K79" s="21"/>
-      <c r="L79" s="21"/>
-      <c r="M79" s="21"/>
-      <c r="N79" s="22"/>
+      <c r="K79" s="17"/>
+      <c r="L79" s="17"/>
+      <c r="M79" s="17"/>
+      <c r="N79" s="18"/>
       <c r="O79" s="2"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B80" s="7"/>
-      <c r="C80" s="25" t="s">
+      <c r="C80" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D80" s="21"/>
-      <c r="E80" s="21"/>
-      <c r="F80" s="21"/>
-      <c r="G80" s="22"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="18"/>
       <c r="H80" s="14"/>
       <c r="I80" s="7"/>
-      <c r="J80" s="25" t="s">
+      <c r="J80" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K80" s="21"/>
-      <c r="L80" s="21"/>
-      <c r="M80" s="21"/>
-      <c r="N80" s="22"/>
+      <c r="K80" s="17"/>
+      <c r="L80" s="17"/>
+      <c r="M80" s="17"/>
+      <c r="N80" s="18"/>
       <c r="O80" s="2"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
@@ -3862,20 +3859,20 @@
       <c r="O85" s="2"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B86" s="23" t="s">
+      <c r="B86" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C86" s="18"/>
-      <c r="D86" s="18"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="20"/>
       <c r="E86" s="14"/>
       <c r="F86" s="4"/>
       <c r="G86" s="15"/>
       <c r="H86" s="14"/>
-      <c r="I86" s="23" t="s">
+      <c r="I86" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J86" s="18"/>
-      <c r="K86" s="18"/>
+      <c r="J86" s="20"/>
+      <c r="K86" s="20"/>
       <c r="L86" s="14"/>
       <c r="M86" s="4"/>
       <c r="N86" s="15"/>
@@ -3917,103 +3914,103 @@
       <c r="O89" s="2"/>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B90" s="26"/>
-      <c r="C90" s="17" t="s">
+      <c r="B90" s="25"/>
+      <c r="C90" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="18"/>
-      <c r="G90" s="19"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="20"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="22"/>
       <c r="H90" s="14"/>
       <c r="I90" s="6"/>
-      <c r="J90" s="17" t="s">
+      <c r="J90" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K90" s="18"/>
-      <c r="L90" s="18"/>
-      <c r="M90" s="18"/>
-      <c r="N90" s="19"/>
+      <c r="K90" s="20"/>
+      <c r="L90" s="20"/>
+      <c r="M90" s="20"/>
+      <c r="N90" s="22"/>
       <c r="O90" s="2"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B91" s="27"/>
-      <c r="C91" s="20" t="s">
+      <c r="B91" s="26"/>
+      <c r="C91" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D91" s="21"/>
-      <c r="E91" s="21"/>
-      <c r="F91" s="21"/>
-      <c r="G91" s="22"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="17"/>
+      <c r="F91" s="17"/>
+      <c r="G91" s="18"/>
       <c r="H91" s="14"/>
       <c r="I91" s="7"/>
-      <c r="J91" s="20" t="s">
+      <c r="J91" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K91" s="21"/>
-      <c r="L91" s="21"/>
-      <c r="M91" s="21"/>
-      <c r="N91" s="22"/>
+      <c r="K91" s="17"/>
+      <c r="L91" s="17"/>
+      <c r="M91" s="17"/>
+      <c r="N91" s="18"/>
       <c r="O91" s="2"/>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B92" s="27"/>
-      <c r="C92" s="20" t="s">
+      <c r="B92" s="26"/>
+      <c r="C92" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D92" s="21"/>
-      <c r="E92" s="21"/>
-      <c r="F92" s="21"/>
-      <c r="G92" s="22"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="18"/>
       <c r="H92" s="14"/>
       <c r="I92" s="7"/>
-      <c r="J92" s="20" t="s">
+      <c r="J92" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K92" s="21"/>
-      <c r="L92" s="21"/>
-      <c r="M92" s="21"/>
-      <c r="N92" s="22"/>
+      <c r="K92" s="17"/>
+      <c r="L92" s="17"/>
+      <c r="M92" s="17"/>
+      <c r="N92" s="18"/>
       <c r="O92" s="2"/>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B93" s="27"/>
+      <c r="B93" s="26"/>
       <c r="C93" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D93" s="21"/>
-      <c r="E93" s="21"/>
-      <c r="F93" s="21"/>
-      <c r="G93" s="22"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="17"/>
+      <c r="F93" s="17"/>
+      <c r="G93" s="18"/>
       <c r="H93" s="14"/>
       <c r="I93" s="7"/>
       <c r="J93" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K93" s="21"/>
-      <c r="L93" s="21"/>
-      <c r="M93" s="21"/>
-      <c r="N93" s="22"/>
+      <c r="K93" s="17"/>
+      <c r="L93" s="17"/>
+      <c r="M93" s="17"/>
+      <c r="N93" s="18"/>
       <c r="O93" s="2"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B94" s="27"/>
-      <c r="C94" s="25" t="s">
+      <c r="B94" s="26"/>
+      <c r="C94" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D94" s="21"/>
-      <c r="E94" s="21"/>
-      <c r="F94" s="21"/>
-      <c r="G94" s="22"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="17"/>
+      <c r="F94" s="17"/>
+      <c r="G94" s="18"/>
       <c r="H94" s="14"/>
       <c r="I94" s="7"/>
-      <c r="J94" s="25" t="s">
+      <c r="J94" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K94" s="21"/>
-      <c r="L94" s="21"/>
-      <c r="M94" s="21"/>
-      <c r="N94" s="22"/>
+      <c r="K94" s="17"/>
+      <c r="L94" s="17"/>
+      <c r="M94" s="17"/>
+      <c r="N94" s="18"/>
       <c r="O94" s="2"/>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
@@ -4113,20 +4110,20 @@
       <c r="O99" s="2"/>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B100" s="23" t="s">
+      <c r="B100" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C100" s="18"/>
-      <c r="D100" s="18"/>
+      <c r="C100" s="20"/>
+      <c r="D100" s="20"/>
       <c r="E100" s="14"/>
       <c r="F100" s="4"/>
       <c r="G100" s="15"/>
       <c r="H100" s="14"/>
-      <c r="I100" s="23" t="s">
+      <c r="I100" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J100" s="18"/>
-      <c r="K100" s="18"/>
+      <c r="J100" s="20"/>
+      <c r="K100" s="20"/>
       <c r="L100" s="14"/>
       <c r="M100" s="4"/>
       <c r="N100" s="15"/>
@@ -4182,62 +4179,62 @@
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104" s="6"/>
-      <c r="C104" s="17" t="s">
+      <c r="C104" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D104" s="18"/>
-      <c r="E104" s="18"/>
-      <c r="F104" s="18"/>
-      <c r="G104" s="19"/>
+      <c r="D104" s="20"/>
+      <c r="E104" s="20"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="22"/>
       <c r="H104" s="14"/>
       <c r="I104" s="6"/>
-      <c r="J104" s="17" t="s">
+      <c r="J104" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K104" s="18"/>
-      <c r="L104" s="18"/>
-      <c r="M104" s="18"/>
-      <c r="N104" s="19"/>
+      <c r="K104" s="20"/>
+      <c r="L104" s="20"/>
+      <c r="M104" s="20"/>
+      <c r="N104" s="22"/>
       <c r="O104" s="2"/>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B105" s="7"/>
-      <c r="C105" s="20" t="s">
+      <c r="C105" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D105" s="21"/>
-      <c r="E105" s="21"/>
-      <c r="F105" s="21"/>
-      <c r="G105" s="22"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="17"/>
+      <c r="F105" s="17"/>
+      <c r="G105" s="18"/>
       <c r="H105" s="14"/>
       <c r="I105" s="7"/>
-      <c r="J105" s="20" t="s">
+      <c r="J105" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K105" s="21"/>
-      <c r="L105" s="21"/>
-      <c r="M105" s="21"/>
-      <c r="N105" s="22"/>
+      <c r="K105" s="17"/>
+      <c r="L105" s="17"/>
+      <c r="M105" s="17"/>
+      <c r="N105" s="18"/>
       <c r="O105" s="2"/>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106" s="7"/>
-      <c r="C106" s="20" t="s">
+      <c r="C106" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D106" s="21"/>
-      <c r="E106" s="21"/>
-      <c r="F106" s="21"/>
-      <c r="G106" s="22"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="17"/>
+      <c r="G106" s="18"/>
       <c r="H106" s="14"/>
       <c r="I106" s="7"/>
-      <c r="J106" s="20" t="s">
+      <c r="J106" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K106" s="21"/>
-      <c r="L106" s="21"/>
-      <c r="M106" s="21"/>
-      <c r="N106" s="22"/>
+      <c r="K106" s="17"/>
+      <c r="L106" s="17"/>
+      <c r="M106" s="17"/>
+      <c r="N106" s="18"/>
       <c r="O106" s="2"/>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
@@ -4245,39 +4242,39 @@
       <c r="C107" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D107" s="21"/>
-      <c r="E107" s="21"/>
-      <c r="F107" s="21"/>
-      <c r="G107" s="22"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
+      <c r="F107" s="17"/>
+      <c r="G107" s="18"/>
       <c r="H107" s="14"/>
       <c r="I107" s="7"/>
       <c r="J107" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K107" s="21"/>
-      <c r="L107" s="21"/>
-      <c r="M107" s="21"/>
-      <c r="N107" s="22"/>
+      <c r="K107" s="17"/>
+      <c r="L107" s="17"/>
+      <c r="M107" s="17"/>
+      <c r="N107" s="18"/>
       <c r="O107" s="2"/>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B108" s="7"/>
-      <c r="C108" s="25" t="s">
+      <c r="C108" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D108" s="21"/>
-      <c r="E108" s="21"/>
-      <c r="F108" s="21"/>
-      <c r="G108" s="22"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="17"/>
+      <c r="F108" s="17"/>
+      <c r="G108" s="18"/>
       <c r="H108" s="14"/>
       <c r="I108" s="7"/>
-      <c r="J108" s="25" t="s">
+      <c r="J108" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K108" s="21"/>
-      <c r="L108" s="21"/>
-      <c r="M108" s="21"/>
-      <c r="N108" s="22"/>
+      <c r="K108" s="17"/>
+      <c r="L108" s="17"/>
+      <c r="M108" s="17"/>
+      <c r="N108" s="18"/>
       <c r="O108" s="2"/>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.25">
@@ -4377,20 +4374,20 @@
       <c r="O113" s="2"/>
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B114" s="23" t="s">
+      <c r="B114" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C114" s="18"/>
-      <c r="D114" s="18"/>
+      <c r="C114" s="20"/>
+      <c r="D114" s="20"/>
       <c r="E114" s="14"/>
       <c r="F114" s="4"/>
       <c r="G114" s="15"/>
       <c r="H114" s="14"/>
-      <c r="I114" s="23" t="s">
+      <c r="I114" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J114" s="18"/>
-      <c r="K114" s="18"/>
+      <c r="J114" s="20"/>
+      <c r="K114" s="20"/>
       <c r="L114" s="14"/>
       <c r="M114" s="4"/>
       <c r="N114" s="15"/>
@@ -4432,103 +4429,103 @@
       <c r="O117" s="2"/>
     </row>
     <row r="118" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B118" s="26"/>
-      <c r="C118" s="17" t="s">
+      <c r="B118" s="25"/>
+      <c r="C118" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D118" s="18"/>
-      <c r="E118" s="18"/>
-      <c r="F118" s="18"/>
-      <c r="G118" s="19"/>
+      <c r="D118" s="20"/>
+      <c r="E118" s="20"/>
+      <c r="F118" s="20"/>
+      <c r="G118" s="22"/>
       <c r="H118" s="14"/>
       <c r="I118" s="6"/>
-      <c r="J118" s="17" t="s">
+      <c r="J118" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K118" s="18"/>
-      <c r="L118" s="18"/>
-      <c r="M118" s="18"/>
-      <c r="N118" s="19"/>
+      <c r="K118" s="20"/>
+      <c r="L118" s="20"/>
+      <c r="M118" s="20"/>
+      <c r="N118" s="22"/>
       <c r="O118" s="2"/>
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B119" s="27"/>
-      <c r="C119" s="20" t="s">
+      <c r="B119" s="26"/>
+      <c r="C119" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D119" s="21"/>
-      <c r="E119" s="21"/>
-      <c r="F119" s="21"/>
-      <c r="G119" s="22"/>
+      <c r="D119" s="17"/>
+      <c r="E119" s="17"/>
+      <c r="F119" s="17"/>
+      <c r="G119" s="18"/>
       <c r="H119" s="14"/>
       <c r="I119" s="7"/>
-      <c r="J119" s="20" t="s">
+      <c r="J119" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K119" s="21"/>
-      <c r="L119" s="21"/>
-      <c r="M119" s="21"/>
-      <c r="N119" s="22"/>
+      <c r="K119" s="17"/>
+      <c r="L119" s="17"/>
+      <c r="M119" s="17"/>
+      <c r="N119" s="18"/>
       <c r="O119" s="2"/>
     </row>
     <row r="120" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B120" s="27"/>
-      <c r="C120" s="20" t="s">
+      <c r="B120" s="26"/>
+      <c r="C120" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D120" s="21"/>
-      <c r="E120" s="21"/>
-      <c r="F120" s="21"/>
-      <c r="G120" s="22"/>
+      <c r="D120" s="17"/>
+      <c r="E120" s="17"/>
+      <c r="F120" s="17"/>
+      <c r="G120" s="18"/>
       <c r="H120" s="14"/>
       <c r="I120" s="7"/>
-      <c r="J120" s="20" t="s">
+      <c r="J120" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K120" s="21"/>
-      <c r="L120" s="21"/>
-      <c r="M120" s="21"/>
-      <c r="N120" s="22"/>
+      <c r="K120" s="17"/>
+      <c r="L120" s="17"/>
+      <c r="M120" s="17"/>
+      <c r="N120" s="18"/>
       <c r="O120" s="2"/>
     </row>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B121" s="27"/>
+      <c r="B121" s="26"/>
       <c r="C121" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D121" s="21"/>
-      <c r="E121" s="21"/>
-      <c r="F121" s="21"/>
-      <c r="G121" s="22"/>
+      <c r="D121" s="17"/>
+      <c r="E121" s="17"/>
+      <c r="F121" s="17"/>
+      <c r="G121" s="18"/>
       <c r="H121" s="14"/>
       <c r="I121" s="7"/>
       <c r="J121" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K121" s="21"/>
-      <c r="L121" s="21"/>
-      <c r="M121" s="21"/>
-      <c r="N121" s="22"/>
+      <c r="K121" s="17"/>
+      <c r="L121" s="17"/>
+      <c r="M121" s="17"/>
+      <c r="N121" s="18"/>
       <c r="O121" s="2"/>
     </row>
     <row r="122" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B122" s="27"/>
-      <c r="C122" s="25" t="s">
+      <c r="B122" s="26"/>
+      <c r="C122" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D122" s="21"/>
-      <c r="E122" s="21"/>
-      <c r="F122" s="21"/>
-      <c r="G122" s="22"/>
+      <c r="D122" s="17"/>
+      <c r="E122" s="17"/>
+      <c r="F122" s="17"/>
+      <c r="G122" s="18"/>
       <c r="H122" s="14"/>
       <c r="I122" s="7"/>
-      <c r="J122" s="25" t="s">
+      <c r="J122" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K122" s="21"/>
-      <c r="L122" s="21"/>
-      <c r="M122" s="21"/>
-      <c r="N122" s="22"/>
+      <c r="K122" s="17"/>
+      <c r="L122" s="17"/>
+      <c r="M122" s="17"/>
+      <c r="N122" s="18"/>
       <c r="O122" s="2"/>
     </row>
     <row r="123" spans="2:15" x14ac:dyDescent="0.25">
@@ -4628,20 +4625,20 @@
       <c r="O127" s="2"/>
     </row>
     <row r="128" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B128" s="23" t="s">
+      <c r="B128" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C128" s="18"/>
-      <c r="D128" s="18"/>
+      <c r="C128" s="20"/>
+      <c r="D128" s="20"/>
       <c r="E128" s="14"/>
       <c r="F128" s="4"/>
       <c r="G128" s="15"/>
       <c r="H128" s="14"/>
-      <c r="I128" s="23" t="s">
+      <c r="I128" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J128" s="18"/>
-      <c r="K128" s="18"/>
+      <c r="J128" s="20"/>
+      <c r="K128" s="20"/>
       <c r="L128" s="14"/>
       <c r="M128" s="4"/>
       <c r="N128" s="15"/>
@@ -4697,62 +4694,62 @@
     </row>
     <row r="132" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
-      <c r="C132" s="17" t="s">
+      <c r="C132" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D132" s="18"/>
-      <c r="E132" s="18"/>
-      <c r="F132" s="18"/>
-      <c r="G132" s="19"/>
+      <c r="D132" s="20"/>
+      <c r="E132" s="20"/>
+      <c r="F132" s="20"/>
+      <c r="G132" s="22"/>
       <c r="H132" s="14"/>
       <c r="I132" s="6"/>
-      <c r="J132" s="17" t="s">
+      <c r="J132" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K132" s="18"/>
-      <c r="L132" s="18"/>
-      <c r="M132" s="18"/>
-      <c r="N132" s="19"/>
+      <c r="K132" s="20"/>
+      <c r="L132" s="20"/>
+      <c r="M132" s="20"/>
+      <c r="N132" s="22"/>
       <c r="O132" s="2"/>
     </row>
     <row r="133" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B133" s="7"/>
-      <c r="C133" s="20" t="s">
+      <c r="C133" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D133" s="21"/>
-      <c r="E133" s="21"/>
-      <c r="F133" s="21"/>
-      <c r="G133" s="22"/>
+      <c r="D133" s="17"/>
+      <c r="E133" s="17"/>
+      <c r="F133" s="17"/>
+      <c r="G133" s="18"/>
       <c r="H133" s="14"/>
       <c r="I133" s="7"/>
-      <c r="J133" s="20" t="s">
+      <c r="J133" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K133" s="21"/>
-      <c r="L133" s="21"/>
-      <c r="M133" s="21"/>
-      <c r="N133" s="22"/>
+      <c r="K133" s="17"/>
+      <c r="L133" s="17"/>
+      <c r="M133" s="17"/>
+      <c r="N133" s="18"/>
       <c r="O133" s="2"/>
     </row>
     <row r="134" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B134" s="7"/>
-      <c r="C134" s="20" t="s">
+      <c r="C134" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D134" s="21"/>
-      <c r="E134" s="21"/>
-      <c r="F134" s="21"/>
-      <c r="G134" s="22"/>
+      <c r="D134" s="17"/>
+      <c r="E134" s="17"/>
+      <c r="F134" s="17"/>
+      <c r="G134" s="18"/>
       <c r="H134" s="14"/>
       <c r="I134" s="7"/>
-      <c r="J134" s="20" t="s">
+      <c r="J134" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K134" s="21"/>
-      <c r="L134" s="21"/>
-      <c r="M134" s="21"/>
-      <c r="N134" s="22"/>
+      <c r="K134" s="17"/>
+      <c r="L134" s="17"/>
+      <c r="M134" s="17"/>
+      <c r="N134" s="18"/>
       <c r="O134" s="2"/>
     </row>
     <row r="135" spans="2:15" x14ac:dyDescent="0.25">
@@ -4760,39 +4757,39 @@
       <c r="C135" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D135" s="21"/>
-      <c r="E135" s="21"/>
-      <c r="F135" s="21"/>
-      <c r="G135" s="22"/>
+      <c r="D135" s="17"/>
+      <c r="E135" s="17"/>
+      <c r="F135" s="17"/>
+      <c r="G135" s="18"/>
       <c r="H135" s="14"/>
       <c r="I135" s="7"/>
       <c r="J135" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K135" s="21"/>
-      <c r="L135" s="21"/>
-      <c r="M135" s="21"/>
-      <c r="N135" s="22"/>
+      <c r="K135" s="17"/>
+      <c r="L135" s="17"/>
+      <c r="M135" s="17"/>
+      <c r="N135" s="18"/>
       <c r="O135" s="2"/>
     </row>
     <row r="136" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B136" s="7"/>
-      <c r="C136" s="25" t="s">
+      <c r="C136" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D136" s="21"/>
-      <c r="E136" s="21"/>
-      <c r="F136" s="21"/>
-      <c r="G136" s="22"/>
+      <c r="D136" s="17"/>
+      <c r="E136" s="17"/>
+      <c r="F136" s="17"/>
+      <c r="G136" s="18"/>
       <c r="H136" s="14"/>
       <c r="I136" s="7"/>
-      <c r="J136" s="25" t="s">
+      <c r="J136" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K136" s="21"/>
-      <c r="L136" s="21"/>
-      <c r="M136" s="21"/>
-      <c r="N136" s="22"/>
+      <c r="K136" s="17"/>
+      <c r="L136" s="17"/>
+      <c r="M136" s="17"/>
+      <c r="N136" s="18"/>
       <c r="O136" s="2"/>
     </row>
     <row r="137" spans="2:15" x14ac:dyDescent="0.25">
@@ -4892,20 +4889,20 @@
       <c r="O141" s="2"/>
     </row>
     <row r="142" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B142" s="23" t="s">
+      <c r="B142" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C142" s="18"/>
-      <c r="D142" s="18"/>
+      <c r="C142" s="20"/>
+      <c r="D142" s="20"/>
       <c r="E142" s="14"/>
       <c r="F142" s="4"/>
       <c r="G142" s="15"/>
       <c r="H142" s="14"/>
-      <c r="I142" s="23" t="s">
+      <c r="I142" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J142" s="18"/>
-      <c r="K142" s="18"/>
+      <c r="J142" s="20"/>
+      <c r="K142" s="20"/>
       <c r="L142" s="14"/>
       <c r="M142" s="4"/>
       <c r="N142" s="15"/>
@@ -4947,103 +4944,103 @@
       <c r="O145" s="2"/>
     </row>
     <row r="146" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B146" s="26"/>
-      <c r="C146" s="17" t="s">
+      <c r="B146" s="25"/>
+      <c r="C146" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D146" s="18"/>
-      <c r="E146" s="18"/>
-      <c r="F146" s="18"/>
-      <c r="G146" s="19"/>
+      <c r="D146" s="20"/>
+      <c r="E146" s="20"/>
+      <c r="F146" s="20"/>
+      <c r="G146" s="22"/>
       <c r="H146" s="14"/>
       <c r="I146" s="6"/>
-      <c r="J146" s="17" t="s">
+      <c r="J146" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K146" s="18"/>
-      <c r="L146" s="18"/>
-      <c r="M146" s="18"/>
-      <c r="N146" s="19"/>
+      <c r="K146" s="20"/>
+      <c r="L146" s="20"/>
+      <c r="M146" s="20"/>
+      <c r="N146" s="22"/>
       <c r="O146" s="2"/>
     </row>
     <row r="147" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B147" s="27"/>
-      <c r="C147" s="20" t="s">
+      <c r="B147" s="26"/>
+      <c r="C147" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D147" s="21"/>
-      <c r="E147" s="21"/>
-      <c r="F147" s="21"/>
-      <c r="G147" s="22"/>
+      <c r="D147" s="17"/>
+      <c r="E147" s="17"/>
+      <c r="F147" s="17"/>
+      <c r="G147" s="18"/>
       <c r="H147" s="14"/>
       <c r="I147" s="7"/>
-      <c r="J147" s="20" t="s">
+      <c r="J147" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K147" s="21"/>
-      <c r="L147" s="21"/>
-      <c r="M147" s="21"/>
-      <c r="N147" s="22"/>
+      <c r="K147" s="17"/>
+      <c r="L147" s="17"/>
+      <c r="M147" s="17"/>
+      <c r="N147" s="18"/>
       <c r="O147" s="2"/>
     </row>
     <row r="148" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B148" s="27"/>
-      <c r="C148" s="20" t="s">
+      <c r="B148" s="26"/>
+      <c r="C148" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D148" s="21"/>
-      <c r="E148" s="21"/>
-      <c r="F148" s="21"/>
-      <c r="G148" s="22"/>
+      <c r="D148" s="17"/>
+      <c r="E148" s="17"/>
+      <c r="F148" s="17"/>
+      <c r="G148" s="18"/>
       <c r="H148" s="14"/>
       <c r="I148" s="7"/>
-      <c r="J148" s="20" t="s">
+      <c r="J148" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K148" s="21"/>
-      <c r="L148" s="21"/>
-      <c r="M148" s="21"/>
-      <c r="N148" s="22"/>
+      <c r="K148" s="17"/>
+      <c r="L148" s="17"/>
+      <c r="M148" s="17"/>
+      <c r="N148" s="18"/>
       <c r="O148" s="2"/>
     </row>
     <row r="149" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B149" s="27"/>
+      <c r="B149" s="26"/>
       <c r="C149" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D149" s="21"/>
-      <c r="E149" s="21"/>
-      <c r="F149" s="21"/>
-      <c r="G149" s="22"/>
+      <c r="D149" s="17"/>
+      <c r="E149" s="17"/>
+      <c r="F149" s="17"/>
+      <c r="G149" s="18"/>
       <c r="H149" s="14"/>
       <c r="I149" s="7"/>
       <c r="J149" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K149" s="21"/>
-      <c r="L149" s="21"/>
-      <c r="M149" s="21"/>
-      <c r="N149" s="22"/>
+      <c r="K149" s="17"/>
+      <c r="L149" s="17"/>
+      <c r="M149" s="17"/>
+      <c r="N149" s="18"/>
       <c r="O149" s="2"/>
     </row>
     <row r="150" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B150" s="27"/>
-      <c r="C150" s="25" t="s">
+      <c r="B150" s="26"/>
+      <c r="C150" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D150" s="21"/>
-      <c r="E150" s="21"/>
-      <c r="F150" s="21"/>
-      <c r="G150" s="22"/>
+      <c r="D150" s="17"/>
+      <c r="E150" s="17"/>
+      <c r="F150" s="17"/>
+      <c r="G150" s="18"/>
       <c r="H150" s="14"/>
       <c r="I150" s="7"/>
-      <c r="J150" s="25" t="s">
+      <c r="J150" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K150" s="21"/>
-      <c r="L150" s="21"/>
-      <c r="M150" s="21"/>
-      <c r="N150" s="22"/>
+      <c r="K150" s="17"/>
+      <c r="L150" s="17"/>
+      <c r="M150" s="17"/>
+      <c r="N150" s="18"/>
       <c r="O150" s="2"/>
     </row>
     <row r="151" spans="2:15" x14ac:dyDescent="0.25">
@@ -5143,20 +5140,20 @@
       <c r="O155" s="2"/>
     </row>
     <row r="156" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B156" s="23" t="s">
+      <c r="B156" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C156" s="18"/>
-      <c r="D156" s="18"/>
+      <c r="C156" s="20"/>
+      <c r="D156" s="20"/>
       <c r="E156" s="14"/>
       <c r="F156" s="4"/>
       <c r="G156" s="15"/>
       <c r="H156" s="14"/>
-      <c r="I156" s="23" t="s">
+      <c r="I156" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J156" s="18"/>
-      <c r="K156" s="18"/>
+      <c r="J156" s="20"/>
+      <c r="K156" s="20"/>
       <c r="L156" s="14"/>
       <c r="M156" s="4"/>
       <c r="N156" s="15"/>
@@ -5212,62 +5209,62 @@
     </row>
     <row r="160" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
-      <c r="C160" s="17" t="s">
+      <c r="C160" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D160" s="18"/>
-      <c r="E160" s="18"/>
-      <c r="F160" s="18"/>
-      <c r="G160" s="19"/>
+      <c r="D160" s="20"/>
+      <c r="E160" s="20"/>
+      <c r="F160" s="20"/>
+      <c r="G160" s="22"/>
       <c r="H160" s="14"/>
       <c r="I160" s="6"/>
-      <c r="J160" s="17" t="s">
+      <c r="J160" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K160" s="18"/>
-      <c r="L160" s="18"/>
-      <c r="M160" s="18"/>
-      <c r="N160" s="19"/>
+      <c r="K160" s="20"/>
+      <c r="L160" s="20"/>
+      <c r="M160" s="20"/>
+      <c r="N160" s="22"/>
       <c r="O160" s="2"/>
     </row>
     <row r="161" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B161" s="7"/>
-      <c r="C161" s="20" t="s">
+      <c r="C161" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D161" s="21"/>
-      <c r="E161" s="21"/>
-      <c r="F161" s="21"/>
-      <c r="G161" s="22"/>
+      <c r="D161" s="17"/>
+      <c r="E161" s="17"/>
+      <c r="F161" s="17"/>
+      <c r="G161" s="18"/>
       <c r="H161" s="14"/>
       <c r="I161" s="7"/>
-      <c r="J161" s="20" t="s">
+      <c r="J161" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K161" s="21"/>
-      <c r="L161" s="21"/>
-      <c r="M161" s="21"/>
-      <c r="N161" s="22"/>
+      <c r="K161" s="17"/>
+      <c r="L161" s="17"/>
+      <c r="M161" s="17"/>
+      <c r="N161" s="18"/>
       <c r="O161" s="2"/>
     </row>
     <row r="162" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B162" s="7"/>
-      <c r="C162" s="20" t="s">
+      <c r="C162" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D162" s="21"/>
-      <c r="E162" s="21"/>
-      <c r="F162" s="21"/>
-      <c r="G162" s="22"/>
+      <c r="D162" s="17"/>
+      <c r="E162" s="17"/>
+      <c r="F162" s="17"/>
+      <c r="G162" s="18"/>
       <c r="H162" s="14"/>
       <c r="I162" s="7"/>
-      <c r="J162" s="20" t="s">
+      <c r="J162" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K162" s="21"/>
-      <c r="L162" s="21"/>
-      <c r="M162" s="21"/>
-      <c r="N162" s="22"/>
+      <c r="K162" s="17"/>
+      <c r="L162" s="17"/>
+      <c r="M162" s="17"/>
+      <c r="N162" s="18"/>
       <c r="O162" s="2"/>
     </row>
     <row r="163" spans="2:15" x14ac:dyDescent="0.25">
@@ -5275,39 +5272,39 @@
       <c r="C163" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D163" s="21"/>
-      <c r="E163" s="21"/>
-      <c r="F163" s="21"/>
-      <c r="G163" s="22"/>
+      <c r="D163" s="17"/>
+      <c r="E163" s="17"/>
+      <c r="F163" s="17"/>
+      <c r="G163" s="18"/>
       <c r="H163" s="14"/>
       <c r="I163" s="7"/>
       <c r="J163" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K163" s="21"/>
-      <c r="L163" s="21"/>
-      <c r="M163" s="21"/>
-      <c r="N163" s="22"/>
+      <c r="K163" s="17"/>
+      <c r="L163" s="17"/>
+      <c r="M163" s="17"/>
+      <c r="N163" s="18"/>
       <c r="O163" s="2"/>
     </row>
     <row r="164" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B164" s="7"/>
-      <c r="C164" s="25" t="s">
+      <c r="C164" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D164" s="21"/>
-      <c r="E164" s="21"/>
-      <c r="F164" s="21"/>
-      <c r="G164" s="22"/>
+      <c r="D164" s="17"/>
+      <c r="E164" s="17"/>
+      <c r="F164" s="17"/>
+      <c r="G164" s="18"/>
       <c r="H164" s="14"/>
       <c r="I164" s="7"/>
-      <c r="J164" s="25" t="s">
+      <c r="J164" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K164" s="21"/>
-      <c r="L164" s="21"/>
-      <c r="M164" s="21"/>
-      <c r="N164" s="22"/>
+      <c r="K164" s="17"/>
+      <c r="L164" s="17"/>
+      <c r="M164" s="17"/>
+      <c r="N164" s="18"/>
       <c r="O164" s="2"/>
     </row>
     <row r="165" spans="2:15" x14ac:dyDescent="0.25">
@@ -5407,20 +5404,20 @@
       <c r="O169" s="2"/>
     </row>
     <row r="170" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B170" s="23" t="s">
+      <c r="B170" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C170" s="18"/>
-      <c r="D170" s="18"/>
+      <c r="C170" s="20"/>
+      <c r="D170" s="20"/>
       <c r="E170" s="14"/>
       <c r="F170" s="4"/>
       <c r="G170" s="15"/>
       <c r="H170" s="14"/>
-      <c r="I170" s="23" t="s">
+      <c r="I170" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J170" s="18"/>
-      <c r="K170" s="18"/>
+      <c r="J170" s="20"/>
+      <c r="K170" s="20"/>
       <c r="L170" s="14"/>
       <c r="M170" s="4"/>
       <c r="N170" s="15"/>
@@ -5462,103 +5459,103 @@
       <c r="O173" s="2"/>
     </row>
     <row r="174" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B174" s="26"/>
-      <c r="C174" s="17" t="s">
+      <c r="B174" s="25"/>
+      <c r="C174" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D174" s="18"/>
-      <c r="E174" s="18"/>
-      <c r="F174" s="18"/>
-      <c r="G174" s="19"/>
+      <c r="D174" s="20"/>
+      <c r="E174" s="20"/>
+      <c r="F174" s="20"/>
+      <c r="G174" s="22"/>
       <c r="H174" s="14"/>
       <c r="I174" s="6"/>
-      <c r="J174" s="17" t="s">
+      <c r="J174" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K174" s="18"/>
-      <c r="L174" s="18"/>
-      <c r="M174" s="18"/>
-      <c r="N174" s="19"/>
+      <c r="K174" s="20"/>
+      <c r="L174" s="20"/>
+      <c r="M174" s="20"/>
+      <c r="N174" s="22"/>
       <c r="O174" s="2"/>
     </row>
     <row r="175" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B175" s="27"/>
-      <c r="C175" s="20" t="s">
+      <c r="B175" s="26"/>
+      <c r="C175" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D175" s="21"/>
-      <c r="E175" s="21"/>
-      <c r="F175" s="21"/>
-      <c r="G175" s="22"/>
+      <c r="D175" s="17"/>
+      <c r="E175" s="17"/>
+      <c r="F175" s="17"/>
+      <c r="G175" s="18"/>
       <c r="H175" s="14"/>
       <c r="I175" s="7"/>
-      <c r="J175" s="20" t="s">
+      <c r="J175" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K175" s="21"/>
-      <c r="L175" s="21"/>
-      <c r="M175" s="21"/>
-      <c r="N175" s="22"/>
+      <c r="K175" s="17"/>
+      <c r="L175" s="17"/>
+      <c r="M175" s="17"/>
+      <c r="N175" s="18"/>
       <c r="O175" s="2"/>
     </row>
     <row r="176" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B176" s="27"/>
-      <c r="C176" s="20" t="s">
+      <c r="B176" s="26"/>
+      <c r="C176" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D176" s="21"/>
-      <c r="E176" s="21"/>
-      <c r="F176" s="21"/>
-      <c r="G176" s="22"/>
+      <c r="D176" s="17"/>
+      <c r="E176" s="17"/>
+      <c r="F176" s="17"/>
+      <c r="G176" s="18"/>
       <c r="H176" s="14"/>
       <c r="I176" s="7"/>
-      <c r="J176" s="20" t="s">
+      <c r="J176" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K176" s="21"/>
-      <c r="L176" s="21"/>
-      <c r="M176" s="21"/>
-      <c r="N176" s="22"/>
+      <c r="K176" s="17"/>
+      <c r="L176" s="17"/>
+      <c r="M176" s="17"/>
+      <c r="N176" s="18"/>
       <c r="O176" s="2"/>
     </row>
     <row r="177" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B177" s="27"/>
+      <c r="B177" s="26"/>
       <c r="C177" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D177" s="21"/>
-      <c r="E177" s="21"/>
-      <c r="F177" s="21"/>
-      <c r="G177" s="22"/>
+      <c r="D177" s="17"/>
+      <c r="E177" s="17"/>
+      <c r="F177" s="17"/>
+      <c r="G177" s="18"/>
       <c r="H177" s="14"/>
       <c r="I177" s="7"/>
       <c r="J177" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K177" s="21"/>
-      <c r="L177" s="21"/>
-      <c r="M177" s="21"/>
-      <c r="N177" s="22"/>
+      <c r="K177" s="17"/>
+      <c r="L177" s="17"/>
+      <c r="M177" s="17"/>
+      <c r="N177" s="18"/>
       <c r="O177" s="2"/>
     </row>
     <row r="178" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B178" s="27"/>
-      <c r="C178" s="25" t="s">
+      <c r="B178" s="26"/>
+      <c r="C178" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D178" s="21"/>
-      <c r="E178" s="21"/>
-      <c r="F178" s="21"/>
-      <c r="G178" s="22"/>
+      <c r="D178" s="17"/>
+      <c r="E178" s="17"/>
+      <c r="F178" s="17"/>
+      <c r="G178" s="18"/>
       <c r="H178" s="14"/>
       <c r="I178" s="7"/>
-      <c r="J178" s="25" t="s">
+      <c r="J178" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K178" s="21"/>
-      <c r="L178" s="21"/>
-      <c r="M178" s="21"/>
-      <c r="N178" s="22"/>
+      <c r="K178" s="17"/>
+      <c r="L178" s="17"/>
+      <c r="M178" s="17"/>
+      <c r="N178" s="18"/>
       <c r="O178" s="2"/>
     </row>
     <row r="179" spans="2:15" x14ac:dyDescent="0.25">
@@ -5658,20 +5655,20 @@
       <c r="O183" s="2"/>
     </row>
     <row r="184" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B184" s="23" t="s">
+      <c r="B184" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C184" s="18"/>
-      <c r="D184" s="18"/>
+      <c r="C184" s="20"/>
+      <c r="D184" s="20"/>
       <c r="E184" s="14"/>
       <c r="F184" s="4"/>
       <c r="G184" s="15"/>
       <c r="H184" s="14"/>
-      <c r="I184" s="23" t="s">
+      <c r="I184" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J184" s="18"/>
-      <c r="K184" s="18"/>
+      <c r="J184" s="20"/>
+      <c r="K184" s="20"/>
       <c r="L184" s="14"/>
       <c r="M184" s="4"/>
       <c r="N184" s="15"/>
@@ -5727,62 +5724,62 @@
     </row>
     <row r="188" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
-      <c r="C188" s="17" t="s">
+      <c r="C188" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D188" s="18"/>
-      <c r="E188" s="18"/>
-      <c r="F188" s="18"/>
-      <c r="G188" s="19"/>
+      <c r="D188" s="20"/>
+      <c r="E188" s="20"/>
+      <c r="F188" s="20"/>
+      <c r="G188" s="22"/>
       <c r="H188" s="14"/>
       <c r="I188" s="6"/>
-      <c r="J188" s="17" t="s">
+      <c r="J188" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K188" s="18"/>
-      <c r="L188" s="18"/>
-      <c r="M188" s="18"/>
-      <c r="N188" s="19"/>
+      <c r="K188" s="20"/>
+      <c r="L188" s="20"/>
+      <c r="M188" s="20"/>
+      <c r="N188" s="22"/>
       <c r="O188" s="2"/>
     </row>
     <row r="189" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B189" s="7"/>
-      <c r="C189" s="20" t="s">
+      <c r="C189" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D189" s="21"/>
-      <c r="E189" s="21"/>
-      <c r="F189" s="21"/>
-      <c r="G189" s="22"/>
+      <c r="D189" s="17"/>
+      <c r="E189" s="17"/>
+      <c r="F189" s="17"/>
+      <c r="G189" s="18"/>
       <c r="H189" s="14"/>
       <c r="I189" s="7"/>
-      <c r="J189" s="20" t="s">
+      <c r="J189" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K189" s="21"/>
-      <c r="L189" s="21"/>
-      <c r="M189" s="21"/>
-      <c r="N189" s="22"/>
+      <c r="K189" s="17"/>
+      <c r="L189" s="17"/>
+      <c r="M189" s="17"/>
+      <c r="N189" s="18"/>
       <c r="O189" s="2"/>
     </row>
     <row r="190" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B190" s="7"/>
-      <c r="C190" s="20" t="s">
+      <c r="C190" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D190" s="21"/>
-      <c r="E190" s="21"/>
-      <c r="F190" s="21"/>
-      <c r="G190" s="22"/>
+      <c r="D190" s="17"/>
+      <c r="E190" s="17"/>
+      <c r="F190" s="17"/>
+      <c r="G190" s="18"/>
       <c r="H190" s="14"/>
       <c r="I190" s="7"/>
-      <c r="J190" s="20" t="s">
+      <c r="J190" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K190" s="21"/>
-      <c r="L190" s="21"/>
-      <c r="M190" s="21"/>
-      <c r="N190" s="22"/>
+      <c r="K190" s="17"/>
+      <c r="L190" s="17"/>
+      <c r="M190" s="17"/>
+      <c r="N190" s="18"/>
       <c r="O190" s="2"/>
     </row>
     <row r="191" spans="2:15" x14ac:dyDescent="0.25">
@@ -5790,39 +5787,39 @@
       <c r="C191" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D191" s="21"/>
-      <c r="E191" s="21"/>
-      <c r="F191" s="21"/>
-      <c r="G191" s="22"/>
+      <c r="D191" s="17"/>
+      <c r="E191" s="17"/>
+      <c r="F191" s="17"/>
+      <c r="G191" s="18"/>
       <c r="H191" s="14"/>
       <c r="I191" s="7"/>
       <c r="J191" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K191" s="21"/>
-      <c r="L191" s="21"/>
-      <c r="M191" s="21"/>
-      <c r="N191" s="22"/>
+      <c r="K191" s="17"/>
+      <c r="L191" s="17"/>
+      <c r="M191" s="17"/>
+      <c r="N191" s="18"/>
       <c r="O191" s="2"/>
     </row>
     <row r="192" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B192" s="7"/>
-      <c r="C192" s="25" t="s">
+      <c r="C192" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D192" s="21"/>
-      <c r="E192" s="21"/>
-      <c r="F192" s="21"/>
-      <c r="G192" s="22"/>
+      <c r="D192" s="17"/>
+      <c r="E192" s="17"/>
+      <c r="F192" s="17"/>
+      <c r="G192" s="18"/>
       <c r="H192" s="14"/>
       <c r="I192" s="7"/>
-      <c r="J192" s="25" t="s">
+      <c r="J192" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K192" s="21"/>
-      <c r="L192" s="21"/>
-      <c r="M192" s="21"/>
-      <c r="N192" s="22"/>
+      <c r="K192" s="17"/>
+      <c r="L192" s="17"/>
+      <c r="M192" s="17"/>
+      <c r="N192" s="18"/>
       <c r="O192" s="2"/>
     </row>
     <row r="193" spans="2:15" x14ac:dyDescent="0.25">
@@ -5922,20 +5919,20 @@
       <c r="O197" s="2"/>
     </row>
     <row r="198" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B198" s="23" t="s">
+      <c r="B198" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C198" s="18"/>
-      <c r="D198" s="18"/>
+      <c r="C198" s="20"/>
+      <c r="D198" s="20"/>
       <c r="E198" s="14"/>
       <c r="F198" s="4"/>
       <c r="G198" s="15"/>
       <c r="H198" s="14"/>
-      <c r="I198" s="23" t="s">
+      <c r="I198" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J198" s="18"/>
-      <c r="K198" s="18"/>
+      <c r="J198" s="20"/>
+      <c r="K198" s="20"/>
       <c r="L198" s="14"/>
       <c r="M198" s="4"/>
       <c r="N198" s="15"/>
@@ -5977,103 +5974,103 @@
       <c r="O201" s="2"/>
     </row>
     <row r="202" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B202" s="26"/>
-      <c r="C202" s="17" t="s">
+      <c r="B202" s="25"/>
+      <c r="C202" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D202" s="18"/>
-      <c r="E202" s="18"/>
-      <c r="F202" s="18"/>
-      <c r="G202" s="19"/>
+      <c r="D202" s="20"/>
+      <c r="E202" s="20"/>
+      <c r="F202" s="20"/>
+      <c r="G202" s="22"/>
       <c r="H202" s="14"/>
       <c r="I202" s="6"/>
-      <c r="J202" s="17" t="s">
+      <c r="J202" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K202" s="18"/>
-      <c r="L202" s="18"/>
-      <c r="M202" s="18"/>
-      <c r="N202" s="19"/>
+      <c r="K202" s="20"/>
+      <c r="L202" s="20"/>
+      <c r="M202" s="20"/>
+      <c r="N202" s="22"/>
       <c r="O202" s="2"/>
     </row>
     <row r="203" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B203" s="27"/>
-      <c r="C203" s="20" t="s">
+      <c r="B203" s="26"/>
+      <c r="C203" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D203" s="21"/>
-      <c r="E203" s="21"/>
-      <c r="F203" s="21"/>
-      <c r="G203" s="22"/>
+      <c r="D203" s="17"/>
+      <c r="E203" s="17"/>
+      <c r="F203" s="17"/>
+      <c r="G203" s="18"/>
       <c r="H203" s="14"/>
       <c r="I203" s="7"/>
-      <c r="J203" s="20" t="s">
+      <c r="J203" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K203" s="21"/>
-      <c r="L203" s="21"/>
-      <c r="M203" s="21"/>
-      <c r="N203" s="22"/>
+      <c r="K203" s="17"/>
+      <c r="L203" s="17"/>
+      <c r="M203" s="17"/>
+      <c r="N203" s="18"/>
       <c r="O203" s="2"/>
     </row>
     <row r="204" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B204" s="27"/>
-      <c r="C204" s="20" t="s">
+      <c r="B204" s="26"/>
+      <c r="C204" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D204" s="21"/>
-      <c r="E204" s="21"/>
-      <c r="F204" s="21"/>
-      <c r="G204" s="22"/>
+      <c r="D204" s="17"/>
+      <c r="E204" s="17"/>
+      <c r="F204" s="17"/>
+      <c r="G204" s="18"/>
       <c r="H204" s="14"/>
       <c r="I204" s="7"/>
-      <c r="J204" s="20" t="s">
+      <c r="J204" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K204" s="21"/>
-      <c r="L204" s="21"/>
-      <c r="M204" s="21"/>
-      <c r="N204" s="22"/>
+      <c r="K204" s="17"/>
+      <c r="L204" s="17"/>
+      <c r="M204" s="17"/>
+      <c r="N204" s="18"/>
       <c r="O204" s="2"/>
     </row>
     <row r="205" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B205" s="27"/>
+      <c r="B205" s="26"/>
       <c r="C205" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D205" s="21"/>
-      <c r="E205" s="21"/>
-      <c r="F205" s="21"/>
-      <c r="G205" s="22"/>
+      <c r="D205" s="17"/>
+      <c r="E205" s="17"/>
+      <c r="F205" s="17"/>
+      <c r="G205" s="18"/>
       <c r="H205" s="14"/>
       <c r="I205" s="7"/>
       <c r="J205" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K205" s="21"/>
-      <c r="L205" s="21"/>
-      <c r="M205" s="21"/>
-      <c r="N205" s="22"/>
+      <c r="K205" s="17"/>
+      <c r="L205" s="17"/>
+      <c r="M205" s="17"/>
+      <c r="N205" s="18"/>
       <c r="O205" s="2"/>
     </row>
     <row r="206" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B206" s="27"/>
-      <c r="C206" s="25" t="s">
+      <c r="B206" s="26"/>
+      <c r="C206" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D206" s="21"/>
-      <c r="E206" s="21"/>
-      <c r="F206" s="21"/>
-      <c r="G206" s="22"/>
+      <c r="D206" s="17"/>
+      <c r="E206" s="17"/>
+      <c r="F206" s="17"/>
+      <c r="G206" s="18"/>
       <c r="H206" s="14"/>
       <c r="I206" s="7"/>
-      <c r="J206" s="25" t="s">
+      <c r="J206" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K206" s="21"/>
-      <c r="L206" s="21"/>
-      <c r="M206" s="21"/>
-      <c r="N206" s="22"/>
+      <c r="K206" s="17"/>
+      <c r="L206" s="17"/>
+      <c r="M206" s="17"/>
+      <c r="N206" s="18"/>
       <c r="O206" s="2"/>
     </row>
     <row r="207" spans="2:15" x14ac:dyDescent="0.25">
@@ -6173,20 +6170,20 @@
       <c r="O211" s="2"/>
     </row>
     <row r="212" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B212" s="23" t="s">
+      <c r="B212" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C212" s="18"/>
-      <c r="D212" s="18"/>
+      <c r="C212" s="20"/>
+      <c r="D212" s="20"/>
       <c r="E212" s="14"/>
       <c r="F212" s="4"/>
       <c r="G212" s="15"/>
       <c r="H212" s="14"/>
-      <c r="I212" s="23" t="s">
+      <c r="I212" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J212" s="18"/>
-      <c r="K212" s="18"/>
+      <c r="J212" s="20"/>
+      <c r="K212" s="20"/>
       <c r="L212" s="14"/>
       <c r="M212" s="4"/>
       <c r="N212" s="15"/>
@@ -6242,62 +6239,62 @@
     </row>
     <row r="216" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B216" s="6"/>
-      <c r="C216" s="17" t="s">
+      <c r="C216" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D216" s="18"/>
-      <c r="E216" s="18"/>
-      <c r="F216" s="18"/>
-      <c r="G216" s="19"/>
+      <c r="D216" s="20"/>
+      <c r="E216" s="20"/>
+      <c r="F216" s="20"/>
+      <c r="G216" s="22"/>
       <c r="H216" s="14"/>
       <c r="I216" s="6"/>
-      <c r="J216" s="17" t="s">
+      <c r="J216" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K216" s="18"/>
-      <c r="L216" s="18"/>
-      <c r="M216" s="18"/>
-      <c r="N216" s="19"/>
+      <c r="K216" s="20"/>
+      <c r="L216" s="20"/>
+      <c r="M216" s="20"/>
+      <c r="N216" s="22"/>
       <c r="O216" s="2"/>
     </row>
     <row r="217" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B217" s="7"/>
-      <c r="C217" s="20" t="s">
+      <c r="C217" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D217" s="21"/>
-      <c r="E217" s="21"/>
-      <c r="F217" s="21"/>
-      <c r="G217" s="22"/>
+      <c r="D217" s="17"/>
+      <c r="E217" s="17"/>
+      <c r="F217" s="17"/>
+      <c r="G217" s="18"/>
       <c r="H217" s="14"/>
       <c r="I217" s="7"/>
-      <c r="J217" s="20" t="s">
+      <c r="J217" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K217" s="21"/>
-      <c r="L217" s="21"/>
-      <c r="M217" s="21"/>
-      <c r="N217" s="22"/>
+      <c r="K217" s="17"/>
+      <c r="L217" s="17"/>
+      <c r="M217" s="17"/>
+      <c r="N217" s="18"/>
       <c r="O217" s="2"/>
     </row>
     <row r="218" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B218" s="7"/>
-      <c r="C218" s="20" t="s">
+      <c r="C218" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D218" s="21"/>
-      <c r="E218" s="21"/>
-      <c r="F218" s="21"/>
-      <c r="G218" s="22"/>
+      <c r="D218" s="17"/>
+      <c r="E218" s="17"/>
+      <c r="F218" s="17"/>
+      <c r="G218" s="18"/>
       <c r="H218" s="14"/>
       <c r="I218" s="7"/>
-      <c r="J218" s="20" t="s">
+      <c r="J218" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K218" s="21"/>
-      <c r="L218" s="21"/>
-      <c r="M218" s="21"/>
-      <c r="N218" s="22"/>
+      <c r="K218" s="17"/>
+      <c r="L218" s="17"/>
+      <c r="M218" s="17"/>
+      <c r="N218" s="18"/>
       <c r="O218" s="2"/>
     </row>
     <row r="219" spans="2:15" x14ac:dyDescent="0.25">
@@ -6305,39 +6302,39 @@
       <c r="C219" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D219" s="21"/>
-      <c r="E219" s="21"/>
-      <c r="F219" s="21"/>
-      <c r="G219" s="22"/>
+      <c r="D219" s="17"/>
+      <c r="E219" s="17"/>
+      <c r="F219" s="17"/>
+      <c r="G219" s="18"/>
       <c r="H219" s="14"/>
       <c r="I219" s="7"/>
       <c r="J219" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K219" s="21"/>
-      <c r="L219" s="21"/>
-      <c r="M219" s="21"/>
-      <c r="N219" s="22"/>
+      <c r="K219" s="17"/>
+      <c r="L219" s="17"/>
+      <c r="M219" s="17"/>
+      <c r="N219" s="18"/>
       <c r="O219" s="2"/>
     </row>
     <row r="220" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B220" s="7"/>
-      <c r="C220" s="25" t="s">
+      <c r="C220" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D220" s="21"/>
-      <c r="E220" s="21"/>
-      <c r="F220" s="21"/>
-      <c r="G220" s="22"/>
+      <c r="D220" s="17"/>
+      <c r="E220" s="17"/>
+      <c r="F220" s="17"/>
+      <c r="G220" s="18"/>
       <c r="H220" s="14"/>
       <c r="I220" s="7"/>
-      <c r="J220" s="25" t="s">
+      <c r="J220" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K220" s="21"/>
-      <c r="L220" s="21"/>
-      <c r="M220" s="21"/>
-      <c r="N220" s="22"/>
+      <c r="K220" s="17"/>
+      <c r="L220" s="17"/>
+      <c r="M220" s="17"/>
+      <c r="N220" s="18"/>
       <c r="O220" s="2"/>
     </row>
     <row r="221" spans="2:15" x14ac:dyDescent="0.25">
@@ -6437,20 +6434,20 @@
       <c r="O225" s="2"/>
     </row>
     <row r="226" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B226" s="23" t="s">
+      <c r="B226" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C226" s="18"/>
-      <c r="D226" s="18"/>
+      <c r="C226" s="20"/>
+      <c r="D226" s="20"/>
       <c r="E226" s="14"/>
       <c r="F226" s="4"/>
       <c r="G226" s="15"/>
       <c r="H226" s="14"/>
-      <c r="I226" s="23" t="s">
+      <c r="I226" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J226" s="18"/>
-      <c r="K226" s="18"/>
+      <c r="J226" s="20"/>
+      <c r="K226" s="20"/>
       <c r="L226" s="14"/>
       <c r="M226" s="4"/>
       <c r="N226" s="15"/>
@@ -6492,103 +6489,103 @@
       <c r="O229" s="2"/>
     </row>
     <row r="230" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B230" s="26"/>
-      <c r="C230" s="17" t="s">
+      <c r="B230" s="25"/>
+      <c r="C230" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D230" s="18"/>
-      <c r="E230" s="18"/>
-      <c r="F230" s="18"/>
-      <c r="G230" s="19"/>
+      <c r="D230" s="20"/>
+      <c r="E230" s="20"/>
+      <c r="F230" s="20"/>
+      <c r="G230" s="22"/>
       <c r="H230" s="14"/>
       <c r="I230" s="6"/>
-      <c r="J230" s="17" t="s">
+      <c r="J230" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K230" s="18"/>
-      <c r="L230" s="18"/>
-      <c r="M230" s="18"/>
-      <c r="N230" s="19"/>
+      <c r="K230" s="20"/>
+      <c r="L230" s="20"/>
+      <c r="M230" s="20"/>
+      <c r="N230" s="22"/>
       <c r="O230" s="2"/>
     </row>
     <row r="231" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B231" s="27"/>
-      <c r="C231" s="20" t="s">
+      <c r="B231" s="26"/>
+      <c r="C231" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D231" s="21"/>
-      <c r="E231" s="21"/>
-      <c r="F231" s="21"/>
-      <c r="G231" s="22"/>
+      <c r="D231" s="17"/>
+      <c r="E231" s="17"/>
+      <c r="F231" s="17"/>
+      <c r="G231" s="18"/>
       <c r="H231" s="14"/>
       <c r="I231" s="7"/>
-      <c r="J231" s="20" t="s">
+      <c r="J231" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K231" s="21"/>
-      <c r="L231" s="21"/>
-      <c r="M231" s="21"/>
-      <c r="N231" s="22"/>
+      <c r="K231" s="17"/>
+      <c r="L231" s="17"/>
+      <c r="M231" s="17"/>
+      <c r="N231" s="18"/>
       <c r="O231" s="2"/>
     </row>
     <row r="232" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B232" s="27"/>
-      <c r="C232" s="20" t="s">
+      <c r="B232" s="26"/>
+      <c r="C232" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D232" s="21"/>
-      <c r="E232" s="21"/>
-      <c r="F232" s="21"/>
-      <c r="G232" s="22"/>
+      <c r="D232" s="17"/>
+      <c r="E232" s="17"/>
+      <c r="F232" s="17"/>
+      <c r="G232" s="18"/>
       <c r="H232" s="14"/>
       <c r="I232" s="7"/>
-      <c r="J232" s="20" t="s">
+      <c r="J232" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K232" s="21"/>
-      <c r="L232" s="21"/>
-      <c r="M232" s="21"/>
-      <c r="N232" s="22"/>
+      <c r="K232" s="17"/>
+      <c r="L232" s="17"/>
+      <c r="M232" s="17"/>
+      <c r="N232" s="18"/>
       <c r="O232" s="2"/>
     </row>
     <row r="233" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B233" s="27"/>
+      <c r="B233" s="26"/>
       <c r="C233" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D233" s="21"/>
-      <c r="E233" s="21"/>
-      <c r="F233" s="21"/>
-      <c r="G233" s="22"/>
+      <c r="D233" s="17"/>
+      <c r="E233" s="17"/>
+      <c r="F233" s="17"/>
+      <c r="G233" s="18"/>
       <c r="H233" s="14"/>
       <c r="I233" s="7"/>
       <c r="J233" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K233" s="21"/>
-      <c r="L233" s="21"/>
-      <c r="M233" s="21"/>
-      <c r="N233" s="22"/>
+      <c r="K233" s="17"/>
+      <c r="L233" s="17"/>
+      <c r="M233" s="17"/>
+      <c r="N233" s="18"/>
       <c r="O233" s="2"/>
     </row>
     <row r="234" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B234" s="27"/>
-      <c r="C234" s="25" t="s">
+      <c r="B234" s="26"/>
+      <c r="C234" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D234" s="21"/>
-      <c r="E234" s="21"/>
-      <c r="F234" s="21"/>
-      <c r="G234" s="22"/>
+      <c r="D234" s="17"/>
+      <c r="E234" s="17"/>
+      <c r="F234" s="17"/>
+      <c r="G234" s="18"/>
       <c r="H234" s="14"/>
       <c r="I234" s="7"/>
-      <c r="J234" s="25" t="s">
+      <c r="J234" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K234" s="21"/>
-      <c r="L234" s="21"/>
-      <c r="M234" s="21"/>
-      <c r="N234" s="22"/>
+      <c r="K234" s="17"/>
+      <c r="L234" s="17"/>
+      <c r="M234" s="17"/>
+      <c r="N234" s="18"/>
       <c r="O234" s="2"/>
     </row>
     <row r="235" spans="2:15" x14ac:dyDescent="0.25">
@@ -6688,20 +6685,20 @@
       <c r="O239" s="2"/>
     </row>
     <row r="240" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B240" s="23" t="s">
+      <c r="B240" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C240" s="18"/>
-      <c r="D240" s="18"/>
+      <c r="C240" s="20"/>
+      <c r="D240" s="20"/>
       <c r="E240" s="14"/>
       <c r="F240" s="4"/>
       <c r="G240" s="15"/>
       <c r="H240" s="14"/>
-      <c r="I240" s="23" t="s">
+      <c r="I240" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J240" s="18"/>
-      <c r="K240" s="18"/>
+      <c r="J240" s="20"/>
+      <c r="K240" s="20"/>
       <c r="L240" s="14"/>
       <c r="M240" s="4"/>
       <c r="N240" s="15"/>
@@ -6757,62 +6754,62 @@
     </row>
     <row r="244" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B244" s="6"/>
-      <c r="C244" s="17" t="s">
+      <c r="C244" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D244" s="18"/>
-      <c r="E244" s="18"/>
-      <c r="F244" s="18"/>
-      <c r="G244" s="19"/>
+      <c r="D244" s="20"/>
+      <c r="E244" s="20"/>
+      <c r="F244" s="20"/>
+      <c r="G244" s="22"/>
       <c r="H244" s="14"/>
       <c r="I244" s="6"/>
-      <c r="J244" s="17" t="s">
+      <c r="J244" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K244" s="18"/>
-      <c r="L244" s="18"/>
-      <c r="M244" s="18"/>
-      <c r="N244" s="19"/>
+      <c r="K244" s="20"/>
+      <c r="L244" s="20"/>
+      <c r="M244" s="20"/>
+      <c r="N244" s="22"/>
       <c r="O244" s="2"/>
     </row>
     <row r="245" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B245" s="7"/>
-      <c r="C245" s="20" t="s">
+      <c r="C245" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D245" s="21"/>
-      <c r="E245" s="21"/>
-      <c r="F245" s="21"/>
-      <c r="G245" s="22"/>
+      <c r="D245" s="17"/>
+      <c r="E245" s="17"/>
+      <c r="F245" s="17"/>
+      <c r="G245" s="18"/>
       <c r="H245" s="14"/>
       <c r="I245" s="7"/>
-      <c r="J245" s="20" t="s">
+      <c r="J245" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K245" s="21"/>
-      <c r="L245" s="21"/>
-      <c r="M245" s="21"/>
-      <c r="N245" s="22"/>
+      <c r="K245" s="17"/>
+      <c r="L245" s="17"/>
+      <c r="M245" s="17"/>
+      <c r="N245" s="18"/>
       <c r="O245" s="2"/>
     </row>
     <row r="246" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B246" s="7"/>
-      <c r="C246" s="20" t="s">
+      <c r="C246" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D246" s="21"/>
-      <c r="E246" s="21"/>
-      <c r="F246" s="21"/>
-      <c r="G246" s="22"/>
+      <c r="D246" s="17"/>
+      <c r="E246" s="17"/>
+      <c r="F246" s="17"/>
+      <c r="G246" s="18"/>
       <c r="H246" s="14"/>
       <c r="I246" s="7"/>
-      <c r="J246" s="20" t="s">
+      <c r="J246" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K246" s="21"/>
-      <c r="L246" s="21"/>
-      <c r="M246" s="21"/>
-      <c r="N246" s="22"/>
+      <c r="K246" s="17"/>
+      <c r="L246" s="17"/>
+      <c r="M246" s="17"/>
+      <c r="N246" s="18"/>
       <c r="O246" s="2"/>
     </row>
     <row r="247" spans="2:15" x14ac:dyDescent="0.25">
@@ -6820,39 +6817,39 @@
       <c r="C247" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D247" s="21"/>
-      <c r="E247" s="21"/>
-      <c r="F247" s="21"/>
-      <c r="G247" s="22"/>
+      <c r="D247" s="17"/>
+      <c r="E247" s="17"/>
+      <c r="F247" s="17"/>
+      <c r="G247" s="18"/>
       <c r="H247" s="14"/>
       <c r="I247" s="7"/>
       <c r="J247" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K247" s="21"/>
-      <c r="L247" s="21"/>
-      <c r="M247" s="21"/>
-      <c r="N247" s="22"/>
+      <c r="K247" s="17"/>
+      <c r="L247" s="17"/>
+      <c r="M247" s="17"/>
+      <c r="N247" s="18"/>
       <c r="O247" s="2"/>
     </row>
     <row r="248" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B248" s="7"/>
-      <c r="C248" s="25" t="s">
+      <c r="C248" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D248" s="21"/>
-      <c r="E248" s="21"/>
-      <c r="F248" s="21"/>
-      <c r="G248" s="22"/>
+      <c r="D248" s="17"/>
+      <c r="E248" s="17"/>
+      <c r="F248" s="17"/>
+      <c r="G248" s="18"/>
       <c r="H248" s="14"/>
       <c r="I248" s="7"/>
-      <c r="J248" s="25" t="s">
+      <c r="J248" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K248" s="21"/>
-      <c r="L248" s="21"/>
-      <c r="M248" s="21"/>
-      <c r="N248" s="22"/>
+      <c r="K248" s="17"/>
+      <c r="L248" s="17"/>
+      <c r="M248" s="17"/>
+      <c r="N248" s="18"/>
       <c r="O248" s="2"/>
     </row>
     <row r="249" spans="2:15" x14ac:dyDescent="0.25">
@@ -6952,20 +6949,20 @@
       <c r="O253" s="2"/>
     </row>
     <row r="254" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B254" s="23" t="s">
+      <c r="B254" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C254" s="18"/>
-      <c r="D254" s="18"/>
+      <c r="C254" s="20"/>
+      <c r="D254" s="20"/>
       <c r="E254" s="14"/>
       <c r="F254" s="4"/>
       <c r="G254" s="15"/>
       <c r="H254" s="14"/>
-      <c r="I254" s="23" t="s">
+      <c r="I254" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J254" s="18"/>
-      <c r="K254" s="18"/>
+      <c r="J254" s="20"/>
+      <c r="K254" s="20"/>
       <c r="L254" s="14"/>
       <c r="M254" s="4"/>
       <c r="N254" s="15"/>
@@ -7007,103 +7004,103 @@
       <c r="O257" s="2"/>
     </row>
     <row r="258" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B258" s="26"/>
-      <c r="C258" s="17" t="s">
+      <c r="B258" s="25"/>
+      <c r="C258" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D258" s="18"/>
-      <c r="E258" s="18"/>
-      <c r="F258" s="18"/>
-      <c r="G258" s="19"/>
+      <c r="D258" s="20"/>
+      <c r="E258" s="20"/>
+      <c r="F258" s="20"/>
+      <c r="G258" s="22"/>
       <c r="H258" s="14"/>
       <c r="I258" s="6"/>
-      <c r="J258" s="17" t="s">
+      <c r="J258" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K258" s="18"/>
-      <c r="L258" s="18"/>
-      <c r="M258" s="18"/>
-      <c r="N258" s="19"/>
+      <c r="K258" s="20"/>
+      <c r="L258" s="20"/>
+      <c r="M258" s="20"/>
+      <c r="N258" s="22"/>
       <c r="O258" s="2"/>
     </row>
     <row r="259" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B259" s="27"/>
-      <c r="C259" s="20" t="s">
+      <c r="B259" s="26"/>
+      <c r="C259" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D259" s="21"/>
-      <c r="E259" s="21"/>
-      <c r="F259" s="21"/>
-      <c r="G259" s="22"/>
+      <c r="D259" s="17"/>
+      <c r="E259" s="17"/>
+      <c r="F259" s="17"/>
+      <c r="G259" s="18"/>
       <c r="H259" s="14"/>
       <c r="I259" s="7"/>
-      <c r="J259" s="20" t="s">
+      <c r="J259" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K259" s="21"/>
-      <c r="L259" s="21"/>
-      <c r="M259" s="21"/>
-      <c r="N259" s="22"/>
+      <c r="K259" s="17"/>
+      <c r="L259" s="17"/>
+      <c r="M259" s="17"/>
+      <c r="N259" s="18"/>
       <c r="O259" s="2"/>
     </row>
     <row r="260" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B260" s="27"/>
-      <c r="C260" s="20" t="s">
+      <c r="B260" s="26"/>
+      <c r="C260" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D260" s="21"/>
-      <c r="E260" s="21"/>
-      <c r="F260" s="21"/>
-      <c r="G260" s="22"/>
+      <c r="D260" s="17"/>
+      <c r="E260" s="17"/>
+      <c r="F260" s="17"/>
+      <c r="G260" s="18"/>
       <c r="H260" s="14"/>
       <c r="I260" s="7"/>
-      <c r="J260" s="20" t="s">
+      <c r="J260" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K260" s="21"/>
-      <c r="L260" s="21"/>
-      <c r="M260" s="21"/>
-      <c r="N260" s="22"/>
+      <c r="K260" s="17"/>
+      <c r="L260" s="17"/>
+      <c r="M260" s="17"/>
+      <c r="N260" s="18"/>
       <c r="O260" s="2"/>
     </row>
     <row r="261" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B261" s="27"/>
+      <c r="B261" s="26"/>
       <c r="C261" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D261" s="21"/>
-      <c r="E261" s="21"/>
-      <c r="F261" s="21"/>
-      <c r="G261" s="22"/>
+      <c r="D261" s="17"/>
+      <c r="E261" s="17"/>
+      <c r="F261" s="17"/>
+      <c r="G261" s="18"/>
       <c r="H261" s="14"/>
       <c r="I261" s="7"/>
       <c r="J261" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K261" s="21"/>
-      <c r="L261" s="21"/>
-      <c r="M261" s="21"/>
-      <c r="N261" s="22"/>
+      <c r="K261" s="17"/>
+      <c r="L261" s="17"/>
+      <c r="M261" s="17"/>
+      <c r="N261" s="18"/>
       <c r="O261" s="2"/>
     </row>
     <row r="262" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B262" s="27"/>
-      <c r="C262" s="25" t="s">
+      <c r="B262" s="26"/>
+      <c r="C262" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D262" s="21"/>
-      <c r="E262" s="21"/>
-      <c r="F262" s="21"/>
-      <c r="G262" s="22"/>
+      <c r="D262" s="17"/>
+      <c r="E262" s="17"/>
+      <c r="F262" s="17"/>
+      <c r="G262" s="18"/>
       <c r="H262" s="14"/>
       <c r="I262" s="7"/>
-      <c r="J262" s="25" t="s">
+      <c r="J262" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K262" s="21"/>
-      <c r="L262" s="21"/>
-      <c r="M262" s="21"/>
-      <c r="N262" s="22"/>
+      <c r="K262" s="17"/>
+      <c r="L262" s="17"/>
+      <c r="M262" s="17"/>
+      <c r="N262" s="18"/>
       <c r="O262" s="2"/>
     </row>
     <row r="263" spans="2:15" x14ac:dyDescent="0.25">
@@ -7203,20 +7200,20 @@
       <c r="O267" s="2"/>
     </row>
     <row r="268" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B268" s="23" t="s">
+      <c r="B268" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C268" s="18"/>
-      <c r="D268" s="18"/>
+      <c r="C268" s="20"/>
+      <c r="D268" s="20"/>
       <c r="E268" s="14"/>
       <c r="F268" s="4"/>
       <c r="G268" s="15"/>
       <c r="H268" s="14"/>
-      <c r="I268" s="23" t="s">
+      <c r="I268" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J268" s="18"/>
-      <c r="K268" s="18"/>
+      <c r="J268" s="20"/>
+      <c r="K268" s="20"/>
       <c r="L268" s="14"/>
       <c r="M268" s="4"/>
       <c r="N268" s="15"/>
@@ -7272,62 +7269,62 @@
     </row>
     <row r="272" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B272" s="6"/>
-      <c r="C272" s="17" t="s">
+      <c r="C272" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D272" s="18"/>
-      <c r="E272" s="18"/>
-      <c r="F272" s="18"/>
-      <c r="G272" s="19"/>
+      <c r="D272" s="20"/>
+      <c r="E272" s="20"/>
+      <c r="F272" s="20"/>
+      <c r="G272" s="22"/>
       <c r="H272" s="14"/>
       <c r="I272" s="6"/>
-      <c r="J272" s="17" t="s">
+      <c r="J272" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K272" s="18"/>
-      <c r="L272" s="18"/>
-      <c r="M272" s="18"/>
-      <c r="N272" s="19"/>
+      <c r="K272" s="20"/>
+      <c r="L272" s="20"/>
+      <c r="M272" s="20"/>
+      <c r="N272" s="22"/>
       <c r="O272" s="2"/>
     </row>
     <row r="273" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B273" s="7"/>
-      <c r="C273" s="20" t="s">
+      <c r="C273" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D273" s="21"/>
-      <c r="E273" s="21"/>
-      <c r="F273" s="21"/>
-      <c r="G273" s="22"/>
+      <c r="D273" s="17"/>
+      <c r="E273" s="17"/>
+      <c r="F273" s="17"/>
+      <c r="G273" s="18"/>
       <c r="H273" s="14"/>
       <c r="I273" s="7"/>
-      <c r="J273" s="20" t="s">
+      <c r="J273" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K273" s="21"/>
-      <c r="L273" s="21"/>
-      <c r="M273" s="21"/>
-      <c r="N273" s="22"/>
+      <c r="K273" s="17"/>
+      <c r="L273" s="17"/>
+      <c r="M273" s="17"/>
+      <c r="N273" s="18"/>
       <c r="O273" s="2"/>
     </row>
     <row r="274" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B274" s="7"/>
-      <c r="C274" s="20" t="s">
+      <c r="C274" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D274" s="21"/>
-      <c r="E274" s="21"/>
-      <c r="F274" s="21"/>
-      <c r="G274" s="22"/>
+      <c r="D274" s="17"/>
+      <c r="E274" s="17"/>
+      <c r="F274" s="17"/>
+      <c r="G274" s="18"/>
       <c r="H274" s="14"/>
       <c r="I274" s="7"/>
-      <c r="J274" s="20" t="s">
+      <c r="J274" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K274" s="21"/>
-      <c r="L274" s="21"/>
-      <c r="M274" s="21"/>
-      <c r="N274" s="22"/>
+      <c r="K274" s="17"/>
+      <c r="L274" s="17"/>
+      <c r="M274" s="17"/>
+      <c r="N274" s="18"/>
       <c r="O274" s="2"/>
     </row>
     <row r="275" spans="2:15" x14ac:dyDescent="0.25">
@@ -7335,39 +7332,39 @@
       <c r="C275" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D275" s="21"/>
-      <c r="E275" s="21"/>
-      <c r="F275" s="21"/>
-      <c r="G275" s="22"/>
+      <c r="D275" s="17"/>
+      <c r="E275" s="17"/>
+      <c r="F275" s="17"/>
+      <c r="G275" s="18"/>
       <c r="H275" s="14"/>
       <c r="I275" s="7"/>
       <c r="J275" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K275" s="21"/>
-      <c r="L275" s="21"/>
-      <c r="M275" s="21"/>
-      <c r="N275" s="22"/>
+      <c r="K275" s="17"/>
+      <c r="L275" s="17"/>
+      <c r="M275" s="17"/>
+      <c r="N275" s="18"/>
       <c r="O275" s="2"/>
     </row>
     <row r="276" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B276" s="7"/>
-      <c r="C276" s="25" t="s">
+      <c r="C276" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D276" s="21"/>
-      <c r="E276" s="21"/>
-      <c r="F276" s="21"/>
-      <c r="G276" s="22"/>
+      <c r="D276" s="17"/>
+      <c r="E276" s="17"/>
+      <c r="F276" s="17"/>
+      <c r="G276" s="18"/>
       <c r="H276" s="14"/>
       <c r="I276" s="7"/>
-      <c r="J276" s="25" t="s">
+      <c r="J276" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K276" s="21"/>
-      <c r="L276" s="21"/>
-      <c r="M276" s="21"/>
-      <c r="N276" s="22"/>
+      <c r="K276" s="17"/>
+      <c r="L276" s="17"/>
+      <c r="M276" s="17"/>
+      <c r="N276" s="18"/>
       <c r="O276" s="2"/>
     </row>
     <row r="277" spans="2:15" x14ac:dyDescent="0.25">
@@ -7467,20 +7464,20 @@
       <c r="O281" s="2"/>
     </row>
     <row r="282" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B282" s="23" t="s">
+      <c r="B282" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C282" s="18"/>
-      <c r="D282" s="18"/>
+      <c r="C282" s="20"/>
+      <c r="D282" s="20"/>
       <c r="E282" s="14"/>
       <c r="F282" s="4"/>
       <c r="G282" s="15"/>
       <c r="H282" s="14"/>
-      <c r="I282" s="23" t="s">
+      <c r="I282" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J282" s="18"/>
-      <c r="K282" s="18"/>
+      <c r="J282" s="20"/>
+      <c r="K282" s="20"/>
       <c r="L282" s="14"/>
       <c r="M282" s="4"/>
       <c r="N282" s="15"/>
@@ -7519,178 +7516,50 @@
     </row>
   </sheetData>
   <mergeCells count="250">
-    <mergeCell ref="C276:G276"/>
-    <mergeCell ref="J276:N276"/>
-    <mergeCell ref="B282:D282"/>
-    <mergeCell ref="I282:K282"/>
-    <mergeCell ref="B268:D268"/>
-    <mergeCell ref="I268:K268"/>
-    <mergeCell ref="C272:G272"/>
-    <mergeCell ref="J272:N272"/>
-    <mergeCell ref="C273:G273"/>
-    <mergeCell ref="J273:N273"/>
-    <mergeCell ref="C274:G274"/>
-    <mergeCell ref="J274:N274"/>
-    <mergeCell ref="C275:G275"/>
-    <mergeCell ref="J275:N275"/>
-    <mergeCell ref="C248:G248"/>
-    <mergeCell ref="J248:N248"/>
-    <mergeCell ref="B254:D254"/>
-    <mergeCell ref="I254:K254"/>
-    <mergeCell ref="B258:B262"/>
-    <mergeCell ref="C258:G258"/>
-    <mergeCell ref="J258:N258"/>
-    <mergeCell ref="C259:G259"/>
-    <mergeCell ref="J259:N259"/>
-    <mergeCell ref="C260:G260"/>
-    <mergeCell ref="J260:N260"/>
-    <mergeCell ref="C261:G261"/>
-    <mergeCell ref="J261:N261"/>
-    <mergeCell ref="C262:G262"/>
-    <mergeCell ref="J262:N262"/>
-    <mergeCell ref="B240:D240"/>
-    <mergeCell ref="I240:K240"/>
-    <mergeCell ref="C244:G244"/>
-    <mergeCell ref="J244:N244"/>
-    <mergeCell ref="C245:G245"/>
-    <mergeCell ref="J245:N245"/>
-    <mergeCell ref="C246:G246"/>
-    <mergeCell ref="J246:N246"/>
-    <mergeCell ref="C247:G247"/>
-    <mergeCell ref="J247:N247"/>
-    <mergeCell ref="B230:B234"/>
-    <mergeCell ref="C230:G230"/>
-    <mergeCell ref="J230:N230"/>
-    <mergeCell ref="C231:G231"/>
-    <mergeCell ref="J231:N231"/>
-    <mergeCell ref="C232:G232"/>
-    <mergeCell ref="J232:N232"/>
-    <mergeCell ref="C233:G233"/>
-    <mergeCell ref="J233:N233"/>
-    <mergeCell ref="C234:G234"/>
-    <mergeCell ref="J234:N234"/>
-    <mergeCell ref="C217:G217"/>
-    <mergeCell ref="J217:N217"/>
-    <mergeCell ref="C218:G218"/>
-    <mergeCell ref="J218:N218"/>
-    <mergeCell ref="C219:G219"/>
-    <mergeCell ref="J219:N219"/>
-    <mergeCell ref="C220:G220"/>
-    <mergeCell ref="J220:N220"/>
-    <mergeCell ref="B226:D226"/>
-    <mergeCell ref="I226:K226"/>
-    <mergeCell ref="B202:B206"/>
-    <mergeCell ref="J202:N202"/>
-    <mergeCell ref="J203:N203"/>
-    <mergeCell ref="J204:N204"/>
-    <mergeCell ref="J205:N205"/>
-    <mergeCell ref="J206:N206"/>
-    <mergeCell ref="B212:D212"/>
-    <mergeCell ref="I212:K212"/>
-    <mergeCell ref="C216:G216"/>
-    <mergeCell ref="J216:N216"/>
-    <mergeCell ref="C204:G204"/>
-    <mergeCell ref="C206:G206"/>
-    <mergeCell ref="C205:G205"/>
-    <mergeCell ref="C202:G202"/>
-    <mergeCell ref="C203:G203"/>
-    <mergeCell ref="B184:D184"/>
-    <mergeCell ref="I184:K184"/>
-    <mergeCell ref="C188:G188"/>
-    <mergeCell ref="J188:N188"/>
-    <mergeCell ref="C189:G189"/>
-    <mergeCell ref="C191:G191"/>
-    <mergeCell ref="C192:G192"/>
-    <mergeCell ref="J192:N192"/>
-    <mergeCell ref="B198:D198"/>
-    <mergeCell ref="I198:K198"/>
-    <mergeCell ref="C190:G190"/>
-    <mergeCell ref="J189:N189"/>
-    <mergeCell ref="C164:G164"/>
-    <mergeCell ref="J164:N164"/>
-    <mergeCell ref="B170:D170"/>
-    <mergeCell ref="I170:K170"/>
-    <mergeCell ref="B174:B178"/>
-    <mergeCell ref="C175:G175"/>
-    <mergeCell ref="C176:G176"/>
-    <mergeCell ref="C177:G177"/>
-    <mergeCell ref="C178:G178"/>
-    <mergeCell ref="J178:N178"/>
-    <mergeCell ref="B156:D156"/>
-    <mergeCell ref="I156:K156"/>
-    <mergeCell ref="C160:G160"/>
-    <mergeCell ref="J160:N160"/>
-    <mergeCell ref="C161:G161"/>
-    <mergeCell ref="J161:N161"/>
-    <mergeCell ref="C162:G162"/>
-    <mergeCell ref="J162:N162"/>
-    <mergeCell ref="C163:G163"/>
-    <mergeCell ref="J163:N163"/>
-    <mergeCell ref="B142:D142"/>
-    <mergeCell ref="I142:K142"/>
-    <mergeCell ref="B146:B150"/>
-    <mergeCell ref="C146:G146"/>
-    <mergeCell ref="J146:N146"/>
-    <mergeCell ref="C147:G147"/>
-    <mergeCell ref="J147:N147"/>
-    <mergeCell ref="C148:G148"/>
-    <mergeCell ref="J148:N148"/>
-    <mergeCell ref="C149:G149"/>
-    <mergeCell ref="J149:N149"/>
-    <mergeCell ref="C150:G150"/>
-    <mergeCell ref="J150:N150"/>
-    <mergeCell ref="C132:G132"/>
-    <mergeCell ref="J132:N132"/>
-    <mergeCell ref="C133:G133"/>
-    <mergeCell ref="J133:N133"/>
-    <mergeCell ref="C134:G134"/>
-    <mergeCell ref="J134:N134"/>
-    <mergeCell ref="C135:G135"/>
-    <mergeCell ref="J135:N135"/>
-    <mergeCell ref="C136:G136"/>
-    <mergeCell ref="J136:N136"/>
-    <mergeCell ref="B118:B122"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="J118:N118"/>
-    <mergeCell ref="C119:G119"/>
-    <mergeCell ref="J119:N119"/>
-    <mergeCell ref="J120:N120"/>
-    <mergeCell ref="C121:G121"/>
-    <mergeCell ref="B128:D128"/>
-    <mergeCell ref="I128:K128"/>
-    <mergeCell ref="B100:D100"/>
-    <mergeCell ref="I100:K100"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="J104:N104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="J105:N105"/>
-    <mergeCell ref="J106:N106"/>
-    <mergeCell ref="J108:N108"/>
-    <mergeCell ref="B114:D114"/>
-    <mergeCell ref="I114:K114"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="I86:K86"/>
-    <mergeCell ref="B90:B94"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="J90:N90"/>
-    <mergeCell ref="J91:N91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="J92:N92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="J93:N93"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="J94:N94"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="I72:K72"/>
-    <mergeCell ref="C77:G77"/>
-    <mergeCell ref="C78:G78"/>
-    <mergeCell ref="J78:N78"/>
-    <mergeCell ref="C79:G79"/>
-    <mergeCell ref="J79:N79"/>
-    <mergeCell ref="C80:G80"/>
-    <mergeCell ref="J80:N80"/>
-    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="C174:G174"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="J76:N76"/>
+    <mergeCell ref="C120:G120"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="J174:N174"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="J77:N77"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="J121:N121"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C62:G62"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="J63:N63"/>
+    <mergeCell ref="C64:G64"/>
+    <mergeCell ref="J64:N64"/>
+    <mergeCell ref="C65:G65"/>
+    <mergeCell ref="J65:N65"/>
+    <mergeCell ref="C66:G66"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="J50:N50"/>
+    <mergeCell ref="C51:G51"/>
+    <mergeCell ref="J51:N51"/>
+    <mergeCell ref="J66:N66"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="J20:N20"/>
     <mergeCell ref="J191:N191"/>
     <mergeCell ref="J176:N176"/>
     <mergeCell ref="J177:N177"/>
@@ -7715,17 +7584,6 @@
     <mergeCell ref="J49:N49"/>
     <mergeCell ref="J62:N62"/>
     <mergeCell ref="B34:B38"/>
-    <mergeCell ref="C65:G65"/>
-    <mergeCell ref="J65:N65"/>
-    <mergeCell ref="C66:G66"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="J50:N50"/>
-    <mergeCell ref="C51:G51"/>
-    <mergeCell ref="J51:N51"/>
-    <mergeCell ref="J66:N66"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="J20:N20"/>
     <mergeCell ref="C34:G34"/>
     <mergeCell ref="J34:N34"/>
     <mergeCell ref="C35:G35"/>
@@ -7736,39 +7594,178 @@
     <mergeCell ref="J37:N37"/>
     <mergeCell ref="C38:G38"/>
     <mergeCell ref="J38:N38"/>
-    <mergeCell ref="C62:G62"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="C63:G63"/>
-    <mergeCell ref="J63:N63"/>
-    <mergeCell ref="C64:G64"/>
-    <mergeCell ref="J64:N64"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="C174:G174"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="J76:N76"/>
-    <mergeCell ref="C120:G120"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="J174:N174"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="J77:N77"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="J121:N121"/>
-    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="I72:K72"/>
+    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="J78:N78"/>
+    <mergeCell ref="C79:G79"/>
+    <mergeCell ref="J79:N79"/>
+    <mergeCell ref="C80:G80"/>
+    <mergeCell ref="J80:N80"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="I86:K86"/>
+    <mergeCell ref="B90:B94"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="J90:N90"/>
+    <mergeCell ref="J91:N91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="J92:N92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="J93:N93"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="J94:N94"/>
+    <mergeCell ref="B100:D100"/>
+    <mergeCell ref="I100:K100"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="J104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="J105:N105"/>
+    <mergeCell ref="J106:N106"/>
+    <mergeCell ref="J108:N108"/>
+    <mergeCell ref="B114:D114"/>
+    <mergeCell ref="I114:K114"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="B118:B122"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="J118:N118"/>
+    <mergeCell ref="C119:G119"/>
+    <mergeCell ref="J119:N119"/>
+    <mergeCell ref="J120:N120"/>
+    <mergeCell ref="C121:G121"/>
+    <mergeCell ref="B128:D128"/>
+    <mergeCell ref="I128:K128"/>
+    <mergeCell ref="C132:G132"/>
+    <mergeCell ref="J132:N132"/>
+    <mergeCell ref="C133:G133"/>
+    <mergeCell ref="J133:N133"/>
+    <mergeCell ref="C134:G134"/>
+    <mergeCell ref="J134:N134"/>
+    <mergeCell ref="C135:G135"/>
+    <mergeCell ref="J135:N135"/>
+    <mergeCell ref="C136:G136"/>
+    <mergeCell ref="J136:N136"/>
+    <mergeCell ref="B142:D142"/>
+    <mergeCell ref="I142:K142"/>
+    <mergeCell ref="B146:B150"/>
+    <mergeCell ref="C146:G146"/>
+    <mergeCell ref="J146:N146"/>
+    <mergeCell ref="C147:G147"/>
+    <mergeCell ref="J147:N147"/>
+    <mergeCell ref="C148:G148"/>
+    <mergeCell ref="J148:N148"/>
+    <mergeCell ref="C149:G149"/>
+    <mergeCell ref="J149:N149"/>
+    <mergeCell ref="C150:G150"/>
+    <mergeCell ref="J150:N150"/>
+    <mergeCell ref="B156:D156"/>
+    <mergeCell ref="I156:K156"/>
+    <mergeCell ref="C160:G160"/>
+    <mergeCell ref="J160:N160"/>
+    <mergeCell ref="C161:G161"/>
+    <mergeCell ref="J161:N161"/>
+    <mergeCell ref="C162:G162"/>
+    <mergeCell ref="J162:N162"/>
+    <mergeCell ref="C163:G163"/>
+    <mergeCell ref="J163:N163"/>
+    <mergeCell ref="C164:G164"/>
+    <mergeCell ref="J164:N164"/>
+    <mergeCell ref="B170:D170"/>
+    <mergeCell ref="I170:K170"/>
+    <mergeCell ref="B174:B178"/>
+    <mergeCell ref="C175:G175"/>
+    <mergeCell ref="C176:G176"/>
+    <mergeCell ref="C177:G177"/>
+    <mergeCell ref="C178:G178"/>
+    <mergeCell ref="J178:N178"/>
+    <mergeCell ref="B184:D184"/>
+    <mergeCell ref="I184:K184"/>
+    <mergeCell ref="C188:G188"/>
+    <mergeCell ref="J188:N188"/>
+    <mergeCell ref="C189:G189"/>
+    <mergeCell ref="C191:G191"/>
+    <mergeCell ref="C192:G192"/>
+    <mergeCell ref="J192:N192"/>
+    <mergeCell ref="B198:D198"/>
+    <mergeCell ref="I198:K198"/>
+    <mergeCell ref="C190:G190"/>
+    <mergeCell ref="J189:N189"/>
+    <mergeCell ref="B202:B206"/>
+    <mergeCell ref="J202:N202"/>
+    <mergeCell ref="J203:N203"/>
+    <mergeCell ref="J204:N204"/>
+    <mergeCell ref="J205:N205"/>
+    <mergeCell ref="J206:N206"/>
+    <mergeCell ref="B212:D212"/>
+    <mergeCell ref="I212:K212"/>
+    <mergeCell ref="C216:G216"/>
+    <mergeCell ref="J216:N216"/>
+    <mergeCell ref="C204:G204"/>
+    <mergeCell ref="C206:G206"/>
+    <mergeCell ref="C205:G205"/>
+    <mergeCell ref="C202:G202"/>
+    <mergeCell ref="C203:G203"/>
+    <mergeCell ref="C217:G217"/>
+    <mergeCell ref="J217:N217"/>
+    <mergeCell ref="C218:G218"/>
+    <mergeCell ref="J218:N218"/>
+    <mergeCell ref="C219:G219"/>
+    <mergeCell ref="J219:N219"/>
+    <mergeCell ref="C220:G220"/>
+    <mergeCell ref="J220:N220"/>
+    <mergeCell ref="B226:D226"/>
+    <mergeCell ref="I226:K226"/>
+    <mergeCell ref="B230:B234"/>
+    <mergeCell ref="C230:G230"/>
+    <mergeCell ref="J230:N230"/>
+    <mergeCell ref="C231:G231"/>
+    <mergeCell ref="J231:N231"/>
+    <mergeCell ref="C232:G232"/>
+    <mergeCell ref="J232:N232"/>
+    <mergeCell ref="C233:G233"/>
+    <mergeCell ref="J233:N233"/>
+    <mergeCell ref="C234:G234"/>
+    <mergeCell ref="J234:N234"/>
+    <mergeCell ref="B240:D240"/>
+    <mergeCell ref="I240:K240"/>
+    <mergeCell ref="C244:G244"/>
+    <mergeCell ref="J244:N244"/>
+    <mergeCell ref="C245:G245"/>
+    <mergeCell ref="J245:N245"/>
+    <mergeCell ref="C246:G246"/>
+    <mergeCell ref="J246:N246"/>
+    <mergeCell ref="C247:G247"/>
+    <mergeCell ref="J247:N247"/>
+    <mergeCell ref="C248:G248"/>
+    <mergeCell ref="J248:N248"/>
+    <mergeCell ref="B254:D254"/>
+    <mergeCell ref="I254:K254"/>
+    <mergeCell ref="B258:B262"/>
+    <mergeCell ref="C258:G258"/>
+    <mergeCell ref="J258:N258"/>
+    <mergeCell ref="C259:G259"/>
+    <mergeCell ref="J259:N259"/>
+    <mergeCell ref="C260:G260"/>
+    <mergeCell ref="J260:N260"/>
+    <mergeCell ref="C261:G261"/>
+    <mergeCell ref="J261:N261"/>
+    <mergeCell ref="C262:G262"/>
+    <mergeCell ref="J262:N262"/>
+    <mergeCell ref="C276:G276"/>
+    <mergeCell ref="J276:N276"/>
+    <mergeCell ref="B282:D282"/>
+    <mergeCell ref="I282:K282"/>
+    <mergeCell ref="B268:D268"/>
+    <mergeCell ref="I268:K268"/>
+    <mergeCell ref="C272:G272"/>
+    <mergeCell ref="J272:N272"/>
+    <mergeCell ref="C273:G273"/>
+    <mergeCell ref="J273:N273"/>
+    <mergeCell ref="C274:G274"/>
+    <mergeCell ref="J274:N274"/>
+    <mergeCell ref="C275:G275"/>
+    <mergeCell ref="J275:N275"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
:sparkles: Seleção de Diretório
Adiciona funcionalidade de seleção de diretório

- Implementa a funcionalidade de permitir que o usuário selecione a pasta onde estão localizados os arquivos necessários para a automação.
- Verifica se os arquivos Lista Piloto-2024.xlsx e ModeloCarteirinha.xlsx existem na pasta selecionada.
- Exibe mensagens de erro caso os arquivos não sejam encontrados ou se nenhuma pasta for selecionada.
</commit_message>
<xml_diff>
--- a/ModeloCarteirinha.xlsx
+++ b/ModeloCarteirinha.xlsx
@@ -81,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +125,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -269,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -316,6 +340,37 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -333,6 +388,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -389,58 +471,6 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="666749" y="200025"/>
-          <a:ext cx="714375" cy="933450"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>657224</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2" descr="logo prefeitura.jpg">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="228599" y="200025"/>
           <a:ext cx="714375" cy="933450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2436,15 +2466,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>71628</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2468,8 +2498,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="228599" y="962025"/>
-          <a:ext cx="714375" cy="933450"/>
+          <a:off x="3771900" y="1024128"/>
+          <a:ext cx="542925" cy="709422"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6157,8 +6187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:R287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A264" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R274" sqref="R274"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6168,87 +6198,87 @@
     <col min="3" max="3" width="6.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
     <col min="7" max="7" width="4" customWidth="1"/>
     <col min="8" max="8" width="3" customWidth="1"/>
     <col min="9" max="9" width="10.140625" customWidth="1"/>
     <col min="10" max="10" width="5.42578125" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" customWidth="1"/>
     <col min="14" max="14" width="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="31"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="48"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="31"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="48"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="44"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="27"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="44"/>
     </row>
     <row r="8" spans="2:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="44"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="27"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="44"/>
     </row>
     <row r="9" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="29"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="46"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="29"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="56"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
@@ -6260,13 +6290,13 @@
       <c r="F10" s="14"/>
       <c r="G10" s="15"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="20" t="s">
+      <c r="J10" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="15"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="57"/>
     </row>
     <row r="11" spans="2:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
@@ -6399,75 +6429,75 @@
     <row r="19" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="31"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="30" t="s">
+      <c r="J20" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="31"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="48"/>
     </row>
     <row r="21" spans="2:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="27"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="44"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="26" t="s">
+      <c r="J21" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="27"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="44"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="44"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="26" t="s">
+      <c r="J22" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="27"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="44"/>
     </row>
     <row r="23" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="29"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="46"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="28" t="s">
+      <c r="J23" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="29"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="46"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
@@ -6617,78 +6647,78 @@
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="31"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="48"/>
       <c r="I34" s="6"/>
-      <c r="J34" s="30" t="s">
+      <c r="J34" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="31"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="48"/>
       <c r="O34" s="2"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
-      <c r="C35" s="26" t="s">
+      <c r="C35" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="27"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="44"/>
       <c r="I35" s="7"/>
-      <c r="J35" s="26" t="s">
+      <c r="J35" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K35" s="26"/>
-      <c r="L35" s="26"/>
-      <c r="M35" s="26"/>
-      <c r="N35" s="27"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="44"/>
       <c r="O35" s="2"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="27"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="44"/>
       <c r="I36" s="7"/>
-      <c r="J36" s="26" t="s">
+      <c r="J36" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
-      <c r="M36" s="26"/>
-      <c r="N36" s="27"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="44"/>
       <c r="O36" s="2"/>
     </row>
     <row r="37" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="29"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="46"/>
       <c r="I37" s="7"/>
-      <c r="J37" s="28" t="s">
+      <c r="J37" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="28"/>
-      <c r="N37" s="29"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
+      <c r="M37" s="45"/>
+      <c r="N37" s="46"/>
       <c r="O37" s="2"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
@@ -6851,78 +6881,78 @@
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
-      <c r="C48" s="30" t="s">
+      <c r="C48" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
-      <c r="G48" s="31"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="48"/>
       <c r="I48" s="6"/>
-      <c r="J48" s="30" t="s">
+      <c r="J48" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K48" s="30"/>
-      <c r="L48" s="30"/>
-      <c r="M48" s="30"/>
-      <c r="N48" s="31"/>
+      <c r="K48" s="47"/>
+      <c r="L48" s="47"/>
+      <c r="M48" s="47"/>
+      <c r="N48" s="48"/>
       <c r="O48" s="2"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="26" t="s">
+      <c r="C49" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="27"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="43"/>
+      <c r="G49" s="44"/>
       <c r="I49" s="7"/>
-      <c r="J49" s="26" t="s">
+      <c r="J49" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K49" s="26"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="26"/>
-      <c r="N49" s="27"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="43"/>
+      <c r="M49" s="43"/>
+      <c r="N49" s="44"/>
       <c r="O49" s="2"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="27"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="43"/>
+      <c r="G50" s="44"/>
       <c r="I50" s="7"/>
-      <c r="J50" s="26" t="s">
+      <c r="J50" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K50" s="26"/>
-      <c r="L50" s="26"/>
-      <c r="M50" s="26"/>
-      <c r="N50" s="27"/>
+      <c r="K50" s="43"/>
+      <c r="L50" s="43"/>
+      <c r="M50" s="43"/>
+      <c r="N50" s="44"/>
       <c r="O50" s="2"/>
     </row>
     <row r="51" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="7"/>
-      <c r="C51" s="28" t="s">
+      <c r="C51" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D51" s="28"/>
-      <c r="E51" s="28"/>
-      <c r="F51" s="28"/>
-      <c r="G51" s="29"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="46"/>
       <c r="I51" s="7"/>
-      <c r="J51" s="28" t="s">
+      <c r="J51" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K51" s="28"/>
-      <c r="L51" s="28"/>
-      <c r="M51" s="28"/>
-      <c r="N51" s="29"/>
+      <c r="K51" s="45"/>
+      <c r="L51" s="45"/>
+      <c r="M51" s="45"/>
+      <c r="N51" s="46"/>
       <c r="O51" s="2"/>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
@@ -7098,78 +7128,78 @@
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
-      <c r="C62" s="30" t="s">
+      <c r="C62" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="30"/>
-      <c r="G62" s="31"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="47"/>
+      <c r="F62" s="47"/>
+      <c r="G62" s="48"/>
       <c r="I62" s="6"/>
-      <c r="J62" s="30" t="s">
+      <c r="J62" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K62" s="30"/>
-      <c r="L62" s="30"/>
-      <c r="M62" s="30"/>
-      <c r="N62" s="31"/>
+      <c r="K62" s="47"/>
+      <c r="L62" s="47"/>
+      <c r="M62" s="47"/>
+      <c r="N62" s="48"/>
       <c r="O62" s="2"/>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
-      <c r="C63" s="26" t="s">
+      <c r="C63" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D63" s="26"/>
-      <c r="E63" s="26"/>
-      <c r="F63" s="26"/>
-      <c r="G63" s="27"/>
+      <c r="D63" s="43"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="43"/>
+      <c r="G63" s="44"/>
       <c r="I63" s="7"/>
-      <c r="J63" s="26" t="s">
+      <c r="J63" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K63" s="26"/>
-      <c r="L63" s="26"/>
-      <c r="M63" s="26"/>
-      <c r="N63" s="27"/>
+      <c r="K63" s="43"/>
+      <c r="L63" s="43"/>
+      <c r="M63" s="43"/>
+      <c r="N63" s="44"/>
       <c r="O63" s="2"/>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B64" s="7"/>
-      <c r="C64" s="26" t="s">
+      <c r="C64" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="26"/>
-      <c r="E64" s="26"/>
-      <c r="F64" s="26"/>
-      <c r="G64" s="27"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="43"/>
+      <c r="G64" s="44"/>
       <c r="I64" s="7"/>
-      <c r="J64" s="26" t="s">
+      <c r="J64" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K64" s="26"/>
-      <c r="L64" s="26"/>
-      <c r="M64" s="26"/>
-      <c r="N64" s="27"/>
+      <c r="K64" s="43"/>
+      <c r="L64" s="43"/>
+      <c r="M64" s="43"/>
+      <c r="N64" s="44"/>
       <c r="O64" s="2"/>
     </row>
     <row r="65" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="7"/>
-      <c r="C65" s="28" t="s">
+      <c r="C65" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="28"/>
-      <c r="E65" s="28"/>
-      <c r="F65" s="28"/>
-      <c r="G65" s="29"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
+      <c r="F65" s="45"/>
+      <c r="G65" s="46"/>
       <c r="I65" s="7"/>
-      <c r="J65" s="28" t="s">
+      <c r="J65" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K65" s="28"/>
-      <c r="L65" s="28"/>
-      <c r="M65" s="28"/>
-      <c r="N65" s="29"/>
+      <c r="K65" s="45"/>
+      <c r="L65" s="45"/>
+      <c r="M65" s="45"/>
+      <c r="N65" s="46"/>
       <c r="O65" s="2"/>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
@@ -7332,78 +7362,78 @@
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
-      <c r="C76" s="30" t="s">
+      <c r="C76" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30"/>
-      <c r="F76" s="30"/>
-      <c r="G76" s="31"/>
+      <c r="D76" s="47"/>
+      <c r="E76" s="47"/>
+      <c r="F76" s="47"/>
+      <c r="G76" s="48"/>
       <c r="I76" s="6"/>
-      <c r="J76" s="30" t="s">
+      <c r="J76" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K76" s="30"/>
-      <c r="L76" s="30"/>
-      <c r="M76" s="30"/>
-      <c r="N76" s="31"/>
+      <c r="K76" s="47"/>
+      <c r="L76" s="47"/>
+      <c r="M76" s="47"/>
+      <c r="N76" s="48"/>
       <c r="O76" s="2"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B77" s="7"/>
-      <c r="C77" s="26" t="s">
+      <c r="C77" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D77" s="26"/>
-      <c r="E77" s="26"/>
-      <c r="F77" s="26"/>
-      <c r="G77" s="27"/>
+      <c r="D77" s="43"/>
+      <c r="E77" s="43"/>
+      <c r="F77" s="43"/>
+      <c r="G77" s="44"/>
       <c r="I77" s="7"/>
-      <c r="J77" s="26" t="s">
+      <c r="J77" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K77" s="26"/>
-      <c r="L77" s="26"/>
-      <c r="M77" s="26"/>
-      <c r="N77" s="27"/>
+      <c r="K77" s="43"/>
+      <c r="L77" s="43"/>
+      <c r="M77" s="43"/>
+      <c r="N77" s="44"/>
       <c r="O77" s="2"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B78" s="7"/>
-      <c r="C78" s="26" t="s">
+      <c r="C78" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D78" s="26"/>
-      <c r="E78" s="26"/>
-      <c r="F78" s="26"/>
-      <c r="G78" s="27"/>
+      <c r="D78" s="43"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="43"/>
+      <c r="G78" s="44"/>
       <c r="I78" s="7"/>
-      <c r="J78" s="26" t="s">
+      <c r="J78" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K78" s="26"/>
-      <c r="L78" s="26"/>
-      <c r="M78" s="26"/>
-      <c r="N78" s="27"/>
+      <c r="K78" s="43"/>
+      <c r="L78" s="43"/>
+      <c r="M78" s="43"/>
+      <c r="N78" s="44"/>
       <c r="O78" s="2"/>
     </row>
     <row r="79" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="7"/>
-      <c r="C79" s="28" t="s">
+      <c r="C79" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D79" s="28"/>
-      <c r="E79" s="28"/>
-      <c r="F79" s="28"/>
-      <c r="G79" s="29"/>
+      <c r="D79" s="45"/>
+      <c r="E79" s="45"/>
+      <c r="F79" s="45"/>
+      <c r="G79" s="46"/>
       <c r="I79" s="7"/>
-      <c r="J79" s="28" t="s">
+      <c r="J79" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K79" s="28"/>
-      <c r="L79" s="28"/>
-      <c r="M79" s="28"/>
-      <c r="N79" s="29"/>
+      <c r="K79" s="45"/>
+      <c r="L79" s="45"/>
+      <c r="M79" s="45"/>
+      <c r="N79" s="46"/>
       <c r="O79" s="2"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
@@ -7579,78 +7609,78 @@
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B90" s="6"/>
-      <c r="C90" s="30" t="s">
+      <c r="C90" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D90" s="30"/>
-      <c r="E90" s="30"/>
-      <c r="F90" s="30"/>
-      <c r="G90" s="31"/>
+      <c r="D90" s="47"/>
+      <c r="E90" s="47"/>
+      <c r="F90" s="47"/>
+      <c r="G90" s="48"/>
       <c r="I90" s="6"/>
-      <c r="J90" s="30" t="s">
+      <c r="J90" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K90" s="30"/>
-      <c r="L90" s="30"/>
-      <c r="M90" s="30"/>
-      <c r="N90" s="31"/>
+      <c r="K90" s="47"/>
+      <c r="L90" s="47"/>
+      <c r="M90" s="47"/>
+      <c r="N90" s="48"/>
       <c r="O90" s="2"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B91" s="7"/>
-      <c r="C91" s="26" t="s">
+      <c r="C91" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D91" s="26"/>
-      <c r="E91" s="26"/>
-      <c r="F91" s="26"/>
-      <c r="G91" s="27"/>
+      <c r="D91" s="43"/>
+      <c r="E91" s="43"/>
+      <c r="F91" s="43"/>
+      <c r="G91" s="44"/>
       <c r="I91" s="7"/>
-      <c r="J91" s="26" t="s">
+      <c r="J91" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K91" s="26"/>
-      <c r="L91" s="26"/>
-      <c r="M91" s="26"/>
-      <c r="N91" s="27"/>
+      <c r="K91" s="43"/>
+      <c r="L91" s="43"/>
+      <c r="M91" s="43"/>
+      <c r="N91" s="44"/>
       <c r="O91" s="2"/>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B92" s="7"/>
-      <c r="C92" s="26" t="s">
+      <c r="C92" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D92" s="26"/>
-      <c r="E92" s="26"/>
-      <c r="F92" s="26"/>
-      <c r="G92" s="27"/>
+      <c r="D92" s="43"/>
+      <c r="E92" s="43"/>
+      <c r="F92" s="43"/>
+      <c r="G92" s="44"/>
       <c r="I92" s="7"/>
-      <c r="J92" s="26" t="s">
+      <c r="J92" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K92" s="26"/>
-      <c r="L92" s="26"/>
-      <c r="M92" s="26"/>
-      <c r="N92" s="27"/>
+      <c r="K92" s="43"/>
+      <c r="L92" s="43"/>
+      <c r="M92" s="43"/>
+      <c r="N92" s="44"/>
       <c r="O92" s="2"/>
     </row>
     <row r="93" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="7"/>
-      <c r="C93" s="28" t="s">
+      <c r="C93" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D93" s="28"/>
-      <c r="E93" s="28"/>
-      <c r="F93" s="28"/>
-      <c r="G93" s="29"/>
+      <c r="D93" s="45"/>
+      <c r="E93" s="45"/>
+      <c r="F93" s="45"/>
+      <c r="G93" s="46"/>
       <c r="I93" s="7"/>
-      <c r="J93" s="28" t="s">
+      <c r="J93" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K93" s="28"/>
-      <c r="L93" s="28"/>
-      <c r="M93" s="28"/>
-      <c r="N93" s="29"/>
+      <c r="K93" s="45"/>
+      <c r="L93" s="45"/>
+      <c r="M93" s="45"/>
+      <c r="N93" s="46"/>
       <c r="O93" s="2"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
@@ -7813,78 +7843,78 @@
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104" s="6"/>
-      <c r="C104" s="30" t="s">
+      <c r="C104" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D104" s="30"/>
-      <c r="E104" s="30"/>
-      <c r="F104" s="30"/>
-      <c r="G104" s="31"/>
+      <c r="D104" s="47"/>
+      <c r="E104" s="47"/>
+      <c r="F104" s="47"/>
+      <c r="G104" s="48"/>
       <c r="I104" s="6"/>
-      <c r="J104" s="30" t="s">
+      <c r="J104" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K104" s="30"/>
-      <c r="L104" s="30"/>
-      <c r="M104" s="30"/>
-      <c r="N104" s="31"/>
+      <c r="K104" s="47"/>
+      <c r="L104" s="47"/>
+      <c r="M104" s="47"/>
+      <c r="N104" s="48"/>
       <c r="O104" s="2"/>
     </row>
     <row r="105" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="7"/>
-      <c r="C105" s="26" t="s">
+      <c r="C105" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D105" s="26"/>
-      <c r="E105" s="26"/>
-      <c r="F105" s="26"/>
-      <c r="G105" s="27"/>
+      <c r="D105" s="43"/>
+      <c r="E105" s="43"/>
+      <c r="F105" s="43"/>
+      <c r="G105" s="44"/>
       <c r="I105" s="7"/>
-      <c r="J105" s="26" t="s">
+      <c r="J105" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K105" s="26"/>
-      <c r="L105" s="26"/>
-      <c r="M105" s="26"/>
-      <c r="N105" s="27"/>
+      <c r="K105" s="43"/>
+      <c r="L105" s="43"/>
+      <c r="M105" s="43"/>
+      <c r="N105" s="44"/>
       <c r="O105" s="2"/>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106" s="7"/>
-      <c r="C106" s="26" t="s">
+      <c r="C106" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D106" s="26"/>
-      <c r="E106" s="26"/>
-      <c r="F106" s="26"/>
-      <c r="G106" s="27"/>
+      <c r="D106" s="43"/>
+      <c r="E106" s="43"/>
+      <c r="F106" s="43"/>
+      <c r="G106" s="44"/>
       <c r="I106" s="7"/>
-      <c r="J106" s="26" t="s">
+      <c r="J106" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K106" s="26"/>
-      <c r="L106" s="26"/>
-      <c r="M106" s="26"/>
-      <c r="N106" s="27"/>
+      <c r="K106" s="43"/>
+      <c r="L106" s="43"/>
+      <c r="M106" s="43"/>
+      <c r="N106" s="44"/>
       <c r="O106" s="2"/>
     </row>
     <row r="107" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="7"/>
-      <c r="C107" s="28" t="s">
+      <c r="C107" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D107" s="28"/>
-      <c r="E107" s="28"/>
-      <c r="F107" s="28"/>
-      <c r="G107" s="29"/>
+      <c r="D107" s="45"/>
+      <c r="E107" s="45"/>
+      <c r="F107" s="45"/>
+      <c r="G107" s="46"/>
       <c r="I107" s="7"/>
-      <c r="J107" s="28" t="s">
+      <c r="J107" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K107" s="28"/>
-      <c r="L107" s="28"/>
-      <c r="M107" s="28"/>
-      <c r="N107" s="29"/>
+      <c r="K107" s="45"/>
+      <c r="L107" s="45"/>
+      <c r="M107" s="45"/>
+      <c r="N107" s="46"/>
       <c r="O107" s="2"/>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
@@ -8044,94 +8074,94 @@
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B117" s="2"/>
-      <c r="C117" s="26"/>
-      <c r="D117" s="26"/>
-      <c r="E117" s="26"/>
-      <c r="F117" s="26"/>
-      <c r="G117" s="26"/>
+      <c r="C117" s="43"/>
+      <c r="D117" s="43"/>
+      <c r="E117" s="43"/>
+      <c r="F117" s="43"/>
+      <c r="G117" s="43"/>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
-      <c r="J117" s="26"/>
-      <c r="K117" s="26"/>
-      <c r="L117" s="26"/>
-      <c r="M117" s="26"/>
-      <c r="N117" s="26"/>
+      <c r="J117" s="43"/>
+      <c r="K117" s="43"/>
+      <c r="L117" s="43"/>
+      <c r="M117" s="43"/>
+      <c r="N117" s="43"/>
       <c r="O117" s="2"/>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B118" s="6"/>
-      <c r="C118" s="30" t="s">
+      <c r="C118" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D118" s="30"/>
-      <c r="E118" s="30"/>
-      <c r="F118" s="30"/>
-      <c r="G118" s="31"/>
+      <c r="D118" s="47"/>
+      <c r="E118" s="47"/>
+      <c r="F118" s="47"/>
+      <c r="G118" s="48"/>
       <c r="I118" s="6"/>
-      <c r="J118" s="30" t="s">
+      <c r="J118" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K118" s="30"/>
-      <c r="L118" s="30"/>
-      <c r="M118" s="30"/>
-      <c r="N118" s="31"/>
+      <c r="K118" s="47"/>
+      <c r="L118" s="47"/>
+      <c r="M118" s="47"/>
+      <c r="N118" s="48"/>
       <c r="O118" s="2"/>
     </row>
     <row r="119" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="7"/>
-      <c r="C119" s="26" t="s">
+      <c r="C119" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D119" s="26"/>
-      <c r="E119" s="26"/>
-      <c r="F119" s="26"/>
-      <c r="G119" s="27"/>
+      <c r="D119" s="43"/>
+      <c r="E119" s="43"/>
+      <c r="F119" s="43"/>
+      <c r="G119" s="44"/>
       <c r="I119" s="7"/>
-      <c r="J119" s="26" t="s">
+      <c r="J119" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K119" s="26"/>
-      <c r="L119" s="26"/>
-      <c r="M119" s="26"/>
-      <c r="N119" s="27"/>
+      <c r="K119" s="43"/>
+      <c r="L119" s="43"/>
+      <c r="M119" s="43"/>
+      <c r="N119" s="44"/>
       <c r="O119" s="2"/>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B120" s="7"/>
-      <c r="C120" s="26" t="s">
+      <c r="C120" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D120" s="26"/>
-      <c r="E120" s="26"/>
-      <c r="F120" s="26"/>
-      <c r="G120" s="27"/>
+      <c r="D120" s="43"/>
+      <c r="E120" s="43"/>
+      <c r="F120" s="43"/>
+      <c r="G120" s="44"/>
       <c r="I120" s="7"/>
-      <c r="J120" s="26" t="s">
+      <c r="J120" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K120" s="26"/>
-      <c r="L120" s="26"/>
-      <c r="M120" s="26"/>
-      <c r="N120" s="27"/>
+      <c r="K120" s="43"/>
+      <c r="L120" s="43"/>
+      <c r="M120" s="43"/>
+      <c r="N120" s="44"/>
       <c r="O120" s="2"/>
     </row>
     <row r="121" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="7"/>
-      <c r="C121" s="28" t="s">
+      <c r="C121" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D121" s="28"/>
-      <c r="E121" s="28"/>
-      <c r="F121" s="28"/>
-      <c r="G121" s="29"/>
+      <c r="D121" s="45"/>
+      <c r="E121" s="45"/>
+      <c r="F121" s="45"/>
+      <c r="G121" s="46"/>
       <c r="I121" s="7"/>
-      <c r="J121" s="28" t="s">
+      <c r="J121" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K121" s="28"/>
-      <c r="L121" s="28"/>
-      <c r="M121" s="28"/>
-      <c r="N121" s="29"/>
+      <c r="K121" s="45"/>
+      <c r="L121" s="45"/>
+      <c r="M121" s="45"/>
+      <c r="N121" s="46"/>
       <c r="O121" s="2"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
@@ -8294,78 +8324,78 @@
     </row>
     <row r="132" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
-      <c r="C132" s="30" t="s">
+      <c r="C132" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D132" s="30"/>
-      <c r="E132" s="30"/>
-      <c r="F132" s="30"/>
-      <c r="G132" s="31"/>
+      <c r="D132" s="47"/>
+      <c r="E132" s="47"/>
+      <c r="F132" s="47"/>
+      <c r="G132" s="48"/>
       <c r="I132" s="6"/>
-      <c r="J132" s="30" t="s">
+      <c r="J132" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K132" s="30"/>
-      <c r="L132" s="30"/>
-      <c r="M132" s="30"/>
-      <c r="N132" s="31"/>
+      <c r="K132" s="47"/>
+      <c r="L132" s="47"/>
+      <c r="M132" s="47"/>
+      <c r="N132" s="48"/>
       <c r="O132" s="2"/>
     </row>
     <row r="133" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B133" s="7"/>
-      <c r="C133" s="26" t="s">
+      <c r="C133" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D133" s="26"/>
-      <c r="E133" s="26"/>
-      <c r="F133" s="26"/>
-      <c r="G133" s="27"/>
+      <c r="D133" s="43"/>
+      <c r="E133" s="43"/>
+      <c r="F133" s="43"/>
+      <c r="G133" s="44"/>
       <c r="I133" s="7"/>
-      <c r="J133" s="26" t="s">
+      <c r="J133" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K133" s="26"/>
-      <c r="L133" s="26"/>
-      <c r="M133" s="26"/>
-      <c r="N133" s="27"/>
+      <c r="K133" s="43"/>
+      <c r="L133" s="43"/>
+      <c r="M133" s="43"/>
+      <c r="N133" s="44"/>
       <c r="O133" s="2"/>
     </row>
     <row r="134" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B134" s="7"/>
-      <c r="C134" s="26" t="s">
+      <c r="C134" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D134" s="26"/>
-      <c r="E134" s="26"/>
-      <c r="F134" s="26"/>
-      <c r="G134" s="27"/>
+      <c r="D134" s="43"/>
+      <c r="E134" s="43"/>
+      <c r="F134" s="43"/>
+      <c r="G134" s="44"/>
       <c r="I134" s="7"/>
-      <c r="J134" s="26" t="s">
+      <c r="J134" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K134" s="26"/>
-      <c r="L134" s="26"/>
-      <c r="M134" s="26"/>
-      <c r="N134" s="27"/>
+      <c r="K134" s="43"/>
+      <c r="L134" s="43"/>
+      <c r="M134" s="43"/>
+      <c r="N134" s="44"/>
       <c r="O134" s="2"/>
     </row>
     <row r="135" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="7"/>
-      <c r="C135" s="28" t="s">
+      <c r="C135" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D135" s="28"/>
-      <c r="E135" s="28"/>
-      <c r="F135" s="28"/>
-      <c r="G135" s="29"/>
+      <c r="D135" s="45"/>
+      <c r="E135" s="45"/>
+      <c r="F135" s="45"/>
+      <c r="G135" s="46"/>
       <c r="I135" s="7"/>
-      <c r="J135" s="28" t="s">
+      <c r="J135" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K135" s="28"/>
-      <c r="L135" s="28"/>
-      <c r="M135" s="28"/>
-      <c r="N135" s="29"/>
+      <c r="K135" s="45"/>
+      <c r="L135" s="45"/>
+      <c r="M135" s="45"/>
+      <c r="N135" s="46"/>
       <c r="O135" s="2"/>
     </row>
     <row r="136" spans="2:15" x14ac:dyDescent="0.25">
@@ -8541,78 +8571,78 @@
     </row>
     <row r="146" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B146" s="6"/>
-      <c r="C146" s="30" t="s">
+      <c r="C146" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D146" s="30"/>
-      <c r="E146" s="30"/>
-      <c r="F146" s="30"/>
-      <c r="G146" s="31"/>
+      <c r="D146" s="47"/>
+      <c r="E146" s="47"/>
+      <c r="F146" s="47"/>
+      <c r="G146" s="48"/>
       <c r="I146" s="6"/>
-      <c r="J146" s="30" t="s">
+      <c r="J146" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K146" s="30"/>
-      <c r="L146" s="30"/>
-      <c r="M146" s="30"/>
-      <c r="N146" s="31"/>
+      <c r="K146" s="47"/>
+      <c r="L146" s="47"/>
+      <c r="M146" s="47"/>
+      <c r="N146" s="48"/>
       <c r="O146" s="2"/>
     </row>
     <row r="147" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B147" s="7"/>
-      <c r="C147" s="26" t="s">
+      <c r="C147" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D147" s="26"/>
-      <c r="E147" s="26"/>
-      <c r="F147" s="26"/>
-      <c r="G147" s="27"/>
+      <c r="D147" s="43"/>
+      <c r="E147" s="43"/>
+      <c r="F147" s="43"/>
+      <c r="G147" s="44"/>
       <c r="I147" s="7"/>
-      <c r="J147" s="26" t="s">
+      <c r="J147" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K147" s="26"/>
-      <c r="L147" s="26"/>
-      <c r="M147" s="26"/>
-      <c r="N147" s="27"/>
+      <c r="K147" s="43"/>
+      <c r="L147" s="43"/>
+      <c r="M147" s="43"/>
+      <c r="N147" s="44"/>
       <c r="O147" s="2"/>
     </row>
     <row r="148" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B148" s="7"/>
-      <c r="C148" s="26" t="s">
+      <c r="C148" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D148" s="26"/>
-      <c r="E148" s="26"/>
-      <c r="F148" s="26"/>
-      <c r="G148" s="27"/>
+      <c r="D148" s="43"/>
+      <c r="E148" s="43"/>
+      <c r="F148" s="43"/>
+      <c r="G148" s="44"/>
       <c r="I148" s="7"/>
-      <c r="J148" s="26" t="s">
+      <c r="J148" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K148" s="26"/>
-      <c r="L148" s="26"/>
-      <c r="M148" s="26"/>
-      <c r="N148" s="27"/>
+      <c r="K148" s="43"/>
+      <c r="L148" s="43"/>
+      <c r="M148" s="43"/>
+      <c r="N148" s="44"/>
       <c r="O148" s="2"/>
     </row>
     <row r="149" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="7"/>
-      <c r="C149" s="28" t="s">
+      <c r="C149" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D149" s="28"/>
-      <c r="E149" s="28"/>
-      <c r="F149" s="28"/>
-      <c r="G149" s="29"/>
+      <c r="D149" s="45"/>
+      <c r="E149" s="45"/>
+      <c r="F149" s="45"/>
+      <c r="G149" s="46"/>
       <c r="I149" s="7"/>
-      <c r="J149" s="28" t="s">
+      <c r="J149" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K149" s="28"/>
-      <c r="L149" s="28"/>
-      <c r="M149" s="28"/>
-      <c r="N149" s="29"/>
+      <c r="K149" s="45"/>
+      <c r="L149" s="45"/>
+      <c r="M149" s="45"/>
+      <c r="N149" s="46"/>
       <c r="O149" s="2"/>
     </row>
     <row r="150" spans="2:15" x14ac:dyDescent="0.25">
@@ -8775,78 +8805,78 @@
     </row>
     <row r="160" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
-      <c r="C160" s="30" t="s">
+      <c r="C160" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D160" s="30"/>
-      <c r="E160" s="30"/>
-      <c r="F160" s="30"/>
-      <c r="G160" s="31"/>
+      <c r="D160" s="47"/>
+      <c r="E160" s="47"/>
+      <c r="F160" s="47"/>
+      <c r="G160" s="48"/>
       <c r="I160" s="6"/>
-      <c r="J160" s="30" t="s">
+      <c r="J160" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K160" s="30"/>
-      <c r="L160" s="30"/>
-      <c r="M160" s="30"/>
-      <c r="N160" s="31"/>
+      <c r="K160" s="47"/>
+      <c r="L160" s="47"/>
+      <c r="M160" s="47"/>
+      <c r="N160" s="48"/>
       <c r="O160" s="2"/>
     </row>
     <row r="161" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B161" s="7"/>
-      <c r="C161" s="26" t="s">
+      <c r="C161" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D161" s="26"/>
-      <c r="E161" s="26"/>
-      <c r="F161" s="26"/>
-      <c r="G161" s="27"/>
+      <c r="D161" s="43"/>
+      <c r="E161" s="43"/>
+      <c r="F161" s="43"/>
+      <c r="G161" s="44"/>
       <c r="I161" s="7"/>
-      <c r="J161" s="26" t="s">
+      <c r="J161" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K161" s="26"/>
-      <c r="L161" s="26"/>
-      <c r="M161" s="26"/>
-      <c r="N161" s="27"/>
+      <c r="K161" s="43"/>
+      <c r="L161" s="43"/>
+      <c r="M161" s="43"/>
+      <c r="N161" s="44"/>
       <c r="O161" s="2"/>
     </row>
     <row r="162" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B162" s="7"/>
-      <c r="C162" s="26" t="s">
+      <c r="C162" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D162" s="26"/>
-      <c r="E162" s="26"/>
-      <c r="F162" s="26"/>
-      <c r="G162" s="27"/>
+      <c r="D162" s="43"/>
+      <c r="E162" s="43"/>
+      <c r="F162" s="43"/>
+      <c r="G162" s="44"/>
       <c r="I162" s="7"/>
-      <c r="J162" s="26" t="s">
+      <c r="J162" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K162" s="26"/>
-      <c r="L162" s="26"/>
-      <c r="M162" s="26"/>
-      <c r="N162" s="27"/>
+      <c r="K162" s="43"/>
+      <c r="L162" s="43"/>
+      <c r="M162" s="43"/>
+      <c r="N162" s="44"/>
       <c r="O162" s="2"/>
     </row>
     <row r="163" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="7"/>
-      <c r="C163" s="28" t="s">
+      <c r="C163" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D163" s="28"/>
-      <c r="E163" s="28"/>
-      <c r="F163" s="28"/>
-      <c r="G163" s="29"/>
+      <c r="D163" s="45"/>
+      <c r="E163" s="45"/>
+      <c r="F163" s="45"/>
+      <c r="G163" s="46"/>
       <c r="I163" s="7"/>
-      <c r="J163" s="28" t="s">
+      <c r="J163" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K163" s="28"/>
-      <c r="L163" s="28"/>
-      <c r="M163" s="28"/>
-      <c r="N163" s="29"/>
+      <c r="K163" s="45"/>
+      <c r="L163" s="45"/>
+      <c r="M163" s="45"/>
+      <c r="N163" s="46"/>
       <c r="O163" s="2"/>
     </row>
     <row r="164" spans="2:15" x14ac:dyDescent="0.25">
@@ -9022,78 +9052,78 @@
     </row>
     <row r="174" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B174" s="6"/>
-      <c r="C174" s="30" t="s">
+      <c r="C174" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D174" s="30"/>
-      <c r="E174" s="30"/>
-      <c r="F174" s="30"/>
-      <c r="G174" s="31"/>
+      <c r="D174" s="47"/>
+      <c r="E174" s="47"/>
+      <c r="F174" s="47"/>
+      <c r="G174" s="48"/>
       <c r="I174" s="6"/>
-      <c r="J174" s="30" t="s">
+      <c r="J174" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K174" s="30"/>
-      <c r="L174" s="30"/>
-      <c r="M174" s="30"/>
-      <c r="N174" s="31"/>
+      <c r="K174" s="47"/>
+      <c r="L174" s="47"/>
+      <c r="M174" s="47"/>
+      <c r="N174" s="48"/>
       <c r="O174" s="2"/>
     </row>
     <row r="175" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B175" s="7"/>
-      <c r="C175" s="26" t="s">
+      <c r="C175" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D175" s="26"/>
-      <c r="E175" s="26"/>
-      <c r="F175" s="26"/>
-      <c r="G175" s="27"/>
+      <c r="D175" s="43"/>
+      <c r="E175" s="43"/>
+      <c r="F175" s="43"/>
+      <c r="G175" s="44"/>
       <c r="I175" s="7"/>
-      <c r="J175" s="26" t="s">
+      <c r="J175" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K175" s="26"/>
-      <c r="L175" s="26"/>
-      <c r="M175" s="26"/>
-      <c r="N175" s="27"/>
+      <c r="K175" s="43"/>
+      <c r="L175" s="43"/>
+      <c r="M175" s="43"/>
+      <c r="N175" s="44"/>
       <c r="O175" s="2"/>
     </row>
     <row r="176" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B176" s="7"/>
-      <c r="C176" s="26" t="s">
+      <c r="C176" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D176" s="26"/>
-      <c r="E176" s="26"/>
-      <c r="F176" s="26"/>
-      <c r="G176" s="27"/>
+      <c r="D176" s="43"/>
+      <c r="E176" s="43"/>
+      <c r="F176" s="43"/>
+      <c r="G176" s="44"/>
       <c r="I176" s="7"/>
-      <c r="J176" s="26" t="s">
+      <c r="J176" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K176" s="26"/>
-      <c r="L176" s="26"/>
-      <c r="M176" s="26"/>
-      <c r="N176" s="27"/>
+      <c r="K176" s="43"/>
+      <c r="L176" s="43"/>
+      <c r="M176" s="43"/>
+      <c r="N176" s="44"/>
       <c r="O176" s="2"/>
     </row>
     <row r="177" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="7"/>
-      <c r="C177" s="28" t="s">
+      <c r="C177" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D177" s="28"/>
-      <c r="E177" s="28"/>
-      <c r="F177" s="28"/>
-      <c r="G177" s="29"/>
+      <c r="D177" s="45"/>
+      <c r="E177" s="45"/>
+      <c r="F177" s="45"/>
+      <c r="G177" s="46"/>
       <c r="I177" s="7"/>
-      <c r="J177" s="28" t="s">
+      <c r="J177" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K177" s="28"/>
-      <c r="L177" s="28"/>
-      <c r="M177" s="28"/>
-      <c r="N177" s="29"/>
+      <c r="K177" s="45"/>
+      <c r="L177" s="45"/>
+      <c r="M177" s="45"/>
+      <c r="N177" s="46"/>
       <c r="O177" s="2"/>
     </row>
     <row r="178" spans="2:15" x14ac:dyDescent="0.25">
@@ -9256,78 +9286,78 @@
     </row>
     <row r="188" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
-      <c r="C188" s="30" t="s">
+      <c r="C188" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D188" s="30"/>
-      <c r="E188" s="30"/>
-      <c r="F188" s="30"/>
-      <c r="G188" s="31"/>
+      <c r="D188" s="47"/>
+      <c r="E188" s="47"/>
+      <c r="F188" s="47"/>
+      <c r="G188" s="48"/>
       <c r="I188" s="6"/>
-      <c r="J188" s="30" t="s">
+      <c r="J188" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K188" s="30"/>
-      <c r="L188" s="30"/>
-      <c r="M188" s="30"/>
-      <c r="N188" s="31"/>
+      <c r="K188" s="47"/>
+      <c r="L188" s="47"/>
+      <c r="M188" s="47"/>
+      <c r="N188" s="48"/>
       <c r="O188" s="2"/>
     </row>
     <row r="189" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B189" s="7"/>
-      <c r="C189" s="26" t="s">
+      <c r="C189" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D189" s="26"/>
-      <c r="E189" s="26"/>
-      <c r="F189" s="26"/>
-      <c r="G189" s="27"/>
+      <c r="D189" s="43"/>
+      <c r="E189" s="43"/>
+      <c r="F189" s="43"/>
+      <c r="G189" s="44"/>
       <c r="I189" s="7"/>
-      <c r="J189" s="26" t="s">
+      <c r="J189" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K189" s="26"/>
-      <c r="L189" s="26"/>
-      <c r="M189" s="26"/>
-      <c r="N189" s="27"/>
+      <c r="K189" s="43"/>
+      <c r="L189" s="43"/>
+      <c r="M189" s="43"/>
+      <c r="N189" s="44"/>
       <c r="O189" s="2"/>
     </row>
     <row r="190" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B190" s="7"/>
-      <c r="C190" s="26" t="s">
+      <c r="C190" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D190" s="26"/>
-      <c r="E190" s="26"/>
-      <c r="F190" s="26"/>
-      <c r="G190" s="27"/>
+      <c r="D190" s="43"/>
+      <c r="E190" s="43"/>
+      <c r="F190" s="43"/>
+      <c r="G190" s="44"/>
       <c r="I190" s="7"/>
-      <c r="J190" s="26" t="s">
+      <c r="J190" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K190" s="26"/>
-      <c r="L190" s="26"/>
-      <c r="M190" s="26"/>
-      <c r="N190" s="27"/>
+      <c r="K190" s="43"/>
+      <c r="L190" s="43"/>
+      <c r="M190" s="43"/>
+      <c r="N190" s="44"/>
       <c r="O190" s="2"/>
     </row>
     <row r="191" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" s="7"/>
-      <c r="C191" s="28" t="s">
+      <c r="C191" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D191" s="28"/>
-      <c r="E191" s="28"/>
-      <c r="F191" s="28"/>
-      <c r="G191" s="29"/>
+      <c r="D191" s="45"/>
+      <c r="E191" s="45"/>
+      <c r="F191" s="45"/>
+      <c r="G191" s="46"/>
       <c r="I191" s="7"/>
-      <c r="J191" s="28" t="s">
+      <c r="J191" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K191" s="28"/>
-      <c r="L191" s="28"/>
-      <c r="M191" s="28"/>
-      <c r="N191" s="29"/>
+      <c r="K191" s="45"/>
+      <c r="L191" s="45"/>
+      <c r="M191" s="45"/>
+      <c r="N191" s="46"/>
       <c r="O191" s="2"/>
     </row>
     <row r="192" spans="2:15" x14ac:dyDescent="0.25">
@@ -9503,78 +9533,78 @@
     </row>
     <row r="202" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B202" s="6"/>
-      <c r="C202" s="30" t="s">
+      <c r="C202" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D202" s="30"/>
-      <c r="E202" s="30"/>
-      <c r="F202" s="30"/>
-      <c r="G202" s="31"/>
+      <c r="D202" s="47"/>
+      <c r="E202" s="47"/>
+      <c r="F202" s="47"/>
+      <c r="G202" s="48"/>
       <c r="I202" s="6"/>
-      <c r="J202" s="30" t="s">
+      <c r="J202" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K202" s="30"/>
-      <c r="L202" s="30"/>
-      <c r="M202" s="30"/>
-      <c r="N202" s="31"/>
+      <c r="K202" s="47"/>
+      <c r="L202" s="47"/>
+      <c r="M202" s="47"/>
+      <c r="N202" s="48"/>
       <c r="O202" s="2"/>
     </row>
     <row r="203" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B203" s="7"/>
-      <c r="C203" s="26" t="s">
+      <c r="C203" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D203" s="26"/>
-      <c r="E203" s="26"/>
-      <c r="F203" s="26"/>
-      <c r="G203" s="27"/>
+      <c r="D203" s="43"/>
+      <c r="E203" s="43"/>
+      <c r="F203" s="43"/>
+      <c r="G203" s="44"/>
       <c r="I203" s="7"/>
-      <c r="J203" s="26" t="s">
+      <c r="J203" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K203" s="26"/>
-      <c r="L203" s="26"/>
-      <c r="M203" s="26"/>
-      <c r="N203" s="27"/>
+      <c r="K203" s="43"/>
+      <c r="L203" s="43"/>
+      <c r="M203" s="43"/>
+      <c r="N203" s="44"/>
       <c r="O203" s="2"/>
     </row>
     <row r="204" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B204" s="7"/>
-      <c r="C204" s="26" t="s">
+      <c r="C204" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D204" s="26"/>
-      <c r="E204" s="26"/>
-      <c r="F204" s="26"/>
-      <c r="G204" s="27"/>
+      <c r="D204" s="43"/>
+      <c r="E204" s="43"/>
+      <c r="F204" s="43"/>
+      <c r="G204" s="44"/>
       <c r="I204" s="7"/>
-      <c r="J204" s="26" t="s">
+      <c r="J204" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K204" s="26"/>
-      <c r="L204" s="26"/>
-      <c r="M204" s="26"/>
-      <c r="N204" s="27"/>
+      <c r="K204" s="43"/>
+      <c r="L204" s="43"/>
+      <c r="M204" s="43"/>
+      <c r="N204" s="44"/>
       <c r="O204" s="2"/>
     </row>
     <row r="205" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B205" s="7"/>
-      <c r="C205" s="28" t="s">
+      <c r="C205" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D205" s="28"/>
-      <c r="E205" s="28"/>
-      <c r="F205" s="28"/>
-      <c r="G205" s="29"/>
+      <c r="D205" s="45"/>
+      <c r="E205" s="45"/>
+      <c r="F205" s="45"/>
+      <c r="G205" s="46"/>
       <c r="I205" s="7"/>
-      <c r="J205" s="28" t="s">
+      <c r="J205" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K205" s="28"/>
-      <c r="L205" s="28"/>
-      <c r="M205" s="28"/>
-      <c r="N205" s="29"/>
+      <c r="K205" s="45"/>
+      <c r="L205" s="45"/>
+      <c r="M205" s="45"/>
+      <c r="N205" s="46"/>
       <c r="O205" s="2"/>
     </row>
     <row r="206" spans="2:15" x14ac:dyDescent="0.25">
@@ -9731,75 +9761,75 @@
     </row>
     <row r="216" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B216" s="6"/>
-      <c r="C216" s="30" t="s">
+      <c r="C216" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D216" s="30"/>
-      <c r="E216" s="30"/>
-      <c r="F216" s="30"/>
-      <c r="G216" s="31"/>
+      <c r="D216" s="47"/>
+      <c r="E216" s="47"/>
+      <c r="F216" s="47"/>
+      <c r="G216" s="48"/>
       <c r="I216" s="6"/>
-      <c r="J216" s="30" t="s">
+      <c r="J216" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K216" s="30"/>
-      <c r="L216" s="30"/>
-      <c r="M216" s="30"/>
-      <c r="N216" s="31"/>
+      <c r="K216" s="47"/>
+      <c r="L216" s="47"/>
+      <c r="M216" s="47"/>
+      <c r="N216" s="48"/>
     </row>
     <row r="217" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B217" s="7"/>
-      <c r="C217" s="26" t="s">
+      <c r="C217" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D217" s="26"/>
-      <c r="E217" s="26"/>
-      <c r="F217" s="26"/>
-      <c r="G217" s="27"/>
+      <c r="D217" s="43"/>
+      <c r="E217" s="43"/>
+      <c r="F217" s="43"/>
+      <c r="G217" s="44"/>
       <c r="I217" s="7"/>
-      <c r="J217" s="26" t="s">
+      <c r="J217" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K217" s="26"/>
-      <c r="L217" s="26"/>
-      <c r="M217" s="26"/>
-      <c r="N217" s="27"/>
+      <c r="K217" s="43"/>
+      <c r="L217" s="43"/>
+      <c r="M217" s="43"/>
+      <c r="N217" s="44"/>
     </row>
     <row r="218" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B218" s="7"/>
-      <c r="C218" s="26" t="s">
+      <c r="C218" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D218" s="26"/>
-      <c r="E218" s="26"/>
-      <c r="F218" s="26"/>
-      <c r="G218" s="27"/>
+      <c r="D218" s="43"/>
+      <c r="E218" s="43"/>
+      <c r="F218" s="43"/>
+      <c r="G218" s="44"/>
       <c r="I218" s="7"/>
-      <c r="J218" s="26" t="s">
+      <c r="J218" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K218" s="26"/>
-      <c r="L218" s="26"/>
-      <c r="M218" s="26"/>
-      <c r="N218" s="27"/>
+      <c r="K218" s="43"/>
+      <c r="L218" s="43"/>
+      <c r="M218" s="43"/>
+      <c r="N218" s="44"/>
     </row>
     <row r="219" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B219" s="7"/>
-      <c r="C219" s="28" t="s">
+      <c r="C219" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D219" s="28"/>
-      <c r="E219" s="28"/>
-      <c r="F219" s="28"/>
-      <c r="G219" s="29"/>
+      <c r="D219" s="45"/>
+      <c r="E219" s="45"/>
+      <c r="F219" s="45"/>
+      <c r="G219" s="46"/>
       <c r="I219" s="7"/>
-      <c r="J219" s="28" t="s">
+      <c r="J219" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K219" s="28"/>
-      <c r="L219" s="28"/>
-      <c r="M219" s="28"/>
-      <c r="N219" s="29"/>
+      <c r="K219" s="45"/>
+      <c r="L219" s="45"/>
+      <c r="M219" s="45"/>
+      <c r="N219" s="46"/>
     </row>
     <row r="220" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B220" s="7"/>
@@ -9949,75 +9979,75 @@
     </row>
     <row r="230" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B230" s="6"/>
-      <c r="C230" s="30" t="s">
+      <c r="C230" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D230" s="30"/>
-      <c r="E230" s="30"/>
-      <c r="F230" s="30"/>
-      <c r="G230" s="31"/>
+      <c r="D230" s="47"/>
+      <c r="E230" s="47"/>
+      <c r="F230" s="47"/>
+      <c r="G230" s="48"/>
       <c r="I230" s="6"/>
-      <c r="J230" s="30" t="s">
+      <c r="J230" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K230" s="30"/>
-      <c r="L230" s="30"/>
-      <c r="M230" s="30"/>
-      <c r="N230" s="31"/>
+      <c r="K230" s="47"/>
+      <c r="L230" s="47"/>
+      <c r="M230" s="47"/>
+      <c r="N230" s="48"/>
     </row>
     <row r="231" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B231" s="7"/>
-      <c r="C231" s="26" t="s">
+      <c r="C231" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D231" s="26"/>
-      <c r="E231" s="26"/>
-      <c r="F231" s="26"/>
-      <c r="G231" s="27"/>
+      <c r="D231" s="43"/>
+      <c r="E231" s="43"/>
+      <c r="F231" s="43"/>
+      <c r="G231" s="44"/>
       <c r="I231" s="7"/>
-      <c r="J231" s="26" t="s">
+      <c r="J231" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K231" s="26"/>
-      <c r="L231" s="26"/>
-      <c r="M231" s="26"/>
-      <c r="N231" s="27"/>
+      <c r="K231" s="43"/>
+      <c r="L231" s="43"/>
+      <c r="M231" s="43"/>
+      <c r="N231" s="44"/>
     </row>
     <row r="232" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B232" s="7"/>
-      <c r="C232" s="26" t="s">
+      <c r="C232" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D232" s="26"/>
-      <c r="E232" s="26"/>
-      <c r="F232" s="26"/>
-      <c r="G232" s="27"/>
+      <c r="D232" s="43"/>
+      <c r="E232" s="43"/>
+      <c r="F232" s="43"/>
+      <c r="G232" s="44"/>
       <c r="I232" s="7"/>
-      <c r="J232" s="26" t="s">
+      <c r="J232" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K232" s="26"/>
-      <c r="L232" s="26"/>
-      <c r="M232" s="26"/>
-      <c r="N232" s="27"/>
+      <c r="K232" s="43"/>
+      <c r="L232" s="43"/>
+      <c r="M232" s="43"/>
+      <c r="N232" s="44"/>
     </row>
     <row r="233" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B233" s="7"/>
-      <c r="C233" s="28" t="s">
+      <c r="C233" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D233" s="28"/>
-      <c r="E233" s="28"/>
-      <c r="F233" s="28"/>
-      <c r="G233" s="29"/>
+      <c r="D233" s="45"/>
+      <c r="E233" s="45"/>
+      <c r="F233" s="45"/>
+      <c r="G233" s="46"/>
       <c r="I233" s="7"/>
-      <c r="J233" s="28" t="s">
+      <c r="J233" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K233" s="28"/>
-      <c r="L233" s="28"/>
-      <c r="M233" s="28"/>
-      <c r="N233" s="29"/>
+      <c r="K233" s="45"/>
+      <c r="L233" s="45"/>
+      <c r="M233" s="45"/>
+      <c r="N233" s="46"/>
     </row>
     <row r="234" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B234" s="7"/>
@@ -10167,75 +10197,75 @@
     </row>
     <row r="244" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B244" s="6"/>
-      <c r="C244" s="30" t="s">
+      <c r="C244" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D244" s="30"/>
-      <c r="E244" s="30"/>
-      <c r="F244" s="30"/>
-      <c r="G244" s="31"/>
+      <c r="D244" s="47"/>
+      <c r="E244" s="47"/>
+      <c r="F244" s="47"/>
+      <c r="G244" s="48"/>
       <c r="I244" s="6"/>
-      <c r="J244" s="30" t="s">
+      <c r="J244" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K244" s="30"/>
-      <c r="L244" s="30"/>
-      <c r="M244" s="30"/>
-      <c r="N244" s="31"/>
+      <c r="K244" s="47"/>
+      <c r="L244" s="47"/>
+      <c r="M244" s="47"/>
+      <c r="N244" s="48"/>
     </row>
     <row r="245" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B245" s="7"/>
-      <c r="C245" s="26" t="s">
+      <c r="C245" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D245" s="26"/>
-      <c r="E245" s="26"/>
-      <c r="F245" s="26"/>
-      <c r="G245" s="27"/>
+      <c r="D245" s="43"/>
+      <c r="E245" s="43"/>
+      <c r="F245" s="43"/>
+      <c r="G245" s="44"/>
       <c r="I245" s="7"/>
-      <c r="J245" s="26" t="s">
+      <c r="J245" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K245" s="26"/>
-      <c r="L245" s="26"/>
-      <c r="M245" s="26"/>
-      <c r="N245" s="27"/>
+      <c r="K245" s="43"/>
+      <c r="L245" s="43"/>
+      <c r="M245" s="43"/>
+      <c r="N245" s="44"/>
     </row>
     <row r="246" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B246" s="7"/>
-      <c r="C246" s="26" t="s">
+      <c r="C246" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D246" s="26"/>
-      <c r="E246" s="26"/>
-      <c r="F246" s="26"/>
-      <c r="G246" s="27"/>
+      <c r="D246" s="43"/>
+      <c r="E246" s="43"/>
+      <c r="F246" s="43"/>
+      <c r="G246" s="44"/>
       <c r="I246" s="7"/>
-      <c r="J246" s="26" t="s">
+      <c r="J246" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K246" s="26"/>
-      <c r="L246" s="26"/>
-      <c r="M246" s="26"/>
-      <c r="N246" s="27"/>
+      <c r="K246" s="43"/>
+      <c r="L246" s="43"/>
+      <c r="M246" s="43"/>
+      <c r="N246" s="44"/>
     </row>
     <row r="247" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B247" s="7"/>
-      <c r="C247" s="28" t="s">
+      <c r="C247" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D247" s="28"/>
-      <c r="E247" s="28"/>
-      <c r="F247" s="28"/>
-      <c r="G247" s="29"/>
+      <c r="D247" s="45"/>
+      <c r="E247" s="45"/>
+      <c r="F247" s="45"/>
+      <c r="G247" s="46"/>
       <c r="I247" s="7"/>
-      <c r="J247" s="28" t="s">
+      <c r="J247" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K247" s="28"/>
-      <c r="L247" s="28"/>
-      <c r="M247" s="28"/>
-      <c r="N247" s="29"/>
+      <c r="K247" s="45"/>
+      <c r="L247" s="45"/>
+      <c r="M247" s="45"/>
+      <c r="N247" s="46"/>
     </row>
     <row r="248" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B248" s="7"/>
@@ -10385,75 +10415,75 @@
     </row>
     <row r="258" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B258" s="6"/>
-      <c r="C258" s="30" t="s">
+      <c r="C258" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D258" s="30"/>
-      <c r="E258" s="30"/>
-      <c r="F258" s="30"/>
-      <c r="G258" s="31"/>
+      <c r="D258" s="47"/>
+      <c r="E258" s="47"/>
+      <c r="F258" s="47"/>
+      <c r="G258" s="48"/>
       <c r="I258" s="6"/>
-      <c r="J258" s="30" t="s">
+      <c r="J258" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K258" s="30"/>
-      <c r="L258" s="30"/>
-      <c r="M258" s="30"/>
-      <c r="N258" s="31"/>
+      <c r="K258" s="47"/>
+      <c r="L258" s="47"/>
+      <c r="M258" s="47"/>
+      <c r="N258" s="48"/>
     </row>
     <row r="259" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B259" s="7"/>
-      <c r="C259" s="26" t="s">
+      <c r="C259" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D259" s="26"/>
-      <c r="E259" s="26"/>
-      <c r="F259" s="26"/>
-      <c r="G259" s="27"/>
+      <c r="D259" s="43"/>
+      <c r="E259" s="43"/>
+      <c r="F259" s="43"/>
+      <c r="G259" s="44"/>
       <c r="I259" s="7"/>
-      <c r="J259" s="26" t="s">
+      <c r="J259" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K259" s="26"/>
-      <c r="L259" s="26"/>
-      <c r="M259" s="26"/>
-      <c r="N259" s="27"/>
+      <c r="K259" s="43"/>
+      <c r="L259" s="43"/>
+      <c r="M259" s="43"/>
+      <c r="N259" s="44"/>
     </row>
     <row r="260" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B260" s="7"/>
-      <c r="C260" s="26" t="s">
+      <c r="C260" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D260" s="26"/>
-      <c r="E260" s="26"/>
-      <c r="F260" s="26"/>
-      <c r="G260" s="27"/>
+      <c r="D260" s="43"/>
+      <c r="E260" s="43"/>
+      <c r="F260" s="43"/>
+      <c r="G260" s="44"/>
       <c r="I260" s="7"/>
-      <c r="J260" s="26" t="s">
+      <c r="J260" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K260" s="26"/>
-      <c r="L260" s="26"/>
-      <c r="M260" s="26"/>
-      <c r="N260" s="27"/>
+      <c r="K260" s="43"/>
+      <c r="L260" s="43"/>
+      <c r="M260" s="43"/>
+      <c r="N260" s="44"/>
     </row>
     <row r="261" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B261" s="7"/>
-      <c r="C261" s="28" t="s">
+      <c r="C261" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D261" s="28"/>
-      <c r="E261" s="28"/>
-      <c r="F261" s="28"/>
-      <c r="G261" s="29"/>
+      <c r="D261" s="45"/>
+      <c r="E261" s="45"/>
+      <c r="F261" s="45"/>
+      <c r="G261" s="46"/>
       <c r="I261" s="7"/>
-      <c r="J261" s="28" t="s">
+      <c r="J261" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K261" s="28"/>
-      <c r="L261" s="28"/>
-      <c r="M261" s="28"/>
-      <c r="N261" s="29"/>
+      <c r="K261" s="45"/>
+      <c r="L261" s="45"/>
+      <c r="M261" s="45"/>
+      <c r="N261" s="46"/>
     </row>
     <row r="262" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B262" s="7"/>
@@ -10602,87 +10632,87 @@
       <c r="N270" s="13"/>
     </row>
     <row r="272" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B272" s="6"/>
-      <c r="C272" s="30" t="s">
+      <c r="B272" s="26"/>
+      <c r="C272" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D272" s="30"/>
-      <c r="E272" s="30"/>
-      <c r="F272" s="30"/>
-      <c r="G272" s="31"/>
+      <c r="D272" s="49"/>
+      <c r="E272" s="49"/>
+      <c r="F272" s="49"/>
+      <c r="G272" s="50"/>
       <c r="I272" s="6"/>
-      <c r="J272" s="30" t="s">
+      <c r="J272" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K272" s="30"/>
-      <c r="L272" s="30"/>
-      <c r="M272" s="30"/>
-      <c r="N272" s="31"/>
+      <c r="K272" s="47"/>
+      <c r="L272" s="47"/>
+      <c r="M272" s="47"/>
+      <c r="N272" s="48"/>
     </row>
     <row r="273" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B273" s="7"/>
-      <c r="C273" s="26" t="s">
+      <c r="B273" s="27"/>
+      <c r="C273" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D273" s="26"/>
-      <c r="E273" s="26"/>
-      <c r="F273" s="26"/>
-      <c r="G273" s="27"/>
+      <c r="D273" s="51"/>
+      <c r="E273" s="51"/>
+      <c r="F273" s="51"/>
+      <c r="G273" s="52"/>
       <c r="I273" s="7"/>
-      <c r="J273" s="26" t="s">
+      <c r="J273" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K273" s="26"/>
-      <c r="L273" s="26"/>
-      <c r="M273" s="26"/>
-      <c r="N273" s="27"/>
+      <c r="K273" s="43"/>
+      <c r="L273" s="43"/>
+      <c r="M273" s="43"/>
+      <c r="N273" s="44"/>
     </row>
     <row r="274" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B274" s="7"/>
-      <c r="C274" s="26" t="s">
+      <c r="B274" s="27"/>
+      <c r="C274" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D274" s="26"/>
-      <c r="E274" s="26"/>
-      <c r="F274" s="26"/>
-      <c r="G274" s="27"/>
+      <c r="D274" s="51"/>
+      <c r="E274" s="51"/>
+      <c r="F274" s="51"/>
+      <c r="G274" s="52"/>
       <c r="I274" s="7"/>
-      <c r="J274" s="26" t="s">
+      <c r="J274" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K274" s="26"/>
-      <c r="L274" s="26"/>
-      <c r="M274" s="26"/>
-      <c r="N274" s="27"/>
+      <c r="K274" s="43"/>
+      <c r="L274" s="43"/>
+      <c r="M274" s="43"/>
+      <c r="N274" s="44"/>
       <c r="R274" s="22"/>
     </row>
     <row r="275" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B275" s="7"/>
-      <c r="C275" s="28" t="s">
+      <c r="B275" s="27"/>
+      <c r="C275" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D275" s="28"/>
-      <c r="E275" s="28"/>
-      <c r="F275" s="28"/>
-      <c r="G275" s="29"/>
+      <c r="D275" s="53"/>
+      <c r="E275" s="53"/>
+      <c r="F275" s="53"/>
+      <c r="G275" s="54"/>
       <c r="I275" s="7"/>
-      <c r="J275" s="28" t="s">
+      <c r="J275" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K275" s="28"/>
-      <c r="L275" s="28"/>
-      <c r="M275" s="28"/>
-      <c r="N275" s="29"/>
+      <c r="K275" s="45"/>
+      <c r="L275" s="45"/>
+      <c r="M275" s="45"/>
+      <c r="N275" s="46"/>
     </row>
     <row r="276" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B276" s="7"/>
-      <c r="C276" s="20" t="s">
+      <c r="B276" s="27"/>
+      <c r="C276" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D276" s="14"/>
-      <c r="E276" s="14"/>
-      <c r="F276" s="14"/>
-      <c r="G276" s="15"/>
+      <c r="D276" s="29"/>
+      <c r="E276" s="29"/>
+      <c r="F276" s="29"/>
+      <c r="G276" s="30"/>
       <c r="I276" s="7"/>
       <c r="J276" s="20" t="s">
         <v>4</v>
@@ -10694,12 +10724,12 @@
       <c r="O276" s="22"/>
     </row>
     <row r="277" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B277" s="7"/>
-      <c r="C277" s="2"/>
-      <c r="D277" s="2"/>
-      <c r="E277" s="2"/>
-      <c r="F277" s="2"/>
-      <c r="G277" s="8"/>
+      <c r="B277" s="27"/>
+      <c r="C277" s="23"/>
+      <c r="D277" s="23"/>
+      <c r="E277" s="23"/>
+      <c r="F277" s="23"/>
+      <c r="G277" s="25"/>
       <c r="I277" s="7"/>
       <c r="J277" s="2"/>
       <c r="K277" s="2"/>
@@ -10708,14 +10738,14 @@
       <c r="N277" s="8"/>
     </row>
     <row r="278" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B278" s="9" t="s">
+      <c r="B278" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C278" s="2"/>
-      <c r="D278" s="2"/>
-      <c r="E278" s="2"/>
-      <c r="F278" s="2"/>
-      <c r="G278" s="8"/>
+      <c r="C278" s="23"/>
+      <c r="D278" s="23"/>
+      <c r="E278" s="23"/>
+      <c r="F278" s="23"/>
+      <c r="G278" s="25"/>
       <c r="I278" s="9" t="s">
         <v>6</v>
       </c>
@@ -10726,14 +10756,14 @@
       <c r="N278" s="8"/>
     </row>
     <row r="279" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B279" s="10" t="s">
+      <c r="B279" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C279" s="2"/>
+      <c r="C279" s="23"/>
       <c r="D279" s="23"/>
-      <c r="E279" s="2"/>
-      <c r="F279" s="2"/>
-      <c r="G279" s="8"/>
+      <c r="E279" s="23"/>
+      <c r="F279" s="23"/>
+      <c r="G279" s="25"/>
       <c r="I279" s="10" t="s">
         <v>7</v>
       </c>
@@ -10744,14 +10774,14 @@
       <c r="N279" s="8"/>
     </row>
     <row r="280" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B280" s="11" t="s">
+      <c r="B280" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C280" s="24"/>
-      <c r="D280" s="24"/>
-      <c r="E280" s="2"/>
-      <c r="F280" s="3"/>
-      <c r="G280" s="8"/>
+      <c r="C280" s="34"/>
+      <c r="D280" s="34"/>
+      <c r="E280" s="23"/>
+      <c r="F280" s="35"/>
+      <c r="G280" s="25"/>
       <c r="I280" s="11" t="s">
         <v>8</v>
       </c>
@@ -10762,12 +10792,12 @@
       <c r="N280" s="8"/>
     </row>
     <row r="281" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B281" s="7"/>
-      <c r="C281" s="2"/>
-      <c r="D281" s="2"/>
-      <c r="E281" s="2"/>
-      <c r="F281" s="4"/>
-      <c r="G281" s="8"/>
+      <c r="B281" s="27"/>
+      <c r="C281" s="23"/>
+      <c r="D281" s="23"/>
+      <c r="E281" s="23"/>
+      <c r="F281" s="36"/>
+      <c r="G281" s="25"/>
       <c r="I281" s="7"/>
       <c r="J281" s="2"/>
       <c r="K281" s="2"/>
@@ -10776,14 +10806,14 @@
       <c r="N281" s="8"/>
     </row>
     <row r="282" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B282" s="16" t="s">
+      <c r="B282" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C282" s="17"/>
-      <c r="D282" s="17"/>
-      <c r="E282" s="2"/>
-      <c r="F282" s="4"/>
-      <c r="G282" s="8"/>
+      <c r="C282" s="38"/>
+      <c r="D282" s="38"/>
+      <c r="E282" s="23"/>
+      <c r="F282" s="36"/>
+      <c r="G282" s="25"/>
       <c r="I282" s="16" t="s">
         <v>5</v>
       </c>
@@ -10794,12 +10824,12 @@
       <c r="N282" s="8"/>
     </row>
     <row r="283" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B283" s="7"/>
-      <c r="C283" s="2"/>
-      <c r="D283" s="2"/>
-      <c r="E283" s="2"/>
-      <c r="F283" s="5"/>
-      <c r="G283" s="8"/>
+      <c r="B283" s="27"/>
+      <c r="C283" s="23"/>
+      <c r="D283" s="23"/>
+      <c r="E283" s="23"/>
+      <c r="F283" s="39"/>
+      <c r="G283" s="25"/>
       <c r="I283" s="7"/>
       <c r="J283" s="2"/>
       <c r="K283" s="2"/>
@@ -10808,12 +10838,12 @@
       <c r="N283" s="8"/>
     </row>
     <row r="284" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B284" s="12"/>
-      <c r="C284" s="1"/>
-      <c r="D284" s="1"/>
-      <c r="E284" s="1"/>
-      <c r="F284" s="1"/>
-      <c r="G284" s="13"/>
+      <c r="B284" s="40"/>
+      <c r="C284" s="41"/>
+      <c r="D284" s="41"/>
+      <c r="E284" s="41"/>
+      <c r="F284" s="41"/>
+      <c r="G284" s="42"/>
       <c r="I284" s="12"/>
       <c r="J284" s="1"/>
       <c r="K284" s="1"/>
@@ -10884,6 +10914,10 @@
     <mergeCell ref="C188:G188"/>
     <mergeCell ref="C189:G189"/>
     <mergeCell ref="C190:G190"/>
+    <mergeCell ref="C191:G191"/>
+    <mergeCell ref="C203:G203"/>
+    <mergeCell ref="C204:G204"/>
+    <mergeCell ref="C205:G205"/>
     <mergeCell ref="J160:N160"/>
     <mergeCell ref="C161:G161"/>
     <mergeCell ref="J161:N161"/>
@@ -10893,11 +10927,6 @@
     <mergeCell ref="J163:N163"/>
     <mergeCell ref="C174:G174"/>
     <mergeCell ref="J174:N174"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="J117:N117"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="C132:G132"/>
-    <mergeCell ref="J132:N132"/>
     <mergeCell ref="C133:G133"/>
     <mergeCell ref="J133:N133"/>
     <mergeCell ref="C48:G48"/>
@@ -10912,24 +10941,11 @@
     <mergeCell ref="J64:N64"/>
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="J50:N50"/>
-    <mergeCell ref="C191:G191"/>
-    <mergeCell ref="C203:G203"/>
-    <mergeCell ref="C204:G204"/>
-    <mergeCell ref="C205:G205"/>
     <mergeCell ref="J118:N118"/>
     <mergeCell ref="C119:G119"/>
     <mergeCell ref="J119:N119"/>
     <mergeCell ref="C121:G121"/>
     <mergeCell ref="J121:N121"/>
-    <mergeCell ref="C134:G134"/>
-    <mergeCell ref="J134:N134"/>
-    <mergeCell ref="C135:G135"/>
-    <mergeCell ref="J135:N135"/>
-    <mergeCell ref="C146:G146"/>
-    <mergeCell ref="J146:N146"/>
-    <mergeCell ref="C147:G147"/>
-    <mergeCell ref="J147:N147"/>
-    <mergeCell ref="C148:G148"/>
     <mergeCell ref="C120:G120"/>
     <mergeCell ref="J120:N120"/>
     <mergeCell ref="J148:N148"/>
@@ -10940,6 +10956,20 @@
     <mergeCell ref="J105:N105"/>
     <mergeCell ref="C106:G106"/>
     <mergeCell ref="J106:N106"/>
+    <mergeCell ref="C134:G134"/>
+    <mergeCell ref="J134:N134"/>
+    <mergeCell ref="C135:G135"/>
+    <mergeCell ref="J135:N135"/>
+    <mergeCell ref="C146:G146"/>
+    <mergeCell ref="J146:N146"/>
+    <mergeCell ref="C147:G147"/>
+    <mergeCell ref="J147:N147"/>
+    <mergeCell ref="C148:G148"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="J117:N117"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="C132:G132"/>
+    <mergeCell ref="J132:N132"/>
     <mergeCell ref="C104:G104"/>
     <mergeCell ref="J104:N104"/>
     <mergeCell ref="C107:G107"/>

</xml_diff>